<commit_message>
test of parcel is not completed
</commit_message>
<xml_diff>
--- a/calc/files/letter2.xlsx
+++ b/calc/files/letter2.xlsx
@@ -459,6 +459,7 @@
       <t>За хрупкие мелкие пакеты с объявленной ценностью  с отметкой "Осторожно" взимается надбавка к плате за  пересылку  мелкого  пакета   в  размере  50%.  На  плату  за  объявленную  ценность  мелкого  пакета надбавка не распространяется</t>
     </r>
   </si>
+  <si/>
   <si>
     <r>
       <rPr>
@@ -2029,9 +2030,10 @@
     <numFmt co:extendedFormatCode="0.00" formatCode="0.00" numFmtId="1003"/>
     <numFmt co:extendedFormatCode="0.0%" formatCode="0.0%" numFmtId="1004"/>
     <numFmt co:extendedFormatCode="0.000" formatCode="0.000" numFmtId="1005"/>
-    <numFmt co:extendedFormatCode="0.00%" formatCode="0.00%" numFmtId="1006"/>
+    <numFmt co:extendedFormatCode="0.0000" formatCode="0.0000" numFmtId="1006"/>
+    <numFmt co:extendedFormatCode="0.00%" formatCode="0.00%" numFmtId="1007"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <name val="Calibri"/>
       <color rgb="000000" tint="0"/>
@@ -2107,11 +2109,6 @@
     </font>
     <font>
       <name val="Microsoft Sans Serif"/>
-      <color rgb="000000" tint="0"/>
-      <sz val="8.5"/>
-    </font>
-    <font>
-      <name val="Microsoft Sans Serif"/>
       <sz val="7.5"/>
     </font>
   </fonts>
@@ -2270,9 +2267,6 @@
     <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="1" numFmtId="1003" quotePrefix="false">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="14" numFmtId="1003" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
@@ -2327,6 +2321,9 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="center" vertical="top" wrapText="true"/>
     </xf>
+    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="1" numFmtId="1006" quotePrefix="false">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="13" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
@@ -2336,7 +2333,7 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="15" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="14" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" indent="1" vertical="top" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="8" numFmtId="1000" quotePrefix="false">
@@ -2375,7 +2372,7 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="8" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="13" numFmtId="1006" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="13" numFmtId="1007" quotePrefix="false">
       <alignment horizontal="right" indent="5" shrinkToFit="true" vertical="top"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="13" numFmtId="1002" quotePrefix="false">
@@ -2384,7 +2381,7 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="13" numFmtId="1004" quotePrefix="false">
       <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="13" numFmtId="1006" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="13" numFmtId="1007" quotePrefix="false">
       <alignment horizontal="right" indent="5" shrinkToFit="true" vertical="center"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="12" numFmtId="1004" quotePrefix="false">
@@ -2833,7 +2830,7 @@
       <c r="G11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="26" t="n">
+      <c r="H11" s="24" t="n">
         <v>3</v>
       </c>
       <c r="I11" s="25" t="n">
@@ -2853,7 +2850,7 @@
       <c r="A12" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="B12" s="27" t="n"/>
+      <c r="B12" s="26" t="n"/>
       <c r="C12" s="11" t="s">
         <v>28</v>
       </c>
@@ -2863,8 +2860,8 @@
       <c r="E12" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="F12" s="27" t="n"/>
-      <c r="G12" s="28" t="s">
+      <c r="F12" s="26" t="n"/>
+      <c r="G12" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H12" s="24" t="n">
@@ -2885,7 +2882,7 @@
       <c r="C13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="29" t="n">
+      <c r="D13" s="28" t="n">
         <v>0.036</v>
       </c>
       <c r="E13" s="23" t="n">
@@ -2895,10 +2892,10 @@
       <c r="G13" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="30" t="n">
+      <c r="H13" s="29" t="n">
         <v>0.03</v>
       </c>
-      <c r="I13" s="31" t="n">
+      <c r="I13" s="30" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">H13*1.2</f>
         <v>0.036</v>
       </c>
@@ -2987,14 +2984,14 @@
       <c r="D17" s="22" t="n">
         <v>3.24</v>
       </c>
-      <c r="E17" s="32" t="n">
+      <c r="E17" s="31" t="n">
         <v>8</v>
       </c>
       <c r="F17" s="16" t="n"/>
       <c r="G17" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="26" t="n">
+      <c r="H17" s="24" t="n">
         <v>3</v>
       </c>
       <c r="I17" s="25" t="n">
@@ -3003,24 +3000,24 @@
       </c>
     </row>
     <row customHeight="true" ht="35.25" outlineLevel="0" r="18">
-      <c r="A18" s="33" t="n">
+      <c r="A18" s="32" t="n">
         <v>9</v>
       </c>
-      <c r="B18" s="27" t="n"/>
-      <c r="C18" s="34" t="s">
+      <c r="B18" s="26" t="n"/>
+      <c r="C18" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="35" t="n">
+      <c r="D18" s="34" t="n">
         <v>0.06</v>
       </c>
-      <c r="E18" s="36" t="n">
+      <c r="E18" s="35" t="n">
         <v>9</v>
       </c>
-      <c r="F18" s="37" t="n"/>
+      <c r="F18" s="36" t="n"/>
       <c r="G18" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="38" t="n">
+      <c r="H18" s="37" t="n">
         <v>0.05</v>
       </c>
       <c r="I18" s="25" t="n">
@@ -3032,11 +3029,11 @@
       <c r="A19" s="21" t="n">
         <v>10</v>
       </c>
-      <c r="B19" s="27" t="n"/>
+      <c r="B19" s="26" t="n"/>
       <c r="C19" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="29" t="n">
+      <c r="D19" s="28" t="n">
         <v>0.036</v>
       </c>
       <c r="E19" s="23" t="n">
@@ -3046,50 +3043,53 @@
       <c r="G19" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="30" t="n">
+      <c r="H19" s="29" t="n">
         <v>0.03</v>
       </c>
-      <c r="I19" s="31" t="n">
+      <c r="I19" s="30" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">H19*1.2</f>
         <v>0.036</v>
       </c>
     </row>
     <row customHeight="true" ht="34.75" outlineLevel="0" r="20">
-      <c r="A20" s="33" t="n">
+      <c r="A20" s="32" t="n">
         <v>11</v>
       </c>
-      <c r="B20" s="27" t="n"/>
-      <c r="C20" s="34" t="s">
+      <c r="B20" s="26" t="n"/>
+      <c r="C20" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="39" t="s"/>
-      <c r="E20" s="36" t="n">
+      <c r="D20" s="38" t="s"/>
+      <c r="E20" s="35" t="n">
         <v>11</v>
       </c>
-      <c r="F20" s="37" t="n"/>
+      <c r="F20" s="36" t="n"/>
       <c r="G20" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="40" t="s"/>
+      <c r="H20" s="39" t="s"/>
       <c r="I20" s="25" t="n"/>
+      <c r="J20" s="0" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row customHeight="true" ht="34.75" outlineLevel="0" r="21">
-      <c r="A21" s="33" t="n">
+      <c r="A21" s="32" t="n">
         <v>12</v>
       </c>
-      <c r="B21" s="27" t="n"/>
+      <c r="B21" s="26" t="n"/>
       <c r="C21" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="41" t="s"/>
-      <c r="E21" s="36" t="n">
+        <v>45</v>
+      </c>
+      <c r="D21" s="40" t="s"/>
+      <c r="E21" s="35" t="n">
         <v>12</v>
       </c>
-      <c r="F21" s="27" t="n"/>
+      <c r="F21" s="26" t="n"/>
       <c r="G21" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="40" t="s"/>
+        <v>46</v>
+      </c>
+      <c r="H21" s="39" t="s"/>
       <c r="I21" s="25" t="n"/>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="22">
@@ -3098,17 +3098,17 @@
         <v>4</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="42" t="s"/>
+        <v>47</v>
+      </c>
+      <c r="D22" s="41" t="s"/>
       <c r="E22" s="16" t="n"/>
       <c r="F22" s="19" t="n">
         <v>4</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="43" t="s"/>
+        <v>48</v>
+      </c>
+      <c r="H22" s="42" t="s"/>
       <c r="I22" s="25" t="n"/>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="23">
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B23" s="16" t="n"/>
       <c r="C23" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D23" s="22" t="n">
         <v>1.68</v>
@@ -3127,7 +3127,7 @@
       </c>
       <c r="F23" s="16" t="n"/>
       <c r="G23" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H23" s="24" t="n">
         <v>1.4</v>
@@ -3143,7 +3143,7 @@
       </c>
       <c r="B24" s="16" t="n"/>
       <c r="C24" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D24" s="22" t="n">
         <v>0.36</v>
@@ -3153,7 +3153,7 @@
       </c>
       <c r="F24" s="16" t="n"/>
       <c r="G24" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H24" s="24" t="n">
         <v>0.3</v>
@@ -3164,40 +3164,40 @@
       </c>
     </row>
     <row customHeight="true" ht="36.75" outlineLevel="0" r="25">
-      <c r="A25" s="33" t="n">
+      <c r="A25" s="32" t="n">
         <v>15</v>
       </c>
-      <c r="B25" s="27" t="n"/>
+      <c r="B25" s="26" t="n"/>
       <c r="C25" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="41" t="s"/>
-      <c r="E25" s="36" t="n">
+        <v>53</v>
+      </c>
+      <c r="D25" s="40" t="s"/>
+      <c r="E25" s="35" t="n">
         <v>15</v>
       </c>
-      <c r="F25" s="27" t="n"/>
+      <c r="F25" s="26" t="n"/>
       <c r="G25" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H25" s="40" t="s"/>
+        <v>54</v>
+      </c>
+      <c r="H25" s="39" t="s"/>
     </row>
     <row customHeight="true" ht="38" outlineLevel="0" r="26">
-      <c r="A26" s="33" t="n">
+      <c r="A26" s="32" t="n">
         <v>16</v>
       </c>
-      <c r="B26" s="27" t="n"/>
+      <c r="B26" s="26" t="n"/>
       <c r="C26" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="41" t="s"/>
-      <c r="E26" s="36" t="n">
+        <v>55</v>
+      </c>
+      <c r="D26" s="40" t="s"/>
+      <c r="E26" s="35" t="n">
         <v>16</v>
       </c>
-      <c r="F26" s="37" t="n"/>
+      <c r="F26" s="36" t="n"/>
       <c r="G26" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H26" s="40" t="s"/>
+        <v>56</v>
+      </c>
+      <c r="H26" s="39" t="s"/>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="27">
       <c r="A27" s="16" t="n"/>
@@ -3205,17 +3205,21 @@
         <v>5</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="42" t="s"/>
+        <v>57</v>
+      </c>
+      <c r="D27" s="41" t="s"/>
       <c r="E27" s="16" t="n"/>
       <c r="F27" s="19" t="n">
         <v>5</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H27" s="16" t="n"/>
+      <c r="K27" s="25" t="n">
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">K29+K30</f>
+        <v>6.265</v>
+      </c>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="28">
       <c r="A28" s="21" t="n">
@@ -3223,23 +3227,23 @@
       </c>
       <c r="B28" s="16" t="n"/>
       <c r="C28" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="41" t="s"/>
+        <v>59</v>
+      </c>
+      <c r="D28" s="40" t="s"/>
       <c r="E28" s="16" t="n"/>
       <c r="F28" s="16" t="n"/>
       <c r="G28" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="H28" s="40" t="s"/>
+        <v>60</v>
+      </c>
+      <c r="H28" s="39" t="s"/>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="29">
-      <c r="A29" s="44" t="s">
-        <v>60</v>
+      <c r="A29" s="43" t="s">
+        <v>61</v>
       </c>
       <c r="B29" s="16" t="n"/>
       <c r="C29" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D29" s="22" t="n">
         <v>3</v>
@@ -3249,39 +3253,56 @@
       </c>
       <c r="F29" s="16" t="n"/>
       <c r="G29" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H29" s="24" t="n">
         <v>4.5</v>
+      </c>
+      <c r="I29" s="44" t="n">
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">ROUND(H29+H30*0.9, 2)</f>
+        <v>5.18</v>
+      </c>
+      <c r="J29" s="44" t="n">
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">ROUND(I29*0.2, 2)</f>
+        <v>1.04</v>
+      </c>
+      <c r="K29" s="44" t="n">
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">I29+J29</f>
+        <v>6.22</v>
       </c>
     </row>
     <row customHeight="true" ht="28.75" outlineLevel="0" r="30">
       <c r="A30" s="21" t="n">
         <v>18</v>
       </c>
-      <c r="B30" s="27" t="n"/>
+      <c r="B30" s="26" t="n"/>
       <c r="C30" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="41" t="s"/>
+        <v>64</v>
+      </c>
+      <c r="D30" s="40" t="s"/>
       <c r="E30" s="23" t="n">
         <v>18</v>
       </c>
       <c r="F30" s="16" t="n"/>
       <c r="G30" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H30" s="24" t="n">
         <v>0.75</v>
       </c>
-    </row>
-    <row customHeight="true" ht="14" outlineLevel="0" r="31">
-      <c r="A31" s="44" t="s">
-        <v>65</v>
+      <c r="J30" s="0" t="n"/>
+      <c r="K30" s="0" t="n">
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.25*3.6/100</f>
+        <v>0.045</v>
+      </c>
+    </row>
+    <row customHeight="true" ht="45.4999389648438" outlineLevel="0" r="31">
+      <c r="A31" s="43" t="s">
+        <v>66</v>
       </c>
       <c r="B31" s="16" t="n"/>
       <c r="C31" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D31" s="22" t="n">
         <v>4</v>
@@ -3289,67 +3310,78 @@
       <c r="E31" s="23" t="n">
         <v>19</v>
       </c>
-      <c r="F31" s="27" t="n"/>
-      <c r="G31" s="28" t="s">
-        <v>67</v>
+      <c r="F31" s="26" t="n"/>
+      <c r="G31" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="H31" s="45" t="s"/>
-    </row>
-    <row customHeight="true" ht="14" outlineLevel="0" r="32">
-      <c r="A32" s="44" t="s">
-        <v>68</v>
+      <c r="I31" s="25" t="n">
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D31+1.16*D32</f>
+        <v>4.87</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="K31" s="25" t="n">
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">J31+I31</f>
+        <v>5.23</v>
+      </c>
+    </row>
+    <row customHeight="true" hidden="false" ht="45" outlineLevel="0" r="32">
+      <c r="A32" s="43" t="s">
+        <v>69</v>
       </c>
       <c r="B32" s="16" t="n"/>
       <c r="C32" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D32" s="22" t="n">
         <v>0.75</v>
       </c>
-      <c r="E32" s="36" t="n">
+      <c r="E32" s="35" t="n">
         <v>20</v>
       </c>
-      <c r="F32" s="27" t="n"/>
+      <c r="F32" s="26" t="n"/>
       <c r="G32" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H32" s="40" t="s"/>
+        <v>71</v>
+      </c>
+      <c r="H32" s="39" t="s"/>
     </row>
     <row customHeight="true" ht="38.75" outlineLevel="0" r="33">
-      <c r="A33" s="33" t="n">
+      <c r="A33" s="32" t="n">
         <v>19</v>
       </c>
-      <c r="B33" s="37" t="n"/>
+      <c r="B33" s="36" t="n"/>
       <c r="C33" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="41" t="s"/>
+        <v>72</v>
+      </c>
+      <c r="D33" s="40" t="s"/>
       <c r="E33" s="23" t="n">
         <v>21</v>
       </c>
-      <c r="F33" s="27" t="n"/>
-      <c r="G33" s="28" t="s">
-        <v>72</v>
+      <c r="F33" s="26" t="n"/>
+      <c r="G33" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="H33" s="24" t="n">
         <v>0.75</v>
       </c>
     </row>
     <row customHeight="true" ht="36.4999389648438" outlineLevel="0" r="34">
-      <c r="A34" s="33" t="n">
+      <c r="A34" s="32" t="n">
         <v>20</v>
       </c>
-      <c r="B34" s="27" t="n"/>
-      <c r="C34" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="39" t="s"/>
-      <c r="E34" s="36" t="n">
+      <c r="B34" s="26" t="n"/>
+      <c r="C34" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="38" t="s"/>
+      <c r="E34" s="35" t="n">
         <v>22</v>
       </c>
-      <c r="F34" s="27" t="n"/>
+      <c r="F34" s="26" t="n"/>
       <c r="G34" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H34" s="46" t="n">
         <v>0.05</v>
@@ -3371,49 +3403,49 @@
       <c r="E35" s="23" t="n">
         <v>23</v>
       </c>
-      <c r="F35" s="27" t="n"/>
-      <c r="G35" s="28" t="s">
-        <v>75</v>
+      <c r="F35" s="26" t="n"/>
+      <c r="G35" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="H35" s="45" t="s"/>
     </row>
     <row outlineLevel="0" r="36">
-      <c r="A36" s="33" t="n">
+      <c r="A36" s="32" t="n">
         <v>21</v>
       </c>
-      <c r="B36" s="27" t="n"/>
-      <c r="C36" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="39" t="s"/>
-      <c r="E36" s="36" t="n">
+      <c r="B36" s="26" t="n"/>
+      <c r="C36" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="38" t="s"/>
+      <c r="E36" s="35" t="n">
         <v>24</v>
       </c>
-      <c r="F36" s="27" t="n"/>
+      <c r="F36" s="26" t="n"/>
       <c r="G36" s="47" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H36" s="48" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row outlineLevel="0" r="37">
       <c r="A37" s="21" t="n">
         <v>22</v>
       </c>
-      <c r="B37" s="27" t="n"/>
+      <c r="B37" s="26" t="n"/>
       <c r="C37" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="29" t="n">
+      <c r="D37" s="28" t="n">
         <v>0.03</v>
       </c>
-      <c r="E37" s="36" t="n">
+      <c r="E37" s="35" t="n">
         <v>25</v>
       </c>
-      <c r="F37" s="27" t="n"/>
-      <c r="G37" s="28" t="s">
-        <v>79</v>
+      <c r="F37" s="26" t="n"/>
+      <c r="G37" s="27" t="s">
+        <v>80</v>
       </c>
       <c r="H37" s="45" t="s"/>
     </row>
@@ -3421,11 +3453,11 @@
       <c r="A38" s="21" t="n">
         <v>23</v>
       </c>
-      <c r="B38" s="27" t="n"/>
-      <c r="C38" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" s="39" t="s"/>
+      <c r="B38" s="26" t="n"/>
+      <c r="C38" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="38" t="s"/>
       <c r="E38" s="23" t="n">
         <v>26</v>
       </c>
@@ -3433,7 +3465,7 @@
       <c r="G38" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H38" s="30" t="n">
+      <c r="H38" s="29" t="n">
         <v>0.03</v>
       </c>
     </row>
@@ -3441,27 +3473,27 @@
       <c r="A39" s="21" t="n">
         <v>24</v>
       </c>
-      <c r="B39" s="27" t="n"/>
-      <c r="C39" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="39" t="s"/>
+      <c r="B39" s="26" t="n"/>
+      <c r="C39" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="38" t="s"/>
       <c r="E39" s="23" t="n">
         <v>27</v>
       </c>
-      <c r="F39" s="27" t="n"/>
-      <c r="G39" s="28" t="s">
-        <v>82</v>
+      <c r="F39" s="26" t="n"/>
+      <c r="G39" s="27" t="s">
+        <v>83</v>
       </c>
       <c r="H39" s="45" t="s"/>
     </row>
     <row outlineLevel="0" r="40">
-      <c r="A40" s="27" t="n"/>
+      <c r="A40" s="26" t="n"/>
       <c r="B40" s="17" t="n">
         <v>6</v>
       </c>
       <c r="C40" s="49" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D40" s="50" t="s"/>
       <c r="E40" s="14" t="s">
@@ -3481,27 +3513,27 @@
       <c r="A41" s="21" t="n">
         <v>25</v>
       </c>
-      <c r="B41" s="27" t="n"/>
+      <c r="B41" s="26" t="n"/>
       <c r="C41" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" s="41" t="s"/>
+        <v>85</v>
+      </c>
+      <c r="D41" s="40" t="s"/>
       <c r="E41" s="16" t="n"/>
       <c r="F41" s="19" t="n">
         <v>6</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="H41" s="43" t="s"/>
+        <v>86</v>
+      </c>
+      <c r="H41" s="42" t="s"/>
     </row>
     <row outlineLevel="0" r="42">
-      <c r="A42" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" s="27" t="n"/>
+      <c r="A42" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="26" t="n"/>
       <c r="C42" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D42" s="22" t="n">
         <v>3</v>
@@ -3509,17 +3541,17 @@
       <c r="E42" s="16" t="n"/>
       <c r="F42" s="16" t="n"/>
       <c r="G42" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="H42" s="43" t="s"/>
+        <v>88</v>
+      </c>
+      <c r="H42" s="42" t="s"/>
     </row>
     <row outlineLevel="0" r="43">
-      <c r="A43" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="27" t="n"/>
+      <c r="A43" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="26" t="n"/>
       <c r="C43" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D43" s="22" t="n">
         <v>4</v>
@@ -3529,19 +3561,19 @@
       </c>
       <c r="F43" s="16" t="n"/>
       <c r="G43" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H43" s="52" t="n">
         <v>2.2</v>
       </c>
     </row>
     <row outlineLevel="0" r="44">
-      <c r="A44" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="27" t="n"/>
+      <c r="A44" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="26" t="n"/>
       <c r="C44" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D44" s="22" t="n">
         <v>5</v>
@@ -3551,7 +3583,7 @@
       </c>
       <c r="F44" s="16" t="n"/>
       <c r="G44" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H44" s="52" t="n">
         <v>2.9</v>
@@ -3561,29 +3593,29 @@
       <c r="A45" s="21" t="n">
         <v>26</v>
       </c>
-      <c r="B45" s="27" t="n"/>
-      <c r="C45" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D45" s="39" t="s"/>
+      <c r="B45" s="26" t="n"/>
+      <c r="C45" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" s="38" t="s"/>
       <c r="E45" s="51" t="n">
         <v>30</v>
       </c>
       <c r="F45" s="16" t="n"/>
       <c r="G45" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H45" s="52" t="n">
         <v>3.65</v>
       </c>
     </row>
     <row outlineLevel="0" r="46">
-      <c r="A46" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" s="27" t="n"/>
+      <c r="A46" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="26" t="n"/>
       <c r="C46" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D46" s="22" t="n">
         <v>4</v>
@@ -3591,17 +3623,17 @@
       <c r="E46" s="16" t="n"/>
       <c r="F46" s="16" t="n"/>
       <c r="G46" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="H46" s="43" t="s"/>
+        <v>98</v>
+      </c>
+      <c r="H46" s="42" t="s"/>
     </row>
     <row outlineLevel="0" r="47">
-      <c r="A47" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="B47" s="27" t="n"/>
+      <c r="A47" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="26" t="n"/>
       <c r="C47" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D47" s="22" t="n">
         <v>0.75</v>
@@ -3611,65 +3643,65 @@
       </c>
       <c r="F47" s="16" t="n"/>
       <c r="G47" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H47" s="52" t="n">
         <v>4.5</v>
       </c>
     </row>
     <row outlineLevel="0" r="48">
-      <c r="A48" s="33" t="n">
+      <c r="A48" s="32" t="n">
         <v>27</v>
       </c>
-      <c r="B48" s="37" t="n"/>
+      <c r="B48" s="36" t="n"/>
       <c r="C48" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D48" s="41" t="s"/>
+        <v>101</v>
+      </c>
+      <c r="D48" s="40" t="s"/>
       <c r="E48" s="51" t="n">
         <v>32</v>
       </c>
       <c r="F48" s="16" t="n"/>
       <c r="G48" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H48" s="52" t="n">
         <v>5.65</v>
       </c>
     </row>
     <row outlineLevel="0" r="49">
-      <c r="A49" s="33" t="n">
+      <c r="A49" s="32" t="n">
         <v>28</v>
       </c>
-      <c r="B49" s="37" t="n"/>
+      <c r="B49" s="36" t="n"/>
       <c r="C49" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D49" s="41" t="s"/>
+        <v>103</v>
+      </c>
+      <c r="D49" s="40" t="s"/>
       <c r="E49" s="51" t="n">
         <v>33</v>
       </c>
       <c r="F49" s="16" t="n"/>
       <c r="G49" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H49" s="52" t="n">
         <v>8.1</v>
       </c>
     </row>
     <row outlineLevel="0" r="50">
-      <c r="A50" s="33" t="n">
+      <c r="A50" s="32" t="n">
         <v>29</v>
       </c>
-      <c r="B50" s="37" t="n"/>
+      <c r="B50" s="36" t="n"/>
       <c r="C50" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D50" s="41" t="s"/>
-      <c r="E50" s="27" t="n"/>
-      <c r="F50" s="27" t="n"/>
-      <c r="G50" s="28" t="s">
         <v>105</v>
+      </c>
+      <c r="D50" s="40" t="s"/>
+      <c r="E50" s="26" t="n"/>
+      <c r="F50" s="26" t="n"/>
+      <c r="G50" s="27" t="s">
+        <v>106</v>
       </c>
       <c r="H50" s="45" t="s"/>
     </row>
@@ -3677,55 +3709,55 @@
       <c r="A51" s="21" t="n">
         <v>30</v>
       </c>
-      <c r="B51" s="27" t="n"/>
-      <c r="C51" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="D51" s="29" t="n">
+      <c r="B51" s="26" t="n"/>
+      <c r="C51" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51" s="28" t="n">
         <v>0.01</v>
       </c>
       <c r="E51" s="51" t="n">
         <v>34</v>
       </c>
-      <c r="F51" s="27" t="n"/>
+      <c r="F51" s="26" t="n"/>
       <c r="G51" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="H51" s="40" t="s"/>
+        <v>108</v>
+      </c>
+      <c r="H51" s="39" t="s"/>
     </row>
     <row outlineLevel="0" r="52">
       <c r="A52" s="21" t="n">
         <v>31</v>
       </c>
-      <c r="B52" s="27" t="n"/>
-      <c r="C52" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="D52" s="39" t="s"/>
+      <c r="B52" s="26" t="n"/>
+      <c r="C52" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="38" t="s"/>
       <c r="E52" s="51" t="n">
         <v>35</v>
       </c>
-      <c r="F52" s="27" t="n"/>
-      <c r="G52" s="28" t="s">
-        <v>109</v>
+      <c r="F52" s="26" t="n"/>
+      <c r="G52" s="27" t="s">
+        <v>110</v>
       </c>
       <c r="H52" s="45" t="s"/>
     </row>
     <row outlineLevel="0" r="53">
-      <c r="A53" s="27" t="n"/>
+      <c r="A53" s="26" t="n"/>
       <c r="B53" s="17" t="n">
         <v>7</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="D53" s="42" t="s"/>
+        <v>111</v>
+      </c>
+      <c r="D53" s="41" t="s"/>
       <c r="E53" s="51" t="n">
         <v>36</v>
       </c>
-      <c r="F53" s="27" t="n"/>
-      <c r="G53" s="28" t="s">
-        <v>111</v>
+      <c r="F53" s="26" t="n"/>
+      <c r="G53" s="27" t="s">
+        <v>112</v>
       </c>
       <c r="H53" s="45" t="s"/>
     </row>
@@ -3733,17 +3765,17 @@
       <c r="A54" s="16" t="n"/>
       <c r="B54" s="16" t="n"/>
       <c r="C54" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D54" s="42" t="s"/>
-      <c r="E54" s="27" t="n"/>
+        <v>113</v>
+      </c>
+      <c r="D54" s="41" t="s"/>
+      <c r="E54" s="26" t="n"/>
       <c r="F54" s="19" t="n">
         <v>7</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H54" s="43" t="s"/>
+        <v>114</v>
+      </c>
+      <c r="H54" s="42" t="s"/>
     </row>
     <row outlineLevel="0" r="55">
       <c r="A55" s="21" t="n">
@@ -3751,7 +3783,7 @@
       </c>
       <c r="B55" s="16" t="n"/>
       <c r="C55" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D55" s="22" t="n">
         <v>2.64</v>
@@ -3761,7 +3793,7 @@
       </c>
       <c r="F55" s="16" t="n"/>
       <c r="G55" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H55" s="52" t="n">
         <v>4.5</v>
@@ -3773,7 +3805,7 @@
       </c>
       <c r="B56" s="16" t="n"/>
       <c r="C56" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D56" s="22" t="n">
         <v>3.48</v>
@@ -3783,7 +3815,7 @@
       </c>
       <c r="F56" s="16" t="n"/>
       <c r="G56" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H56" s="52" t="n">
         <v>5.65</v>
@@ -3795,7 +3827,7 @@
       </c>
       <c r="B57" s="16" t="n"/>
       <c r="C57" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D57" s="22" t="n">
         <v>4.38</v>
@@ -3805,7 +3837,7 @@
       </c>
       <c r="F57" s="16" t="n"/>
       <c r="G57" s="14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H57" s="52" t="n">
         <v>8.1</v>
@@ -3815,13 +3847,13 @@
       <c r="A58" s="16" t="n"/>
       <c r="B58" s="16" t="n"/>
       <c r="C58" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D58" s="42" t="s"/>
+        <v>121</v>
+      </c>
+      <c r="D58" s="41" t="s"/>
       <c r="E58" s="51" t="n">
         <v>40</v>
       </c>
-      <c r="F58" s="27" t="n"/>
+      <c r="F58" s="26" t="n"/>
       <c r="G58" s="14" t="s">
         <v>31</v>
       </c>
@@ -3835,7 +3867,7 @@
       </c>
       <c r="B59" s="16" t="n"/>
       <c r="C59" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D59" s="22" t="n">
         <v>5.4</v>
@@ -3843,9 +3875,9 @@
       <c r="E59" s="51" t="n">
         <v>41</v>
       </c>
-      <c r="F59" s="27" t="n"/>
-      <c r="G59" s="28" t="s">
-        <v>122</v>
+      <c r="F59" s="26" t="n"/>
+      <c r="G59" s="27" t="s">
+        <v>123</v>
       </c>
       <c r="H59" s="45" t="s"/>
     </row>
@@ -3855,19 +3887,19 @@
       </c>
       <c r="B60" s="16" t="n"/>
       <c r="C60" s="11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D60" s="22" t="n">
         <v>6.78</v>
       </c>
-      <c r="E60" s="27" t="n"/>
+      <c r="E60" s="26" t="n"/>
       <c r="F60" s="19" t="n">
         <v>8</v>
       </c>
       <c r="G60" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="H60" s="43" t="s"/>
+        <v>125</v>
+      </c>
+      <c r="H60" s="42" t="s"/>
     </row>
     <row outlineLevel="0" r="61">
       <c r="A61" s="21" t="n">
@@ -3875,7 +3907,7 @@
       </c>
       <c r="B61" s="16" t="n"/>
       <c r="C61" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D61" s="22" t="n">
         <v>9.72</v>
@@ -3885,37 +3917,37 @@
       </c>
       <c r="F61" s="16" t="n"/>
       <c r="G61" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H61" s="52" t="n">
         <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="62">
-      <c r="A62" s="27" t="n"/>
-      <c r="B62" s="27" t="n"/>
+      <c r="A62" s="26" t="n"/>
+      <c r="B62" s="26" t="n"/>
       <c r="C62" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="D62" s="41" t="s"/>
+        <v>127</v>
+      </c>
+      <c r="D62" s="40" t="s"/>
       <c r="E62" s="51" t="n">
         <v>43</v>
       </c>
       <c r="F62" s="16" t="n"/>
       <c r="G62" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H62" s="52" t="n">
         <v>30</v>
       </c>
     </row>
     <row outlineLevel="0" r="63">
-      <c r="A63" s="33" t="n">
+      <c r="A63" s="32" t="n">
         <v>38</v>
       </c>
-      <c r="B63" s="27" t="n"/>
+      <c r="B63" s="26" t="n"/>
       <c r="C63" s="54" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D63" s="55" t="s"/>
       <c r="E63" s="51" t="n">
@@ -3923,7 +3955,7 @@
       </c>
       <c r="F63" s="16" t="n"/>
       <c r="G63" s="14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H63" s="52" t="n">
         <v>42.5</v>
@@ -3933,17 +3965,17 @@
       <c r="A64" s="21" t="n">
         <v>39</v>
       </c>
-      <c r="B64" s="27" t="n"/>
+      <c r="B64" s="26" t="n"/>
       <c r="C64" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D64" s="41" t="s"/>
+        <v>129</v>
+      </c>
+      <c r="D64" s="40" t="s"/>
       <c r="E64" s="16" t="n"/>
       <c r="F64" s="19" t="n">
         <v>9</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H64" s="16" t="n"/>
     </row>
@@ -3953,15 +3985,15 @@
       </c>
       <c r="B65" s="57" t="n"/>
       <c r="C65" s="58" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D65" s="59" t="s"/>
       <c r="E65" s="51" t="n">
         <v>45</v>
       </c>
-      <c r="F65" s="27" t="n"/>
-      <c r="G65" s="28" t="s">
-        <v>131</v>
+      <c r="F65" s="26" t="n"/>
+      <c r="G65" s="27" t="s">
+        <v>132</v>
       </c>
       <c r="H65" s="53" t="n">
         <v>0.03</v>
@@ -3973,15 +4005,15 @@
         <v>7</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="D66" s="42" t="s"/>
-      <c r="E66" s="27" t="n"/>
-      <c r="F66" s="27" t="n"/>
+        <v>133</v>
+      </c>
+      <c r="D66" s="41" t="s"/>
+      <c r="E66" s="26" t="n"/>
+      <c r="F66" s="26" t="n"/>
       <c r="G66" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="H66" s="40" t="s"/>
+        <v>134</v>
+      </c>
+      <c r="H66" s="39" t="s"/>
     </row>
     <row outlineLevel="0" r="67">
       <c r="A67" s="21" t="n">
@@ -3989,7 +4021,7 @@
       </c>
       <c r="B67" s="16" t="n"/>
       <c r="C67" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D67" s="22" t="n">
         <v>5.4</v>
@@ -3997,9 +4029,9 @@
       <c r="E67" s="51" t="n">
         <v>46</v>
       </c>
-      <c r="F67" s="37" t="n"/>
-      <c r="G67" s="28" t="s">
-        <v>135</v>
+      <c r="F67" s="36" t="n"/>
+      <c r="G67" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="H67" s="61" t="n">
         <v>0.0233</v>
@@ -4011,7 +4043,7 @@
       </c>
       <c r="B68" s="16" t="n"/>
       <c r="C68" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D68" s="22" t="n">
         <v>6.78</v>
@@ -4019,9 +4051,9 @@
       <c r="E68" s="51" t="n">
         <v>47</v>
       </c>
-      <c r="F68" s="37" t="n"/>
-      <c r="G68" s="28" t="s">
-        <v>137</v>
+      <c r="F68" s="36" t="n"/>
+      <c r="G68" s="27" t="s">
+        <v>138</v>
       </c>
       <c r="H68" s="61" t="n">
         <v>0.0233</v>
@@ -4033,7 +4065,7 @@
       </c>
       <c r="B69" s="16" t="n"/>
       <c r="C69" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D69" s="22" t="n">
         <v>9.72</v>
@@ -4041,9 +4073,9 @@
       <c r="E69" s="62" t="n">
         <v>48</v>
       </c>
-      <c r="F69" s="37" t="n"/>
+      <c r="F69" s="36" t="n"/>
       <c r="G69" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H69" s="63" t="n">
         <v>0.015</v>
@@ -4057,31 +4089,31 @@
       <c r="C70" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D70" s="29" t="n">
+      <c r="D70" s="28" t="n">
         <v>0.03</v>
       </c>
-      <c r="E70" s="37" t="n"/>
-      <c r="F70" s="37" t="n"/>
+      <c r="E70" s="36" t="n"/>
+      <c r="F70" s="36" t="n"/>
       <c r="G70" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H70" s="40" t="s"/>
+        <v>141</v>
+      </c>
+      <c r="H70" s="39" t="s"/>
     </row>
     <row outlineLevel="0" r="71">
-      <c r="A71" s="33" t="n">
+      <c r="A71" s="32" t="n">
         <v>45</v>
       </c>
-      <c r="B71" s="27" t="n"/>
+      <c r="B71" s="26" t="n"/>
       <c r="C71" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="D71" s="41" t="s"/>
+        <v>142</v>
+      </c>
+      <c r="D71" s="40" t="s"/>
       <c r="E71" s="62" t="n">
         <v>49</v>
       </c>
-      <c r="F71" s="37" t="n"/>
+      <c r="F71" s="36" t="n"/>
       <c r="G71" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H71" s="64" t="n">
         <v>0.0233</v>
@@ -4093,27 +4125,27 @@
         <v>8</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D72" s="16" t="n"/>
       <c r="E72" s="62" t="n">
         <v>50</v>
       </c>
-      <c r="F72" s="27" t="n"/>
-      <c r="G72" s="28" t="s">
-        <v>144</v>
+      <c r="F72" s="26" t="n"/>
+      <c r="G72" s="27" t="s">
+        <v>145</v>
       </c>
       <c r="H72" s="46" t="n">
         <v>0.015</v>
       </c>
     </row>
     <row outlineLevel="0" r="73">
-      <c r="A73" s="33" t="n">
+      <c r="A73" s="32" t="n">
         <v>46</v>
       </c>
-      <c r="B73" s="27" t="n"/>
+      <c r="B73" s="26" t="n"/>
       <c r="C73" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D73" s="65" t="n">
         <v>0.03</v>
@@ -4121,41 +4153,41 @@
       <c r="E73" s="62" t="n">
         <v>51</v>
       </c>
-      <c r="F73" s="37" t="n"/>
+      <c r="F73" s="36" t="n"/>
       <c r="G73" s="14" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H73" s="46" t="n">
         <v>0.005</v>
       </c>
     </row>
     <row outlineLevel="0" r="74">
-      <c r="A74" s="33" t="n">
+      <c r="A74" s="32" t="n">
         <v>47</v>
       </c>
-      <c r="B74" s="37" t="n"/>
+      <c r="B74" s="36" t="n"/>
       <c r="C74" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D74" s="41" t="s"/>
+        <v>148</v>
+      </c>
+      <c r="D74" s="40" t="s"/>
       <c r="E74" s="51" t="n">
         <v>52</v>
       </c>
-      <c r="F74" s="27" t="n"/>
-      <c r="G74" s="28" t="s">
-        <v>148</v>
+      <c r="F74" s="26" t="n"/>
+      <c r="G74" s="27" t="s">
+        <v>149</v>
       </c>
       <c r="H74" s="66" t="n">
         <v>0.009</v>
       </c>
     </row>
     <row outlineLevel="0" r="75">
-      <c r="A75" s="33" t="n">
+      <c r="A75" s="32" t="n">
         <v>48</v>
       </c>
-      <c r="B75" s="37" t="n"/>
+      <c r="B75" s="36" t="n"/>
       <c r="C75" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D75" s="65" t="n">
         <v>0.015</v>
@@ -4165,27 +4197,27 @@
         <v>8</v>
       </c>
       <c r="G75" s="20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H75" s="16" t="n"/>
     </row>
     <row outlineLevel="0" r="76">
-      <c r="A76" s="33" t="n">
+      <c r="A76" s="32" t="n">
         <v>49</v>
       </c>
-      <c r="B76" s="37" t="n"/>
+      <c r="B76" s="36" t="n"/>
       <c r="C76" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D76" s="35" t="n">
+        <v>152</v>
+      </c>
+      <c r="D76" s="34" t="n">
         <v>0.01</v>
       </c>
       <c r="E76" s="51" t="n">
         <v>53</v>
       </c>
-      <c r="F76" s="37" t="n"/>
-      <c r="G76" s="28" t="s">
-        <v>152</v>
+      <c r="F76" s="36" t="n"/>
+      <c r="G76" s="27" t="s">
+        <v>153</v>
       </c>
       <c r="H76" s="45" t="s"/>
     </row>
@@ -4195,33 +4227,33 @@
         <v>9</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="D77" s="42" t="s"/>
+        <v>154</v>
+      </c>
+      <c r="D77" s="41" t="s"/>
       <c r="E77" s="16" t="n"/>
       <c r="F77" s="19" t="n">
         <v>9</v>
       </c>
       <c r="G77" s="20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H77" s="16" t="n"/>
     </row>
     <row outlineLevel="0" r="78">
-      <c r="A78" s="33" t="n">
+      <c r="A78" s="32" t="n">
         <v>50</v>
       </c>
-      <c r="B78" s="37" t="n"/>
+      <c r="B78" s="36" t="n"/>
       <c r="C78" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="D78" s="41" t="s"/>
+        <v>156</v>
+      </c>
+      <c r="D78" s="40" t="s"/>
       <c r="E78" s="62" t="n">
         <v>54</v>
       </c>
-      <c r="F78" s="27" t="n"/>
-      <c r="G78" s="28" t="s">
-        <v>156</v>
+      <c r="F78" s="26" t="n"/>
+      <c r="G78" s="27" t="s">
+        <v>157</v>
       </c>
       <c r="H78" s="45" t="s"/>
     </row>
@@ -4231,15 +4263,15 @@
         <v>10</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="D79" s="42" t="s"/>
+        <v>158</v>
+      </c>
+      <c r="D79" s="41" t="s"/>
       <c r="E79" s="62" t="n">
         <v>55</v>
       </c>
-      <c r="F79" s="27" t="n"/>
-      <c r="G79" s="28" t="s">
-        <v>158</v>
+      <c r="F79" s="26" t="n"/>
+      <c r="G79" s="27" t="s">
+        <v>159</v>
       </c>
       <c r="H79" s="46" t="n">
         <v>0.03</v>
@@ -4251,7 +4283,7 @@
       </c>
       <c r="B80" s="16" t="n"/>
       <c r="C80" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D80" s="22" t="n">
         <v>0.72</v>
@@ -4259,9 +4291,9 @@
       <c r="E80" s="51" t="n">
         <v>56</v>
       </c>
-      <c r="F80" s="27" t="n"/>
-      <c r="G80" s="28" t="s">
-        <v>160</v>
+      <c r="F80" s="26" t="n"/>
+      <c r="G80" s="27" t="s">
+        <v>161</v>
       </c>
       <c r="H80" s="45" t="s"/>
     </row>
@@ -4271,7 +4303,7 @@
       </c>
       <c r="B81" s="16" t="n"/>
       <c r="C81" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D81" s="22" t="n">
         <v>2.34</v>
@@ -4281,9 +4313,9 @@
         <v>10</v>
       </c>
       <c r="G81" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="H81" s="43" t="s"/>
+        <v>163</v>
+      </c>
+      <c r="H81" s="42" t="s"/>
     </row>
     <row outlineLevel="0" r="82">
       <c r="A82" s="21" t="n">
@@ -4291,7 +4323,7 @@
       </c>
       <c r="B82" s="16" t="n"/>
       <c r="C82" s="11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D82" s="22" t="n">
         <v>0.54</v>
@@ -4301,7 +4333,7 @@
       </c>
       <c r="F82" s="16" t="n"/>
       <c r="G82" s="14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H82" s="24" t="n">
         <v>0.6</v>
@@ -4313,7 +4345,7 @@
         <v>11</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D83" s="16" t="n"/>
       <c r="E83" s="51" t="n">
@@ -4321,7 +4353,7 @@
       </c>
       <c r="F83" s="16" t="n"/>
       <c r="G83" s="14" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H83" s="24" t="n">
         <v>1.95</v>
@@ -4331,17 +4363,17 @@
       <c r="A84" s="21" t="n">
         <v>54</v>
       </c>
-      <c r="B84" s="37" t="n"/>
+      <c r="B84" s="36" t="n"/>
       <c r="C84" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="D84" s="41" t="s"/>
+        <v>168</v>
+      </c>
+      <c r="D84" s="40" t="s"/>
       <c r="E84" s="51" t="n">
         <v>59</v>
       </c>
       <c r="F84" s="16" t="n"/>
       <c r="G84" s="14" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H84" s="24" t="n">
         <v>0.45</v>
@@ -4353,17 +4385,17 @@
         <v>11</v>
       </c>
       <c r="G85" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="H85" s="43" t="s"/>
+        <v>170</v>
+      </c>
+      <c r="H85" s="42" t="s"/>
     </row>
     <row outlineLevel="0" r="86">
       <c r="E86" s="51" t="n">
         <v>60</v>
       </c>
-      <c r="F86" s="27" t="n"/>
-      <c r="G86" s="28" t="s">
-        <v>170</v>
+      <c r="F86" s="26" t="n"/>
+      <c r="G86" s="27" t="s">
+        <v>171</v>
       </c>
       <c r="H86" s="45" t="s"/>
     </row>
@@ -4373,19 +4405,19 @@
       </c>
       <c r="F87" s="16" t="n"/>
       <c r="G87" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="H87" s="40" t="s"/>
+        <v>172</v>
+      </c>
+      <c r="H87" s="39" t="s"/>
     </row>
     <row outlineLevel="0" r="88">
       <c r="E88" s="51" t="n">
         <v>62</v>
       </c>
-      <c r="F88" s="27" t="n"/>
+      <c r="F88" s="26" t="n"/>
       <c r="G88" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="H88" s="40" t="s"/>
+        <v>173</v>
+      </c>
+      <c r="H88" s="39" t="s"/>
     </row>
     <row outlineLevel="0" r="89">
       <c r="E89" s="16" t="n"/>
@@ -4393,17 +4425,17 @@
         <v>12</v>
       </c>
       <c r="G89" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="H89" s="43" t="s"/>
+        <v>151</v>
+      </c>
+      <c r="H89" s="42" t="s"/>
     </row>
     <row outlineLevel="0" r="90">
       <c r="E90" s="62" t="n">
         <v>63</v>
       </c>
-      <c r="F90" s="27" t="n"/>
-      <c r="G90" s="28" t="s">
-        <v>173</v>
+      <c r="F90" s="26" t="n"/>
+      <c r="G90" s="27" t="s">
+        <v>174</v>
       </c>
       <c r="H90" s="45" t="s"/>
     </row>

</xml_diff>

<commit_message>
find ems table row
</commit_message>
<xml_diff>
--- a/calc/files/letter2.xlsx
+++ b/calc/files/letter2.xlsx
@@ -53,16 +53,16 @@
         <rFont val="Microsoft Sans Serif"/>
         <sz val="9"/>
       </rPr>
-      <t>№987  от  28.09.2023</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Microsoft Sans Serif"/>
-        <sz val="8.5"/>
-      </rPr>
-      <t>от 06.04.2023 №350</t>
+      <t>04 марта 2024 № 222</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Microsoft Sans Serif"/>
+        <sz val="8.5"/>
+      </rPr>
+      <t>от 04/03.2024 №222</t>
     </r>
   </si>
   <si>
@@ -93,7 +93,7 @@
         <color rgb="FF0000" tint="0"/>
         <sz val="9"/>
       </rPr>
-      <t>в действии c 09.10.2023</t>
+      <t>в действии c 01.04.2024</t>
     </r>
   </si>
   <si>
@@ -105,7 +105,7 @@
         <color rgb="FF0000" tint="0"/>
         <sz val="8.5"/>
       </rPr>
-      <t>в действии c 11.04.2023</t>
+      <t>в действии c 01.04.2024</t>
     </r>
   </si>
   <si>
@@ -456,7 +456,7 @@
         <rFont val="Microsoft Sans Serif"/>
         <sz val="8.5"/>
       </rPr>
-      <t>За хрупкие мелкие пакеты с объявленной ценностью  с отметкой "Осторожно" взимается надбавка к плате за  пересылку  мелкого  пакета   в  размере  50%.  На  плату  за  объявленную  ценность  мелкого  пакета надбавка не распространяется</t>
+      <t>За хрупкие мелкие пакеты с объявленной ценностью  с отметкой "Хрупкое" взимается надбавка к плате за  пересылку  мелкого  пакета   в  размере  50%.  На  плату  за  объявленную  ценность  мелкого  пакета надбавка не распространяется</t>
     </r>
   </si>
   <si>
@@ -2747,7 +2747,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="22" t="n">
-        <v>2.52</v>
+        <v>2.7</v>
       </c>
       <c r="E8" s="23" t="n">
         <v>1</v>
@@ -2757,11 +2757,11 @@
         <v>21</v>
       </c>
       <c r="H8" s="24" t="n">
-        <v>2.1</v>
+        <v>2.25</v>
       </c>
       <c r="I8" s="25" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">H8*1.2</f>
-        <v>2.52</v>
+        <v>2.6999999999999997</v>
       </c>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="9">
@@ -2792,7 +2792,7 @@
         <v>24</v>
       </c>
       <c r="D10" s="22" t="n">
-        <v>2.76</v>
+        <v>3</v>
       </c>
       <c r="E10" s="23" t="n">
         <v>2</v>
@@ -2802,11 +2802,11 @@
         <v>25</v>
       </c>
       <c r="H10" s="24" t="n">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="I10" s="25" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">H10*1.2</f>
-        <v>2.76</v>
+        <v>3</v>
       </c>
       <c r="J10" s="25" t="n"/>
       <c r="K10" s="25" t="n"/>
@@ -2820,7 +2820,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="22" t="n">
-        <v>3.24</v>
+        <v>3.48</v>
       </c>
       <c r="E11" s="23" t="n">
         <v>3</v>
@@ -2830,19 +2830,19 @@
         <v>27</v>
       </c>
       <c r="H11" s="24" t="n">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="I11" s="25" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">H11*1.2</f>
-        <v>3.5999999999999996</v>
+        <v>3.84</v>
       </c>
       <c r="J11" s="25" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">I11+0.36</f>
-        <v>3.9599999999999995</v>
+        <v>4.2</v>
       </c>
       <c r="K11" s="25" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">J11/1.2*0.2</f>
-        <v>0.66</v>
+        <v>0.7000000000000002</v>
       </c>
     </row>
     <row customHeight="true" ht="27.25" outlineLevel="0" r="12">
@@ -2929,7 +2929,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="22" t="n">
-        <v>0.78</v>
+        <v>0.84</v>
       </c>
       <c r="E15" s="23" t="n">
         <v>6</v>
@@ -2939,11 +2939,11 @@
         <v>35</v>
       </c>
       <c r="H15" s="24" t="n">
-        <v>0.65</v>
+        <v>0.7</v>
       </c>
       <c r="I15" s="25" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">H15*1.2</f>
-        <v>0.78</v>
+        <v>0.84</v>
       </c>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="16">
@@ -2955,7 +2955,7 @@
         <v>36</v>
       </c>
       <c r="D16" s="22" t="n">
-        <v>2.76</v>
+        <v>3</v>
       </c>
       <c r="E16" s="23" t="n">
         <v>7</v>
@@ -2965,11 +2965,11 @@
         <v>37</v>
       </c>
       <c r="H16" s="24" t="n">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="I16" s="25" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">H16*1.2</f>
-        <v>2.76</v>
+        <v>3</v>
       </c>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="17">
@@ -2981,7 +2981,7 @@
         <v>38</v>
       </c>
       <c r="D17" s="22" t="n">
-        <v>3.24</v>
+        <v>3.48</v>
       </c>
       <c r="E17" s="31" t="n">
         <v>8</v>
@@ -2991,11 +2991,11 @@
         <v>39</v>
       </c>
       <c r="H17" s="24" t="n">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="I17" s="25" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">H17*1.2</f>
-        <v>3.5999999999999996</v>
+        <v>3.84</v>
       </c>
     </row>
     <row customHeight="true" ht="35.25" outlineLevel="0" r="18">
@@ -3117,7 +3117,7 @@
         <v>48</v>
       </c>
       <c r="D23" s="22" t="n">
-        <v>1.68</v>
+        <v>1.86</v>
       </c>
       <c r="E23" s="23" t="n">
         <v>13</v>
@@ -3127,11 +3127,11 @@
         <v>49</v>
       </c>
       <c r="H23" s="24" t="n">
-        <v>1.4</v>
+        <v>1.55</v>
       </c>
       <c r="I23" s="25" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">H23*1.2</f>
-        <v>1.68</v>
+        <v>1.8599999999999999</v>
       </c>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="24">
@@ -3243,7 +3243,7 @@
         <v>61</v>
       </c>
       <c r="D29" s="22" t="n">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="E29" s="23" t="n">
         <v>17</v>
@@ -3314,7 +3314,7 @@
       <c r="H31" s="45" t="s"/>
       <c r="I31" s="25" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D31+1.8*D32</f>
-        <v>5.35</v>
+        <v>5.44</v>
       </c>
       <c r="J31" s="0" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">ROUND(10.72*0.03, 2)</f>
@@ -3322,7 +3322,7 @@
       </c>
       <c r="K31" s="25" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">J31+I31</f>
-        <v>5.67</v>
+        <v>5.760000000000001</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="45" outlineLevel="0" r="32">
@@ -3334,7 +3334,7 @@
         <v>69</v>
       </c>
       <c r="D32" s="22" t="n">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="E32" s="35" t="n">
         <v>20</v>
@@ -3563,7 +3563,7 @@
         <v>90</v>
       </c>
       <c r="H43" s="52" t="n">
-        <v>2.2</v>
+        <v>2.35</v>
       </c>
     </row>
     <row outlineLevel="0" r="44">
@@ -3585,7 +3585,7 @@
         <v>93</v>
       </c>
       <c r="H44" s="52" t="n">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
     </row>
     <row outlineLevel="0" r="45">
@@ -3605,7 +3605,7 @@
         <v>95</v>
       </c>
       <c r="H45" s="52" t="n">
-        <v>3.65</v>
+        <v>3.9</v>
       </c>
     </row>
     <row outlineLevel="0" r="46">
@@ -3635,7 +3635,7 @@
         <v>69</v>
       </c>
       <c r="D47" s="22" t="n">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="E47" s="51" t="n">
         <v>31</v>
@@ -3785,7 +3785,7 @@
         <v>114</v>
       </c>
       <c r="D55" s="22" t="n">
-        <v>2.64</v>
+        <v>2.82</v>
       </c>
       <c r="E55" s="51" t="n">
         <v>37</v>
@@ -3807,7 +3807,7 @@
         <v>116</v>
       </c>
       <c r="D56" s="22" t="n">
-        <v>3.48</v>
+        <v>3.72</v>
       </c>
       <c r="E56" s="51" t="n">
         <v>38</v>
@@ -3829,7 +3829,7 @@
         <v>118</v>
       </c>
       <c r="D57" s="22" t="n">
-        <v>4.38</v>
+        <v>9.72</v>
       </c>
       <c r="E57" s="51" t="n">
         <v>39</v>
@@ -4285,7 +4285,7 @@
         <v>159</v>
       </c>
       <c r="D80" s="22" t="n">
-        <v>0.72</v>
+        <v>0.78</v>
       </c>
       <c r="E80" s="51" t="n">
         <v>56</v>
@@ -4305,7 +4305,7 @@
         <v>161</v>
       </c>
       <c r="D81" s="22" t="n">
-        <v>2.34</v>
+        <v>2.52</v>
       </c>
       <c r="E81" s="16" t="n"/>
       <c r="F81" s="19" t="n">
@@ -4335,7 +4335,7 @@
         <v>164</v>
       </c>
       <c r="H82" s="24" t="n">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
     </row>
     <row outlineLevel="0" r="83">
@@ -4355,7 +4355,7 @@
         <v>166</v>
       </c>
       <c r="H83" s="24" t="n">
-        <v>1.95</v>
+        <v>2.1</v>
       </c>
     </row>
     <row outlineLevel="0" r="84">

</xml_diff>

<commit_message>
ems documents and goods cost
</commit_message>
<xml_diff>
--- a/calc/files/letter2.xlsx
+++ b/calc/files/letter2.xlsx
@@ -3253,7 +3253,10 @@
         <v>4.5</v>
       </c>
       <c r="I29" s="44" t="n"/>
-      <c r="J29" s="44" t="n"/>
+      <c r="J29" s="44" t="n">
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">6.82/120*20</f>
+        <v>1.1366666666666667</v>
+      </c>
       <c r="K29" s="44" t="n"/>
     </row>
     <row customHeight="true" ht="28.75" outlineLevel="0" r="30">
@@ -3276,26 +3279,14 @@
         <v>0.8</v>
       </c>
       <c r="J30" s="0" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="K30" s="0" t="n">
-        <v>3.46</v>
-      </c>
-      <c r="L30" s="0" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">J30*K30+J31</f>
-        <v>6.768000000000001</v>
-      </c>
-      <c r="M30" s="0" t="n">
-        <v>8.85</v>
-      </c>
-      <c r="N30" s="0" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">M30*3/100</f>
-        <v>0.26549999999999996</v>
-      </c>
-      <c r="O30" s="0" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">N30*1.2</f>
-        <v>0.31859999999999994</v>
-      </c>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">4.5/120*20</f>
+        <v>0.75</v>
+      </c>
+      <c r="K30" s="0" t="n"/>
+      <c r="L30" s="0" t="n"/>
+      <c r="M30" s="0" t="n"/>
+      <c r="N30" s="0" t="n"/>
+      <c r="O30" s="0" t="n"/>
     </row>
     <row customHeight="true" ht="45.4999389648438" outlineLevel="0" r="31">
       <c r="A31" s="43" t="s">
@@ -3317,14 +3308,9 @@
       </c>
       <c r="H31" s="45" t="s"/>
       <c r="I31" s="25" t="n"/>
-      <c r="J31" s="0" t="n">
-        <v>4</v>
-      </c>
+      <c r="J31" s="0" t="n"/>
       <c r="K31" s="25" t="n"/>
-      <c r="N31" s="0" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">L30+N30</f>
-        <v>7.033500000000001</v>
-      </c>
+      <c r="N31" s="0" t="n"/>
     </row>
     <row customHeight="true" hidden="false" ht="45" outlineLevel="0" r="32">
       <c r="A32" s="43" t="s">

</xml_diff>

<commit_message>
QR box yur, rounding, package USA
</commit_message>
<xml_diff>
--- a/calc/files/letter2.xlsx
+++ b/calc/files/letter2.xlsx
@@ -700,9 +700,10 @@
       <rPr>
         <rFont val="Arial"/>
         <b val="true"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Услуга "Оплаченная пересылка" (без учета стоимости упаковки)</t>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Пересылка посылки QR</t>
     </r>
   </si>
   <si>
@@ -718,10 +719,10 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <b val="true"/>
-        <sz val="11"/>
-      </rPr>
-      <t>пересылка заказного мелкого пакета ( в т.ч. принятого посредством почтомата)</t>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>плата за отправление</t>
     </r>
   </si>
   <si>
@@ -746,9 +747,10 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Размер S (229х324)</t>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>плата за объявленную ценность, % от суммы объявленной ценности, но не менее 0,50 руб</t>
     </r>
   </si>
   <si>
@@ -773,22 +775,10 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Размер M (280х380)</t>
-    </r>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>За пересылку посылки массой свыше 5 кг до 50 кг взимается плата за отправление и за массу</t>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>За  досылку и  (или)  возвращение  посылок  без  объявленной  ценности  и  с  объявленной  ценностью</t>
     </r>
     <r>
       <t xml:space="preserve">
@@ -800,135 +790,20 @@
         <color rgb="000000" tint="0"/>
         <sz val="11"/>
       </rPr>
-      <t>посылки</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Размер L (320х355)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>24.1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b val="true"/>
-        <sz val="11"/>
-      </rPr>
-      <t>пересылка посылки (в т.ч. принятой посредством почтомата)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>24.2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Размер S (270х175х60)</t>
-    </r>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Тарификация  за  массу  посылки  массой  свыше  5  кг  без  объявленной  ценности  осуществляется  с точностью до сотен граммов. Любое количество граммов округляется до сотни граммов в большую сторону</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Размер M (320х220х110)</t>
-    </r>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Тарификация  за  массу  посылки  массой  свыше  5  кг  с  объявленной  ценностью  осуществляется  с точностью  до  десятков  граммов.  Любое  количество  граммов  округляется  до  десятков  граммов  в большую сторону</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Размер L (400х250х200)</t>
-    </r>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>За хрупкие посылки с отметкой "Хрупкое и громоздкие взимается надбавка к плате за пересылку посылки   в   размере   50%.   Если   посылка   является   одновременно   хрупкой   и   громоздкой,   то дополнительная плата взимается только один раз</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t xml:space="preserve">Тариф на услугу "Оплаченная пересылка" установлен без учета стоимости упаковки (пластиковый </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>конверт, коробка)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>плата за объявленную ценность, % от суммы объявленной ценности,</t>
+      <t>взимается плата за пересылку посылки  (поз.26)</t>
+    </r>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>За пересылку посылки массой свыше 5 кг до 50 кг взимается плата за отправление и за массу</t>
     </r>
     <r>
       <t xml:space="preserve">
@@ -940,26 +815,129 @@
         <color rgb="000000" tint="0"/>
         <sz val="11"/>
       </rPr>
-      <t>но не менее 0,50 руб.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>За возвращение заказных мелких пакетов в оплаченной упаковке плата не взимается</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>За  досылку и  (или)  возвращение  посылок  без  объявленной  ценности  и  с  объявленной  ценностью</t>
+      <t>посылки</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="true"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Услуга "Оплаченная пересылка" (без учета стоимости упаковки)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>24.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="true"/>
+        <sz val="11"/>
+      </rPr>
+      <t>пересылка заказного мелкого пакета ( в т.ч. принятого посредством почтомата)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>24.2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Размер S (229х324)</t>
+    </r>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Тарификация  за  массу  посылки  массой  свыше  5  кг  без  объявленной  ценности  осуществляется  с точностью до сотен граммов. Любое количество граммов округляется до сотни граммов в большую сторону</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Размер M (280х380)</t>
+    </r>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Тарификация  за  массу  посылки  массой  свыше  5  кг  с  объявленной  ценностью  осуществляется  с точностью  до  десятков  граммов.  Любое  количество  граммов  округляется  до  десятков  граммов  в большую сторону</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Размер L (320х355)</t>
+    </r>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>За хрупкие посылки с отметкой "Хрупкое и громоздкие взимается надбавка к плате за пересылку посылки   в   размере   50%.   Если   посылка   является   одновременно   хрупкой   и   громоздкой,   то дополнительная плата взимается только один раз</t>
+    </r>
+  </si>
+  <si/>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="true"/>
+        <sz val="11"/>
+      </rPr>
+      <t>пересылка посылки (в т.ч. принятой посредством почтомата)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>плата за объявленную ценность, % от суммы объявленной ценности,</t>
     </r>
     <r>
       <t xml:space="preserve">
@@ -971,17 +949,26 @@
         <color rgb="000000" tint="0"/>
         <sz val="11"/>
       </rPr>
-      <t>взимается плата за пересылку посылки  (поз.23-24)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>За  досылку  заказных  мелких  пакетов  в  оплаченной  упаковке  по  письменному  распоряжению  взимается</t>
+      <t>но не менее 0,50 руб.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Размер S (270х175х60)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>За  досылку и  (или)  возвращение  посылок  без  объявленной  ценности  и  с  объявленной  ценностью</t>
     </r>
     <r>
       <t xml:space="preserve">
@@ -993,75 +980,52 @@
         <color rgb="000000" tint="0"/>
         <sz val="11"/>
       </rPr>
-      <t>плата за пересылку заказного мелкого пакета (поз. 26, 27, 28)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b val="true"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Пересылка посылки QR</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t xml:space="preserve">За досылку и (или) возвращение посылок в оплаченной упаковке взимается плата за пересылку посылки </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>(поз. 31,32,33)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>плата за отправление</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b val="true"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Пересылка посылки, принятой посредством почтомата</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>плата за объявленную ценность, % от суммы объявленной ценности, но не менее 0,50 руб</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Размер ячейки S  (119,4x400x500)</t>
+      <t>взимается плата за пересылку посылки  (поз.23-24)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Размер M (320х220х110)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Размер L (400х250х200)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">Тариф на услугу "Оплаченная пересылка" установлен без учета стоимости упаковки (пластиковый </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>конверт, коробка)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>За возвращение заказных мелких пакетов в оплаченной упаковке плата не взимается</t>
     </r>
   </si>
   <si>
@@ -1090,102 +1054,10 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Размер ячейки M  (245,4x400x500)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Размер ячейки L (379x400x500)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t xml:space="preserve">За   досылку   и   (или)   возвращение   посылок,   принятых   посредством   почтомата,   взимается   плата   за </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>пересылку посылки  (согласно поз. 35, 36, 37)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b val="true"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Услуга по доступу и управлению ячейкой почтомата, в месяц</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b val="true"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Пересылка почтового денежного перевода</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t xml:space="preserve">Плата  за  пересылку  почтового  денежного  перевода  с  выплатой  в  ОПС,  %  от </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>суммы перевода, но не менее 1,00 руб.**</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Тариф на услугу "Оплаченная пересылка" установлен без учета стоимости упаковки (пластиковый конверт, коробка)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>**При  пересылке  почтового  денежного  перевода  суммой  свыше  150,00  руб.  предоставляются  скидки согласно действующему Положению о порядке применения скидок</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Плата  за  пересылку,  доставку  и  выплату  почтового  денежного  перевода  с пенсиями   и   другими   социальными   выплатами   (выплатами   на   погребение, единовременной материальной помощью), % от суммы перевода, но не менее</t>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>За  досылку  заказных  мелких  пакетов  в  оплаченной  упаковке  по  письменному  распоряжению  взимается</t>
     </r>
     <r>
       <t xml:space="preserve">
@@ -1197,7 +1069,99 @@
         <color rgb="000000" tint="0"/>
         <sz val="11"/>
       </rPr>
-      <t>минимальной денежной единицы</t>
+      <t>плата за пересылку заказного мелкого пакета (поз. 26, 27, 28)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">За досылку и (или) возвращение посылок в оплаченной упаковке взимается плата за пересылку посылки </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>(поз. 31,32,33)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="true"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Пересылка посылки, принятой посредством почтомата</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Размер ячейки S  (119,4x400x500)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Размер ячейки M  (245,4x400x500)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Размер ячейки L (379x400x500)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">За   досылку   и   (или)   возвращение   посылок,   принятых   посредством   почтомата,   взимается   плата   за </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>пересылку посылки  (согласно поз. 35, 36, 37)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="true"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Услуга по доступу и управлению ячейкой почтомата, в месяц</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Тариф на услугу "Оплаченная пересылка" установлен без учета стоимости упаковки (пластиковый конверт, коробка)</t>
     </r>
   </si>
   <si>
@@ -1213,18 +1177,10 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t xml:space="preserve">Плата  за  пересылку,  доставку  и  выплату  почтового  денежного  перевода  с вознаграждением     за     проведение     социальных     мероприятий     (перепись населения,  обследование  домашних  хозяйств),  %  от  суммы  перевода,   но  не </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>менее 0,20 руб.</t>
+        <b val="true"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Пересылка почтового денежного перевода</t>
     </r>
   </si>
   <si>
@@ -1240,18 +1196,27 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Плата  за  пересылку  почтового  денежного  перевода  с  выплатой  за  сданную сельскохозяйственную  продукцию,  %  от  суммы  перевода,  но  не  менее  0,20 руб. ***</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>***   При   пересылке    почтового   денежного   перевода  с   выплатами  за   сданную   сельскохозяйственную продукцию  суммой  свыше  20,00  рублей  предоставляются  скидки   согласно  действующему  Положению  о порядке применения скидок</t>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">Плата  за  пересылку  почтового  денежного  перевода  с  выплатой  в  ОПС,  %  от </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>суммы перевода, но не менее 1,00 руб.**</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>**При  пересылке  почтового  денежного  перевода  суммой  свыше  150,00  руб.  предоставляются  скидки согласно действующему Положению о порядке применения скидок</t>
     </r>
   </si>
   <si>
@@ -1267,28 +1232,10 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Плата  за  пересылку  и  выплату  почтового  денежного  перевода,  принятого  от учреждений   уголовно   исполнительной   системы   (исправительные   колонии, исправительные  колонии-поселения,  воспитательные  колонии,  следственные изоляторы,    тюрьмы    и    лечебно-трудовые    профилактории)    Министерства внутренних    дел    Республики    Беларусь    (выплаты     по    исполнительным документам),  %  от  суммы  перевода,  но  не  менее  минимальной  денежной единицы</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Размер ячейки M</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Плата  за  пересылку  и  выплату  (доставку)  почтового  денежного  перевода  с суммами страхового обеспечения (возмещения), % от суммы перевода, но не</t>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Плата  за  пересылку,  доставку  и  выплату  почтового  денежного  перевода  с пенсиями   и   другими   социальными   выплатами   (выплатами   на   погребение, единовременной материальной помощью), % от суммы перевода, но не менее</t>
     </r>
     <r>
       <t xml:space="preserve">
@@ -1300,7 +1247,34 @@
         <color rgb="000000" tint="0"/>
         <sz val="11"/>
       </rPr>
-      <t>менее минимальной денежной единицы</t>
+      <t>минимальной денежной единицы</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Размер ячейки M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">Плата  за  пересылку,  доставку  и  выплату  почтового  денежного  перевода  с вознаграждением     за     проведение     социальных     мероприятий     (перепись населения,  обследование  домашних  хозяйств),  %  от  суммы  перевода,   но  не </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>менее 0,20 руб.</t>
     </r>
   </si>
   <si>
@@ -1318,25 +1292,16 @@
         <rFont val="Arial"/>
         <sz val="11"/>
       </rPr>
-      <t>Плата   за  пересылку  и  выплату  почтового  денежного  перевода  в  объекте почтовой   связи   в   рамках   многостороннего   сотрудничества   с   Белорусским Красным    Крестом    и    Представительством    Детского    фонда    Организации Объединенных  Наций  в  Республике  Беларусь  (ЮНИСЕФ  в  Беларуси),  %  от суммы денежного перевода, но не менее минимальной денежной единицы</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t xml:space="preserve">Письменное  сообщение  в  электронном  денежном  переводе  оплачивается  за </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>каждое слово при пересылке электронным сообщением</t>
+      <t>Плата  за  пересылку  почтового  денежного  перевода  с  выплатой  за  сданную сельскохозяйственную  продукцию,  %  от  суммы  перевода,  но  не  менее  0,20 руб. ***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>***   При   пересылке    почтового   денежного   перевода  с   выплатами  за   сданную   сельскохозяйственную продукцию  суммой  свыше  20,00  рублей  предоставляются  скидки   согласно  действующему  Положению  о порядке применения скидок</t>
     </r>
   </si>
   <si>
@@ -1352,19 +1317,18 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Плата  за  пересылку  и  выплату  почтового  денежного  перевода,  принятого  от учреждений   уголовно   исполнительной   системы   (исправительные   колонии, исправительные  колонии-поселения,  воспитательные  колонии,  следственные изоляторы,    тюрьмы    и    лечебно-трудовые    профилактории)    Министерства внутренних    дел    Республики    Беларусь    (выплаты     по    исполнительным документам),  %  от  суммы  перевода,  но  не  менее  минимальной  денежной единицы</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
         <b val="true"/>
         <sz val="11"/>
       </rPr>
-      <t>Примечание:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b val="true"/>
-        <sz val="11"/>
-      </rPr>
       <t>Пересылка посылки "По пути" по Республике Беларусь, за 1 отправление</t>
     </r>
   </si>
@@ -1375,91 +1339,7 @@
         <color rgb="000000" tint="0"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve">Почтовые  денежные  переводы,  принятые  от  юридических  лиц,  но  с  оплатой  их  пересылки  за  счет физических   лиц   (переводы   с   алиментами,   по   исполнительным   листам),   считаются   переводами, отправляемыми   физическими   лицами.   Оплата   их   производится   по   тарифам,   установленным   для </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>физических лиц, без взимания налога на добавленную стоимость</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t xml:space="preserve">   - с документами (конверт)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b val="true"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Пересылка почтового денежного перевода наложенного платежа</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t xml:space="preserve">   - с товарным вложением</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t xml:space="preserve">За пересылку почтового денежного  перевода наложенного платежа плата взимается  объектом  почтовой связи,   осуществляющим   выдачу   почтового   отправления,   в   соответствии   с   тарифами   на   пересылку </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>почтового денежного перевода</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b val="true"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Пересылка посылки "По пути" в пределах филиала (одной области)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>утверждается филиалом самостоятельно</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="000000" tint="0"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Плата  за  пересылку  почтового  денежного  перевода  наложенного  платежа  с оплатой отправителем платы за пересылку внутренней ускоренной почты, % от</t>
+      <t>Плата  за  пересылку  и  выплату  (доставку)  почтового  денежного  перевода  с суммами страхового обеспечения (возмещения), % от суммы перевода, но не</t>
     </r>
     <r>
       <t xml:space="preserve">
@@ -1471,6 +1351,177 @@
         <color rgb="000000" tint="0"/>
         <sz val="11"/>
       </rPr>
+      <t>менее минимальной денежной единицы</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">   - с документами (конверт)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Плата   за  пересылку  и  выплату  почтового  денежного  перевода  в  объекте почтовой   связи   в   рамках   многостороннего   сотрудничества   с   Белорусским Красным    Крестом    и    Представительством    Детского    фонда    Организации Объединенных  Наций  в  Республике  Беларусь  (ЮНИСЕФ  в  Беларуси),  %  от суммы денежного перевода, но не менее минимальной денежной единицы</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">   - с товарным вложением</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">Письменное  сообщение  в  электронном  денежном  переводе  оплачивается  за </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>каждое слово при пересылке электронным сообщением</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="true"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Пересылка посылки "По пути" в пределах филиала (одной области)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>утверждается филиалом самостоятельно</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="true"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Примечание:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>За возвращение посылки "По пути" с отправителя дополнительно взимается плата за пересылку посылки "По пути" согласно действующим тарифам</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">Почтовые  денежные  переводы,  принятые  от  юридических  лиц,  но  с  оплатой  их  пересылки  за  счет физических   лиц   (переводы   с   алиментами,   по   исполнительным   листам),   считаются   переводами, отправляемыми   физическими   лицами.   Оплата   их   производится   по   тарифам,   установленным   для </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>физических лиц, без взимания налога на добавленную стоимость</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="false"/>
+        <sz val="11"/>
+      </rPr>
+      <t>По заявке получателя доставка посылки "По пути" может осуществляться на дом по тарифам на услугу "Почтовый курьер"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="true"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Пересылка почтового денежного перевода наложенного платежа</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">За пересылку почтового денежного  перевода наложенного платежа плата взимается  объектом  почтовой связи,   осуществляющим   выдачу   почтового   отправления,   в   соответствии   с   тарифами   на   пересылку </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>почтового денежного перевода</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Плата  за  пересылку  почтового  денежного  перевода  с  выплатой  в ОПС, % от суммы перевода, но не менее 1,00 руб.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Плата  за  пересылку  почтового  денежного  перевода  наложенного  платежа  с оплатой отправителем платы за пересылку внутренней ускоренной почты, % от</t>
+    </r>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
       <t>суммы перевода, но не менее 1,00 руб.****</t>
     </r>
   </si>
@@ -1480,7 +1531,7 @@
         <rFont val="Arial"/>
         <sz val="11"/>
       </rPr>
-      <t>За возвращение посылки "По пути" с отправителя дополнительно взимается плата за пересылку посылки "По пути" согласно действующим тарифам</t>
+      <t>*При  пересылке  почтового  денежного  перевода  суммой  свыше  150,00  рублей  предоставляются скидки согласно действующему Положению о порядке применения скидок</t>
     </r>
   </si>
   <si>
@@ -1505,10 +1556,9 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <b val="false"/>
-        <sz val="11"/>
-      </rPr>
-      <t>По заявке получателя доставка посылки "По пути" может осуществляться на дом по тарифам на услугу "Почтовый курьер"</t>
+        <sz val="11"/>
+      </rPr>
+      <t>При  приеме  почтового  денежного  перевода   с  использованием  БПК нерезидентов Республики Беларусь взимается дополнительная плата в размере, % от суммы перевода</t>
     </r>
   </si>
   <si>
@@ -1527,6 +1577,15 @@
         <rFont val="Arial"/>
         <sz val="11"/>
       </rPr>
+      <t>Письменное     сообщение     в     электронном     денежном     переводе оплачивается    за    каждое    слово    при    пересылке    электронным сообщением</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
       <t>простого</t>
     </r>
   </si>
@@ -1536,15 +1595,6 @@
         <rFont val="Arial"/>
         <sz val="11"/>
       </rPr>
-      <t>Плата  за  пересылку  почтового  денежного  перевода  с  выплатой  в ОПС, % от суммы перевода, но не менее 1,00 руб.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
       <t>заказного</t>
     </r>
   </si>
@@ -1554,7 +1604,7 @@
         <rFont val="Arial"/>
         <sz val="11"/>
       </rPr>
-      <t>*При  пересылке  почтового  денежного  перевода  суммой  свыше  150,00  рублей  предоставляются скидки согласно действующему Положению о порядке применения скидок</t>
+      <t>За  пересылку  почтового  денежного  перевода  наложенного  платежа  плата  взимается  объектом почтовой  связи,  осуществляющим  выдачу  почтового  отправления,  в  соответствии  с  тарифами  на пересылку почтового денежного перевода</t>
     </r>
   </si>
   <si>
@@ -1570,15 +1620,6 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>При  приеме  почтового  денежного  перевода   с  использованием  БПК нерезидентов Республики Беларусь взимается дополнительная плата в размере, % от суммы перевода</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
         <b val="true"/>
         <sz val="11"/>
       </rPr>
@@ -1589,15 +1630,6 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Письменное     сообщение     в     электронном     денежном     переводе оплачивается    за    каждое    слово    при    пересылке    электронным сообщением</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
         <color rgb="000000" tint="0"/>
         <sz val="11"/>
       </rPr>
@@ -1627,15 +1659,6 @@
         <rFont val="Arial"/>
         <sz val="11"/>
       </rPr>
-      <t>За  пересылку  почтового  денежного  перевода  наложенного  платежа  плата  взимается  объектом почтовой  связи,  осуществляющим  выдачу  почтового  отправления,  в  соответствии  с  тарифами  на пересылку почтового денежного перевода</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
       <t>Тарифы применяются при наличии договора с юридическим лицом (индивидуальным предпринимателем)</t>
     </r>
   </si>
@@ -1643,6 +1666,15 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Тарифы  на  услуги,  оказываемые  физическим  лицам  (кроме  индивидуальных  предпринимателей), установлены   с   налогом   на   добавленную   стоимость   в   соответствии   с    законодательством Республики  Беларусь,  за  исключением  услуг  по  пересылке  посылок  и (или)  почтовых  денежных переводов, принятых от физических лиц (п.1.22 ст.118 НК РБ)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
         <color rgb="000000" tint="0"/>
         <sz val="11"/>
       </rPr>
@@ -1655,15 +1687,6 @@
         <sz val="11"/>
       </rPr>
       <t>Республики Беларусь</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11"/>
-      </rPr>
-      <t>Тарифы  на  услуги,  оказываемые  физическим  лицам  (кроме  индивидуальных  предпринимателей), установлены   с   налогом   на   добавленную   стоимость   в   соответствии   с    законодательством Республики  Беларусь,  за  исключением  услуг  по  пересылке  посылок  и (или)  почтовых  денежных переводов, принятых от физических лиц (п.1.22 ст.118 НК РБ)</t>
     </r>
   </si>
 </sst>
@@ -1672,21 +1695,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a15="http://schemas.microsoft.com/office/drawing/2012/main" xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:co="http://ncloudtech.com" xmlns:co-ooxml="http://ncloudtech.com/ooxml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:x="urn:schemas-microsoft-com:office:excel" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" mc:Ignorable="co co-ooxml w14 x14 w15">
   <numFmts>
-    <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1000"/>
-    <numFmt co:extendedFormatCode="0.00;-0.00" formatCode="0.00;-0.00" numFmtId="1001"/>
-    <numFmt co:extendedFormatCode="0" formatCode="0" numFmtId="1002"/>
-    <numFmt co:extendedFormatCode="0.00" formatCode="0.00" numFmtId="1003"/>
     <numFmt co:extendedFormatCode="0.0%" formatCode="0.0%" numFmtId="1004"/>
     <numFmt co:extendedFormatCode="0.000" formatCode="0.000" numFmtId="1005"/>
+    <numFmt co:extendedFormatCode="0.00" formatCode="0.00" numFmtId="1003"/>
+    <numFmt co:extendedFormatCode="0.0000" formatCode="0.0000" numFmtId="1007"/>
+    <numFmt co:extendedFormatCode="0.00;-0.00" formatCode="0.00;-0.00" numFmtId="1001"/>
     <numFmt co:extendedFormatCode="@" formatCode="@" numFmtId="1006"/>
-    <numFmt co:extendedFormatCode="0.0000" formatCode="0.0000" numFmtId="1007"/>
+    <numFmt co:extendedFormatCode="0" formatCode="0" numFmtId="1002"/>
+    <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1000"/>
+    <numFmt co:extendedFormatCode="0.00%" formatCode="0.00%" numFmtId="1009"/>
     <numFmt co:extendedFormatCode="0.00000;-0.00000" formatCode="0.00000;-0.00000" numFmtId="1008"/>
-    <numFmt co:extendedFormatCode="0.00%" formatCode="0.00%" numFmtId="1009"/>
+    <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1010"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <name val="Calibri"/>
-      <color rgb="000000" tint="0"/>
       <sz val="11"/>
     </font>
     <font>
@@ -1726,8 +1749,20 @@
       <sz val="11"/>
     </font>
     <font>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <b val="false"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="000000" tint="0"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -1744,7 +1779,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="68">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -1786,22 +1821,470 @@
       </bottom>
     </border>
     <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="000000" tint="0"/>
       </left>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
         <color rgb="000000" tint="0"/>
       </left>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="000000" tint="0"/>
+      </left>
       <right style="thin">
         <color rgb="000000" tint="0"/>
       </right>
@@ -1818,6 +2301,126 @@
         <color rgb="000000" tint="0"/>
       </top>
       <bottom style="none"/>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
     </border>
     <border>
       <left style="thin">
@@ -1851,307 +2454,462 @@
       </diagonal>
     </border>
     <border>
-      <right style="none">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="none">
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
         <color rgb="000000" tint="0"/>
       </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false">
+  <cellXfs count="137">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="2" quotePrefix="false"/>
-    <xf applyAlignment="true" applyFont="true" borderId="0" fillId="0" fontId="2" quotePrefix="false">
+    <xf applyBorder="false" applyFill="false" applyFont="true" borderId="0" fillId="0" fontId="2" quotePrefix="false"/>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" borderId="0" fillId="0" fontId="2" quotePrefix="false">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="center" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="false" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="center" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="bottom" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="2" fontId="5" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" indent="2" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="3" numFmtId="1001" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="3" numFmtId="1001" quotePrefix="false">
       <alignment horizontal="center" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" indent="13" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" indent="2" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="center" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="right" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="center" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1005" quotePrefix="false">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="7" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="11" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="12" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="13" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1006" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="14" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="15" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1006" quotePrefix="false">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1003" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1007" quotePrefix="false">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="16" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1008" quotePrefix="false">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="17" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="18" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1006" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="19" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="7" numFmtId="1003" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="20" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="21" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="22" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" indent="1" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="23" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="24" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="25" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="26" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="27" fillId="0" fontId="6" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="28" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" borderId="29" fillId="0" fontId="8" quotePrefix="false">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1001" quotePrefix="false">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1001" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" borderId="29" fillId="0" fontId="9" quotePrefix="false">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1009" quotePrefix="false">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1010" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="32" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="33" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="34" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="35" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="36" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
+      <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="37" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="38" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="39" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="40" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="41" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="42" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
+      <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="43" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="44" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="45" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="46" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="48" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="49" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="50" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1009" quotePrefix="false">
+      <alignment horizontal="right" indent="5" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
+      <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="51" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1009" quotePrefix="false">
+      <alignment horizontal="right" indent="5" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1001" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1001" quotePrefix="false">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1005" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1005" quotePrefix="false">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="52" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="justify" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="10" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="53" fillId="0" fontId="10" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="54" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="55" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="56" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="57" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="58" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="59" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="justify" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1006" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="60" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="61" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1006" quotePrefix="false">
-      <alignment horizontal="center" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1003" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="62" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1007" quotePrefix="false">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1008" quotePrefix="false">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1006" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="63" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="64" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="61" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="bottom" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="65" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="66" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="7" numFmtId="1003" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" indent="1" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="6" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1001" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
-      <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="67" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="justify" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1001" quotePrefix="false">
-      <alignment horizontal="center" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1009" quotePrefix="false">
-      <alignment horizontal="center" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
-      <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1009" quotePrefix="false">
-      <alignment horizontal="right" indent="5" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="7" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
-      <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="center" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1009" quotePrefix="false">
-      <alignment horizontal="right" indent="5" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1005" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1001" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1001" quotePrefix="false">
-      <alignment horizontal="center" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="8" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="8" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="6" numFmtId="1002" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="0" quotePrefix="false"/>
+    <xf applyBorder="false" applyFill="false" applyFont="true" borderId="0" fillId="0" fontId="11" quotePrefix="false"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2569,7 +3327,7 @@
       <c r="H10" s="23" t="n">
         <v>2.7</v>
       </c>
-      <c r="I10" s="25" t="n">
+      <c r="I10" s="24" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">H10*1.2</f>
         <v>3.24</v>
       </c>
@@ -2591,7 +3349,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="17" t="n"/>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="25" t="s">
         <v>17</v>
       </c>
       <c r="H11" s="23" t="n">
@@ -2693,24 +3451,24 @@
       </c>
     </row>
     <row customHeight="true" ht="43.25" outlineLevel="0" r="16">
-      <c r="A16" s="27" t="n">
+      <c r="A16" s="26" t="n">
         <v>7</v>
       </c>
-      <c r="B16" s="28" t="n"/>
-      <c r="C16" s="26" t="s">
+      <c r="B16" s="27" t="n"/>
+      <c r="C16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="29" t="n">
+      <c r="D16" s="28" t="n">
         <v>0.07</v>
       </c>
-      <c r="E16" s="27" t="n">
+      <c r="E16" s="26" t="n">
         <v>7</v>
       </c>
-      <c r="F16" s="26" t="n"/>
+      <c r="F16" s="25" t="n"/>
       <c r="G16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="29" t="n">
+      <c r="H16" s="28" t="n">
         <v>0.06</v>
       </c>
       <c r="I16" s="24" t="n"/>
@@ -2719,11 +3477,11 @@
       <c r="A17" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="B17" s="28" t="n"/>
+      <c r="B17" s="27" t="n"/>
       <c r="C17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="30" t="n">
+      <c r="D17" s="29" t="n">
         <v>0.036</v>
       </c>
       <c r="E17" s="22" t="n">
@@ -2733,48 +3491,48 @@
       <c r="G17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="30" t="n">
+      <c r="H17" s="29" t="n">
         <v>0.03</v>
       </c>
-      <c r="I17" s="31" t="n"/>
+      <c r="I17" s="30" t="n"/>
     </row>
     <row customHeight="true" ht="36.3837280273438" outlineLevel="0" r="18">
-      <c r="A18" s="27" t="n">
+      <c r="A18" s="26" t="n">
         <v>9</v>
       </c>
-      <c r="B18" s="28" t="n"/>
-      <c r="C18" s="32" t="s">
+      <c r="B18" s="27" t="n"/>
+      <c r="C18" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="33" t="s"/>
-      <c r="E18" s="27" t="n">
+      <c r="D18" s="32" t="s"/>
+      <c r="E18" s="26" t="n">
         <v>9</v>
       </c>
-      <c r="F18" s="26" t="n"/>
+      <c r="F18" s="25" t="n"/>
       <c r="G18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="34" t="s"/>
+      <c r="H18" s="33" t="s"/>
       <c r="I18" s="24" t="n"/>
-      <c r="J18" s="35" t="n"/>
+      <c r="J18" s="34" t="n"/>
     </row>
     <row customHeight="true" ht="49.1162414550781" outlineLevel="0" r="19">
-      <c r="A19" s="27" t="n">
+      <c r="A19" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="B19" s="28" t="n"/>
+      <c r="B19" s="27" t="n"/>
       <c r="C19" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="34" t="s"/>
-      <c r="E19" s="27" t="n">
+      <c r="D19" s="35" t="s"/>
+      <c r="E19" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="F19" s="28" t="n"/>
+      <c r="F19" s="27" t="n"/>
       <c r="G19" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="34" t="s"/>
+      <c r="H19" s="36" t="s"/>
       <c r="I19" s="24" t="n"/>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="20">
@@ -2785,7 +3543,7 @@
       <c r="C20" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="36" t="s"/>
+      <c r="D20" s="37" t="s"/>
       <c r="E20" s="20" t="n"/>
       <c r="F20" s="21" t="n">
         <v>4</v>
@@ -2793,7 +3551,7 @@
       <c r="G20" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="36" t="s"/>
+      <c r="H20" s="38" t="s"/>
       <c r="I20" s="24" t="n"/>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="21">
@@ -2843,40 +3601,40 @@
       <c r="I22" s="24" t="n"/>
     </row>
     <row customHeight="true" ht="36.75" outlineLevel="0" r="23">
-      <c r="A23" s="27" t="n">
+      <c r="A23" s="26" t="n">
         <v>13</v>
       </c>
-      <c r="B23" s="28" t="n"/>
+      <c r="B23" s="27" t="n"/>
       <c r="C23" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="34" t="s"/>
-      <c r="E23" s="27" t="n">
+      <c r="D23" s="39" t="s"/>
+      <c r="E23" s="26" t="n">
         <v>13</v>
       </c>
-      <c r="F23" s="28" t="n"/>
+      <c r="F23" s="27" t="n"/>
       <c r="G23" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="34" t="s"/>
+      <c r="H23" s="40" t="s"/>
     </row>
     <row customHeight="true" ht="38" outlineLevel="0" r="24">
-      <c r="A24" s="27" t="n">
+      <c r="A24" s="26" t="n">
         <v>14</v>
       </c>
-      <c r="B24" s="28" t="n"/>
+      <c r="B24" s="27" t="n"/>
       <c r="C24" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="34" t="s"/>
-      <c r="E24" s="27" t="n">
+      <c r="D24" s="41" t="s"/>
+      <c r="E24" s="26" t="n">
         <v>14</v>
       </c>
-      <c r="F24" s="26" t="n"/>
+      <c r="F24" s="25" t="n"/>
       <c r="G24" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H24" s="34" t="s"/>
+      <c r="H24" s="42" t="s"/>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="25">
       <c r="A25" s="17" t="n"/>
@@ -2886,7 +3644,7 @@
       <c r="C25" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="36" t="s"/>
+      <c r="D25" s="43" t="s"/>
       <c r="E25" s="20" t="n"/>
       <c r="F25" s="21" t="n">
         <v>5</v>
@@ -2898,23 +3656,23 @@
       <c r="K25" s="24" t="n"/>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="26">
-      <c r="A26" s="37" t="n">
+      <c r="A26" s="44" t="n">
         <v>15</v>
       </c>
       <c r="B26" s="17" t="n"/>
       <c r="C26" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="34" t="s"/>
+      <c r="D26" s="45" t="s"/>
       <c r="E26" s="20" t="n"/>
       <c r="F26" s="17" t="n"/>
       <c r="G26" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H26" s="34" t="s"/>
+      <c r="H26" s="46" t="s"/>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="27">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="47" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="17" t="n"/>
@@ -2931,22 +3689,22 @@
       <c r="G27" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H27" s="39" t="n">
+      <c r="H27" s="48" t="n">
         <v>4.5</v>
       </c>
-      <c r="I27" s="40" t="n"/>
-      <c r="J27" s="40" t="n"/>
-      <c r="K27" s="40" t="n"/>
+      <c r="I27" s="49" t="n"/>
+      <c r="J27" s="49" t="n"/>
+      <c r="K27" s="49" t="n"/>
     </row>
     <row customHeight="true" ht="28.75" outlineLevel="0" r="28">
-      <c r="A28" s="37" t="n">
+      <c r="A28" s="44" t="n">
         <v>16</v>
       </c>
-      <c r="B28" s="28" t="n"/>
+      <c r="B28" s="27" t="n"/>
       <c r="C28" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="34" t="s"/>
+      <c r="D28" s="50" t="s"/>
       <c r="E28" s="22" t="n">
         <v>16</v>
       </c>
@@ -2954,101 +3712,101 @@
       <c r="G28" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H28" s="39" t="n">
+      <c r="H28" s="48" t="n">
         <v>0.85</v>
       </c>
       <c r="I28" s="24" t="n"/>
-      <c r="J28" s="35" t="n"/>
-      <c r="K28" s="41" t="n"/>
-      <c r="L28" s="35" t="n"/>
-      <c r="M28" s="35" t="n"/>
-      <c r="N28" s="35" t="n"/>
-      <c r="O28" s="35" t="n"/>
+      <c r="J28" s="34" t="n"/>
+      <c r="K28" s="51" t="n"/>
+      <c r="L28" s="34" t="n"/>
+      <c r="M28" s="34" t="n"/>
+      <c r="N28" s="34" t="n"/>
+      <c r="O28" s="34" t="n"/>
     </row>
     <row customHeight="true" ht="45.4999389648438" outlineLevel="0" r="29">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="47" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="17" t="n"/>
       <c r="C29" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="39" t="n">
+      <c r="D29" s="48" t="n">
         <v>4</v>
       </c>
       <c r="E29" s="22" t="n">
         <v>17</v>
       </c>
-      <c r="F29" s="28" t="n"/>
-      <c r="G29" s="26" t="s">
+      <c r="F29" s="27" t="n"/>
+      <c r="G29" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="H29" s="42" t="s"/>
+      <c r="H29" s="52" t="s"/>
       <c r="I29" s="24" t="n"/>
-      <c r="J29" s="35" t="n"/>
-      <c r="K29" s="40" t="n"/>
-      <c r="L29" s="35" t="n"/>
-      <c r="M29" s="35" t="n"/>
-      <c r="N29" s="35" t="n"/>
+      <c r="J29" s="34" t="n"/>
+      <c r="K29" s="49" t="n"/>
+      <c r="L29" s="34" t="n"/>
+      <c r="M29" s="34" t="n"/>
+      <c r="N29" s="34" t="n"/>
     </row>
     <row customHeight="true" hidden="false" ht="45" outlineLevel="0" r="30">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="47" t="s">
         <v>46</v>
       </c>
       <c r="B30" s="17" t="n"/>
       <c r="C30" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="39" t="n">
+      <c r="D30" s="48" t="n">
         <v>0.85</v>
       </c>
-      <c r="E30" s="27" t="n">
+      <c r="E30" s="26" t="n">
         <v>18</v>
       </c>
-      <c r="F30" s="28" t="n"/>
+      <c r="F30" s="27" t="n"/>
       <c r="G30" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H30" s="34" t="s"/>
+      <c r="H30" s="53" t="s"/>
       <c r="I30" s="24" t="n"/>
     </row>
     <row customHeight="true" ht="38.75" outlineLevel="0" r="31">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="26" t="n"/>
+      <c r="B31" s="25" t="n"/>
       <c r="C31" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="34" t="s"/>
+      <c r="D31" s="55" t="s"/>
       <c r="E31" s="22" t="n">
         <v>19</v>
       </c>
-      <c r="F31" s="28" t="n"/>
-      <c r="G31" s="26" t="s">
+      <c r="F31" s="27" t="n"/>
+      <c r="G31" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="H31" s="44" t="n">
+      <c r="H31" s="56" t="n">
         <v>0.85</v>
       </c>
     </row>
     <row customHeight="true" ht="36.4999389648438" outlineLevel="0" r="32">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="28" t="n"/>
-      <c r="C32" s="26" t="s">
+      <c r="B32" s="27" t="n"/>
+      <c r="C32" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="42" t="s"/>
-      <c r="E32" s="27" t="n">
+      <c r="D32" s="57" t="s"/>
+      <c r="E32" s="26" t="n">
         <v>20</v>
       </c>
-      <c r="F32" s="28" t="n"/>
+      <c r="F32" s="27" t="n"/>
       <c r="G32" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H32" s="45" t="n">
+      <c r="H32" s="58" t="n">
         <v>0.05</v>
       </c>
     </row>
@@ -3068,29 +3826,29 @@
       <c r="E33" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="F33" s="28" t="n"/>
-      <c r="G33" s="26" t="s">
+      <c r="F33" s="27" t="n"/>
+      <c r="G33" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="H33" s="42" t="s"/>
+      <c r="H33" s="59" t="s"/>
     </row>
     <row outlineLevel="0" r="34">
-      <c r="A34" s="27" t="n">
+      <c r="A34" s="26" t="n">
         <v>19</v>
       </c>
-      <c r="B34" s="28" t="n"/>
-      <c r="C34" s="26" t="s">
+      <c r="B34" s="27" t="n"/>
+      <c r="C34" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="42" t="s"/>
-      <c r="E34" s="27" t="n">
+      <c r="D34" s="60" t="s"/>
+      <c r="E34" s="26" t="n">
         <v>22</v>
       </c>
-      <c r="F34" s="28" t="n"/>
-      <c r="G34" s="46" t="s">
+      <c r="F34" s="27" t="n"/>
+      <c r="G34" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="H34" s="47" t="s">
+      <c r="H34" s="62" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3098,31 +3856,31 @@
       <c r="A35" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="B35" s="28" t="n"/>
+      <c r="B35" s="27" t="n"/>
       <c r="C35" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="30" t="n">
+      <c r="D35" s="29" t="n">
         <v>0.03</v>
       </c>
-      <c r="E35" s="27" t="n">
+      <c r="E35" s="26" t="n">
         <v>23</v>
       </c>
-      <c r="F35" s="28" t="n"/>
-      <c r="G35" s="26" t="s">
+      <c r="F35" s="27" t="n"/>
+      <c r="G35" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="H35" s="42" t="s"/>
+      <c r="H35" s="63" t="s"/>
     </row>
     <row outlineLevel="0" r="36">
       <c r="A36" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="B36" s="28" t="n"/>
-      <c r="C36" s="26" t="s">
+      <c r="B36" s="27" t="n"/>
+      <c r="C36" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D36" s="42" t="s"/>
+      <c r="D36" s="64" t="s"/>
       <c r="E36" s="22" t="n">
         <v>24</v>
       </c>
@@ -3130,7 +3888,7 @@
       <c r="G36" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="30" t="n">
+      <c r="H36" s="29" t="n">
         <v>0.03</v>
       </c>
     </row>
@@ -3138,29 +3896,29 @@
       <c r="A37" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="B37" s="28" t="n"/>
-      <c r="C37" s="26" t="s">
+      <c r="B37" s="27" t="n"/>
+      <c r="C37" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="42" t="s"/>
+      <c r="D37" s="65" t="s"/>
       <c r="E37" s="22" t="n">
         <v>25</v>
       </c>
-      <c r="F37" s="28" t="n"/>
-      <c r="G37" s="26" t="s">
+      <c r="F37" s="27" t="n"/>
+      <c r="G37" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H37" s="42" t="s"/>
+      <c r="H37" s="66" t="s"/>
     </row>
     <row outlineLevel="0" r="38">
-      <c r="A38" s="28" t="n"/>
+      <c r="A38" s="27" t="n"/>
       <c r="B38" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="C38" s="48" t="s">
+      <c r="C38" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="49" t="s"/>
+      <c r="D38" s="68" t="s"/>
       <c r="E38" s="16" t="s">
         <v>6</v>
       </c>
@@ -3170,7 +3928,7 @@
       <c r="G38" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H38" s="13" t="s">
+      <c r="H38" s="16" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3178,43 +3936,47 @@
       <c r="A39" s="22" t="n">
         <v>23</v>
       </c>
-      <c r="B39" s="28" t="n"/>
+      <c r="B39" s="27" t="n"/>
       <c r="C39" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="34" t="s"/>
+      <c r="D39" s="69" t="s"/>
       <c r="E39" s="22" t="n"/>
-      <c r="F39" s="21" t="n">
+      <c r="F39" s="70" t="n">
         <v>6</v>
       </c>
-      <c r="G39" s="50" t="s">
+      <c r="G39" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="H39" s="51" t="s"/>
+      <c r="H39" s="71" t="n"/>
     </row>
     <row outlineLevel="0" r="40">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="28" t="n"/>
+      <c r="B40" s="27" t="n"/>
       <c r="C40" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="52" t="n">
+      <c r="D40" s="72" t="n">
         <v>3</v>
       </c>
       <c r="E40" s="20" t="n"/>
-      <c r="F40" s="17" t="n"/>
-      <c r="G40" s="50" t="s">
+      <c r="F40" s="73" t="n">
+        <v>26</v>
+      </c>
+      <c r="G40" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H40" s="51" t="s"/>
+      <c r="H40" s="71" t="n">
+        <v>4.5</v>
+      </c>
     </row>
     <row outlineLevel="0" r="41">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="28" t="n"/>
+      <c r="B41" s="27" t="n"/>
       <c r="C41" s="13" t="s">
         <v>68</v>
       </c>
@@ -3224,19 +3986,21 @@
       <c r="E41" s="22" t="n">
         <v>26</v>
       </c>
-      <c r="F41" s="17" t="n"/>
-      <c r="G41" s="13" t="s">
+      <c r="F41" s="73" t="n">
+        <v>27</v>
+      </c>
+      <c r="G41" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H41" s="23" t="n">
-        <v>2.5</v>
+      <c r="H41" s="74" t="n">
+        <v>0.01</v>
       </c>
     </row>
     <row outlineLevel="0" r="42">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="28" t="n"/>
+      <c r="B42" s="27" t="n"/>
       <c r="C42" s="13" t="s">
         <v>71</v>
       </c>
@@ -3246,57 +4010,57 @@
       <c r="E42" s="22" t="n">
         <v>27</v>
       </c>
-      <c r="F42" s="17" t="n"/>
-      <c r="G42" s="13" t="s">
+      <c r="F42" s="73" t="n">
+        <v>28</v>
+      </c>
+      <c r="G42" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="H42" s="23" t="n">
-        <v>3.3</v>
-      </c>
+      <c r="H42" s="1" t="n"/>
     </row>
     <row outlineLevel="0" r="43">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="28" t="n"/>
-      <c r="C43" s="26" t="s">
+      <c r="B43" s="27" t="n"/>
+      <c r="C43" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="D43" s="42" t="s"/>
+      <c r="D43" s="76" t="s"/>
       <c r="E43" s="22" t="n">
         <v>28</v>
       </c>
-      <c r="F43" s="17" t="n"/>
-      <c r="G43" s="13" t="s">
+      <c r="F43" s="21" t="n">
+        <v>7</v>
+      </c>
+      <c r="G43" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="H43" s="23" t="n">
-        <v>4.1</v>
-      </c>
+      <c r="H43" s="1" t="n"/>
     </row>
     <row outlineLevel="0" r="44">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="B44" s="28" t="n"/>
+      <c r="B44" s="27" t="n"/>
       <c r="C44" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D44" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="E44" s="53" t="n"/>
+      <c r="E44" s="77" t="n"/>
       <c r="F44" s="17" t="n"/>
-      <c r="G44" s="19" t="s">
+      <c r="G44" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="H44" s="36" t="s"/>
+      <c r="H44" s="79" t="s"/>
     </row>
     <row outlineLevel="0" r="45">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="28" t="n"/>
+      <c r="B45" s="27" t="n"/>
       <c r="C45" s="13" t="s">
         <v>43</v>
       </c>
@@ -3306,225 +4070,237 @@
       <c r="E45" s="22" t="n">
         <v>29</v>
       </c>
-      <c r="F45" s="17" t="n"/>
+      <c r="F45" s="20" t="n">
+        <v>29</v>
+      </c>
       <c r="G45" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="H45" s="54" t="n">
-        <v>4.5</v>
+      <c r="H45" s="23" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row outlineLevel="0" r="46">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="26" t="n"/>
-      <c r="C46" s="55" t="s">
+      <c r="B46" s="25" t="n"/>
+      <c r="C46" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="56" t="s"/>
+      <c r="D46" s="81" t="s"/>
       <c r="E46" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="F46" s="17" t="n"/>
+      <c r="F46" s="20" t="n">
+        <v>30</v>
+      </c>
       <c r="G46" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="H46" s="54" t="n">
-        <v>5.65</v>
+      <c r="H46" s="23" t="n">
+        <v>3.3</v>
       </c>
     </row>
     <row outlineLevel="0" r="47">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="26" t="n"/>
-      <c r="C47" s="55" t="s">
+      <c r="B47" s="25" t="n"/>
+      <c r="C47" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="D47" s="56" t="s"/>
+      <c r="D47" s="82" t="s"/>
       <c r="E47" s="22" t="n">
         <v>31</v>
       </c>
-      <c r="F47" s="17" t="n"/>
+      <c r="F47" s="20" t="n">
+        <v>31</v>
+      </c>
       <c r="G47" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="H47" s="54" t="n">
-        <v>8.1</v>
+      <c r="H47" s="23" t="n">
+        <v>4.1</v>
       </c>
     </row>
     <row outlineLevel="0" r="48">
-      <c r="A48" s="43" t="s">
+      <c r="A48" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="26" t="n"/>
-      <c r="C48" s="55" t="s">
+      <c r="B48" s="25" t="n"/>
+      <c r="C48" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="D48" s="56" t="s"/>
+      <c r="D48" s="83" t="s"/>
       <c r="E48" s="22" t="n"/>
-      <c r="F48" s="28" t="n"/>
-      <c r="G48" s="26" t="s">
+      <c r="F48" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="H48" s="42" t="s"/>
+      <c r="G48" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H48" s="84" t="s"/>
     </row>
     <row outlineLevel="0" r="49">
       <c r="A49" s="22" t="n">
         <v>28</v>
       </c>
-      <c r="B49" s="28" t="n"/>
-      <c r="C49" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D49" s="30" t="n">
+      <c r="B49" s="27" t="n"/>
+      <c r="C49" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="29" t="n">
         <v>0.01</v>
       </c>
       <c r="E49" s="22" t="n">
         <v>32</v>
       </c>
-      <c r="F49" s="28" t="n"/>
+      <c r="F49" s="20" t="n">
+        <v>32</v>
+      </c>
       <c r="G49" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H49" s="34" t="s"/>
+        <v>91</v>
+      </c>
+      <c r="H49" s="85" t="n">
+        <v>4.5</v>
+      </c>
     </row>
     <row outlineLevel="0" r="50">
       <c r="A50" s="22" t="n">
         <v>29</v>
       </c>
-      <c r="B50" s="28" t="n"/>
-      <c r="C50" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="D50" s="42" t="s"/>
+      <c r="B50" s="27" t="n"/>
+      <c r="C50" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50" s="86" t="s"/>
       <c r="E50" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="F50" s="28" t="n"/>
-      <c r="G50" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="H50" s="42" t="s"/>
+      <c r="F50" s="20" t="n">
+        <v>33</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H50" s="85" t="n">
+        <v>5.65</v>
+      </c>
     </row>
     <row outlineLevel="0" r="51">
       <c r="A51" s="22" t="n"/>
-      <c r="B51" s="28" t="n">
+      <c r="B51" s="27" t="n">
         <v>7</v>
       </c>
-      <c r="C51" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="D51" s="57" t="n"/>
+      <c r="C51" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="71" t="n"/>
       <c r="E51" s="22" t="n">
         <v>34</v>
       </c>
-      <c r="F51" s="28" t="n"/>
-      <c r="G51" s="26" t="s">
+      <c r="F51" s="20" t="n">
+        <v>34</v>
+      </c>
+      <c r="G51" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H51" s="42" t="s"/>
+      <c r="H51" s="85" t="n">
+        <v>8.1</v>
+      </c>
     </row>
     <row outlineLevel="0" r="52">
       <c r="A52" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="B52" s="28" t="n"/>
-      <c r="C52" s="26" t="s">
+      <c r="B52" s="27" t="n"/>
+      <c r="C52" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="71" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E52" s="77" t="n"/>
+      <c r="F52" s="27" t="n"/>
+      <c r="G52" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="D52" s="57" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E52" s="53" t="n"/>
-      <c r="F52" s="21" t="n">
-        <v>7</v>
-      </c>
-      <c r="G52" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="H52" s="36" t="s"/>
+      <c r="H52" s="87" t="s"/>
     </row>
     <row outlineLevel="0" r="53">
       <c r="A53" s="22" t="n">
         <v>31</v>
       </c>
-      <c r="B53" s="28" t="n"/>
-      <c r="C53" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="D53" s="58" t="n">
+      <c r="B53" s="27" t="n"/>
+      <c r="C53" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" s="74" t="n">
         <v>0.01</v>
       </c>
       <c r="E53" s="22" t="n">
         <v>35</v>
       </c>
-      <c r="F53" s="17" t="n"/>
+      <c r="F53" s="27" t="n"/>
       <c r="G53" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="H53" s="54" t="n">
-        <v>4.5</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="H53" s="1" t="n"/>
     </row>
     <row outlineLevel="0" r="54">
       <c r="A54" s="22" t="n">
         <v>32</v>
       </c>
-      <c r="B54" s="28" t="n"/>
-      <c r="C54" s="59" t="s">
-        <v>99</v>
-      </c>
-      <c r="D54" s="60" t="s"/>
+      <c r="B54" s="27" t="n"/>
+      <c r="C54" s="88" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" s="89" t="s"/>
       <c r="E54" s="22" t="n">
         <v>36</v>
       </c>
-      <c r="F54" s="17" t="n"/>
-      <c r="G54" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="H54" s="54" t="n">
-        <v>5.65</v>
-      </c>
+      <c r="F54" s="27" t="n"/>
+      <c r="G54" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="H54" s="1" t="n"/>
     </row>
     <row outlineLevel="0" r="55">
-      <c r="A55" s="28" t="n"/>
+      <c r="A55" s="27" t="n"/>
       <c r="B55" s="18" t="n">
         <v>8</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D55" s="36" t="s"/>
+        <v>75</v>
+      </c>
+      <c r="D55" s="90" t="s"/>
       <c r="E55" s="22" t="n">
         <v>37</v>
       </c>
-      <c r="F55" s="17" t="n"/>
-      <c r="G55" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="H55" s="54" t="n">
-        <v>8.1</v>
-      </c>
+      <c r="F55" s="27" t="n"/>
+      <c r="G55" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H55" s="1" t="n"/>
     </row>
     <row outlineLevel="0" r="56">
       <c r="A56" s="17" t="n"/>
       <c r="B56" s="17" t="n"/>
       <c r="C56" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D56" s="36" t="s"/>
+        <v>77</v>
+      </c>
+      <c r="D56" s="91" t="s"/>
       <c r="E56" s="22" t="n">
         <v>38</v>
       </c>
-      <c r="F56" s="28" t="n"/>
-      <c r="G56" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H56" s="61" t="n">
-        <v>0.03</v>
-      </c>
+      <c r="F56" s="21" t="n">
+        <v>7</v>
+      </c>
+      <c r="G56" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="H56" s="1" t="n"/>
     </row>
     <row outlineLevel="0" r="57">
       <c r="A57" s="22" t="n">
@@ -3532,7 +4308,7 @@
       </c>
       <c r="B57" s="17" t="n"/>
       <c r="C57" s="13" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D57" s="23" t="n">
         <v>3</v>
@@ -3540,11 +4316,13 @@
       <c r="E57" s="22" t="n">
         <v>39</v>
       </c>
-      <c r="F57" s="28" t="n"/>
-      <c r="G57" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="H57" s="42" t="s"/>
+      <c r="F57" s="17" t="n"/>
+      <c r="G57" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="H57" s="85" t="n">
+        <v>4.5</v>
+      </c>
     </row>
     <row outlineLevel="0" r="58">
       <c r="A58" s="22" t="n">
@@ -3552,19 +4330,19 @@
       </c>
       <c r="B58" s="17" t="n"/>
       <c r="C58" s="13" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D58" s="23" t="n">
         <v>3.96</v>
       </c>
-      <c r="E58" s="53" t="n"/>
-      <c r="F58" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="G58" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H58" s="36" t="s"/>
+      <c r="E58" s="77" t="n"/>
+      <c r="F58" s="17" t="n"/>
+      <c r="G58" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H58" s="85" t="n">
+        <v>5.65</v>
+      </c>
     </row>
     <row outlineLevel="0" r="59">
       <c r="A59" s="22" t="n">
@@ -3572,7 +4350,7 @@
       </c>
       <c r="B59" s="17" t="n"/>
       <c r="C59" s="13" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D59" s="23" t="n">
         <v>4.92</v>
@@ -3582,28 +4360,28 @@
       </c>
       <c r="F59" s="17" t="n"/>
       <c r="G59" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="H59" s="54" t="n">
-        <v>15</v>
+        <v>103</v>
+      </c>
+      <c r="H59" s="85" t="n">
+        <v>8.1</v>
       </c>
     </row>
     <row outlineLevel="0" r="60">
       <c r="A60" s="17" t="n"/>
       <c r="B60" s="17" t="n"/>
       <c r="C60" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D60" s="36" t="s"/>
+        <v>89</v>
+      </c>
+      <c r="D60" s="92" t="s"/>
       <c r="E60" s="22" t="n">
         <v>41</v>
       </c>
-      <c r="F60" s="17" t="n"/>
+      <c r="F60" s="27" t="n"/>
       <c r="G60" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="H60" s="54" t="n">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="H60" s="93" t="n">
+        <v>0.03</v>
       </c>
     </row>
     <row outlineLevel="0" r="61">
@@ -3612,7 +4390,7 @@
       </c>
       <c r="B61" s="17" t="n"/>
       <c r="C61" s="13" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="D61" s="23" t="n">
         <v>5.4</v>
@@ -3620,13 +4398,11 @@
       <c r="E61" s="22" t="n">
         <v>42</v>
       </c>
-      <c r="F61" s="17" t="n"/>
-      <c r="G61" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="H61" s="54" t="n">
-        <v>42.5</v>
-      </c>
+      <c r="F61" s="27" t="n"/>
+      <c r="G61" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="H61" s="1" t="n"/>
     </row>
     <row outlineLevel="0" r="62">
       <c r="A62" s="22" t="n">
@@ -3634,19 +4410,19 @@
       </c>
       <c r="B62" s="17" t="n"/>
       <c r="C62" s="13" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="D62" s="23" t="n">
         <v>6.78</v>
       </c>
       <c r="E62" s="20" t="n"/>
       <c r="F62" s="21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="H62" s="17" t="n"/>
+        <v>105</v>
+      </c>
+      <c r="H62" s="94" t="s"/>
     </row>
     <row outlineLevel="0" r="63">
       <c r="A63" s="22" t="n">
@@ -3654,7 +4430,7 @@
       </c>
       <c r="B63" s="17" t="n"/>
       <c r="C63" s="13" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D63" s="23" t="n">
         <v>9.72</v>
@@ -3662,86 +4438,88 @@
       <c r="E63" s="22" t="n">
         <v>43</v>
       </c>
-      <c r="F63" s="28" t="n"/>
-      <c r="G63" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="H63" s="61" t="n">
-        <v>0.03</v>
+      <c r="F63" s="17" t="n"/>
+      <c r="G63" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="H63" s="85" t="n">
+        <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="64">
-      <c r="A64" s="28" t="n"/>
-      <c r="B64" s="28" t="n"/>
+      <c r="A64" s="27" t="n"/>
+      <c r="B64" s="27" t="n"/>
       <c r="C64" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D64" s="34" t="s"/>
-      <c r="E64" s="53" t="n"/>
-      <c r="F64" s="28" t="n"/>
-      <c r="G64" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="H64" s="56" t="s"/>
+      <c r="D64" s="95" t="s"/>
+      <c r="E64" s="77" t="n"/>
+      <c r="F64" s="17" t="n"/>
+      <c r="G64" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H64" s="85" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row outlineLevel="0" r="65">
-      <c r="A65" s="27" t="n">
+      <c r="A65" s="26" t="n">
         <v>39</v>
       </c>
-      <c r="B65" s="28" t="n"/>
-      <c r="C65" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="D65" s="62" t="s"/>
+      <c r="B65" s="27" t="n"/>
+      <c r="C65" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="D65" s="96" t="s"/>
       <c r="E65" s="22" t="n">
         <v>44</v>
       </c>
-      <c r="F65" s="26" t="n"/>
-      <c r="G65" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="H65" s="63" t="n">
-        <v>0.0233</v>
+      <c r="F65" s="17" t="n"/>
+      <c r="G65" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="H65" s="85" t="n">
+        <v>42.5</v>
       </c>
     </row>
     <row outlineLevel="0" r="66">
       <c r="A66" s="22" t="n">
         <v>40</v>
       </c>
-      <c r="B66" s="28" t="n"/>
+      <c r="B66" s="27" t="n"/>
       <c r="C66" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D66" s="34" t="s"/>
+        <v>107</v>
+      </c>
+      <c r="D66" s="97" t="s"/>
       <c r="E66" s="22" t="n">
         <v>45</v>
       </c>
-      <c r="F66" s="26" t="n"/>
-      <c r="G66" s="32" t="s">
+      <c r="F66" s="21" t="n">
+        <v>9</v>
+      </c>
+      <c r="G66" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="H66" s="17" t="n"/>
+    </row>
+    <row outlineLevel="0" r="67">
+      <c r="A67" s="98" t="n">
+        <v>41</v>
+      </c>
+      <c r="B67" s="99" t="n"/>
+      <c r="C67" s="100" t="s">
+        <v>109</v>
+      </c>
+      <c r="D67" s="101" t="s"/>
+      <c r="E67" s="26" t="n">
+        <v>46</v>
+      </c>
+      <c r="F67" s="27" t="n"/>
+      <c r="G67" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="H66" s="63" t="n">
-        <v>0.0233</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="67">
-      <c r="A67" s="64" t="n">
-        <v>41</v>
-      </c>
-      <c r="B67" s="65" t="n"/>
-      <c r="C67" s="66" t="s">
-        <v>111</v>
-      </c>
-      <c r="D67" s="67" t="s"/>
-      <c r="E67" s="27" t="n">
-        <v>46</v>
-      </c>
-      <c r="F67" s="26" t="n"/>
-      <c r="G67" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="H67" s="68" t="n">
-        <v>0.015</v>
+      <c r="H67" s="93" t="n">
+        <v>0.03</v>
       </c>
     </row>
     <row outlineLevel="0" r="68">
@@ -3750,15 +4528,15 @@
         <v>9</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="D68" s="36" t="s"/>
-      <c r="E68" s="69" t="n"/>
-      <c r="F68" s="26" t="n"/>
-      <c r="G68" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="H68" s="34" t="s"/>
+        <v>100</v>
+      </c>
+      <c r="D68" s="102" t="s"/>
+      <c r="E68" s="103" t="n"/>
+      <c r="F68" s="27" t="n"/>
+      <c r="G68" s="80" t="s">
+        <v>111</v>
+      </c>
+      <c r="H68" s="104" t="s"/>
     </row>
     <row outlineLevel="0" r="69">
       <c r="A69" s="22" t="n">
@@ -3766,19 +4544,19 @@
       </c>
       <c r="B69" s="17" t="n"/>
       <c r="C69" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D69" s="23" t="n">
         <v>5.4</v>
       </c>
-      <c r="E69" s="27" t="n">
+      <c r="E69" s="26" t="n">
         <v>47</v>
       </c>
-      <c r="F69" s="26" t="n"/>
-      <c r="G69" s="55" t="s">
-        <v>115</v>
-      </c>
-      <c r="H69" s="70" t="n">
+      <c r="F69" s="25" t="n"/>
+      <c r="G69" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="H69" s="105" t="n">
         <v>0.0233</v>
       </c>
     </row>
@@ -3788,20 +4566,20 @@
       </c>
       <c r="B70" s="17" t="n"/>
       <c r="C70" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D70" s="23" t="n">
         <v>6.78</v>
       </c>
-      <c r="E70" s="27" t="n">
+      <c r="E70" s="26" t="n">
         <v>48</v>
       </c>
-      <c r="F70" s="28" t="n"/>
-      <c r="G70" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="H70" s="45" t="n">
-        <v>0.015</v>
+      <c r="F70" s="25" t="n"/>
+      <c r="G70" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="H70" s="105" t="n">
+        <v>0.0233</v>
       </c>
     </row>
     <row outlineLevel="0" r="71">
@@ -3810,20 +4588,20 @@
       </c>
       <c r="B71" s="17" t="n"/>
       <c r="C71" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D71" s="23" t="n">
         <v>9.72</v>
       </c>
-      <c r="E71" s="27" t="n">
+      <c r="E71" s="26" t="n">
         <v>49</v>
       </c>
-      <c r="F71" s="26" t="n"/>
-      <c r="G71" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="H71" s="45" t="n">
-        <v>0.005</v>
+      <c r="F71" s="25" t="n"/>
+      <c r="G71" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H71" s="106" t="n">
+        <v>0.015</v>
       </c>
     </row>
     <row outlineLevel="0" r="72">
@@ -3834,37 +4612,35 @@
       <c r="C72" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D72" s="30" t="n">
+      <c r="D72" s="29" t="n">
         <v>0.03</v>
       </c>
       <c r="E72" s="22" t="n">
         <v>50</v>
       </c>
-      <c r="F72" s="28" t="n"/>
-      <c r="G72" s="26" t="s">
+      <c r="F72" s="25" t="n"/>
+      <c r="G72" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H72" s="1" t="n"/>
+    </row>
+    <row outlineLevel="0" r="73">
+      <c r="A73" s="26" t="n">
+        <v>46</v>
+      </c>
+      <c r="B73" s="27" t="n"/>
+      <c r="C73" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D73" s="107" t="s"/>
+      <c r="E73" s="20" t="n"/>
+      <c r="F73" s="25" t="n"/>
+      <c r="G73" s="80" t="s">
         <v>120</v>
       </c>
-      <c r="H72" s="71" t="n">
-        <v>0.009</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="73">
-      <c r="A73" s="27" t="n">
-        <v>46</v>
-      </c>
-      <c r="B73" s="28" t="n"/>
-      <c r="C73" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D73" s="34" t="s"/>
-      <c r="E73" s="20" t="n"/>
-      <c r="F73" s="21" t="n">
-        <v>10</v>
-      </c>
-      <c r="G73" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H73" s="17" t="n"/>
+      <c r="H73" s="108" t="n">
+        <v>0.0233</v>
+      </c>
     </row>
     <row outlineLevel="0" r="74">
       <c r="A74" s="17" t="n"/>
@@ -3872,115 +4648,119 @@
         <v>10</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D74" s="17" t="n"/>
       <c r="E74" s="22" t="n">
         <v>51</v>
       </c>
-      <c r="F74" s="26" t="n"/>
-      <c r="G74" s="32" t="s">
+      <c r="F74" s="27" t="n"/>
+      <c r="G74" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H74" s="58" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="75">
+      <c r="A75" s="26" t="n">
+        <v>47</v>
+      </c>
+      <c r="B75" s="27" t="n"/>
+      <c r="C75" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D75" s="109" t="n">
+        <v>4</v>
+      </c>
+      <c r="E75" s="20" t="n"/>
+      <c r="F75" s="25" t="n"/>
+      <c r="G75" s="80" t="s">
         <v>124</v>
       </c>
-      <c r="H74" s="33" t="s"/>
-    </row>
-    <row outlineLevel="0" r="75">
-      <c r="A75" s="27" t="n">
-        <v>47</v>
-      </c>
-      <c r="B75" s="28" t="n"/>
-      <c r="C75" s="13" t="s">
+      <c r="H75" s="58" t="n">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="76">
+      <c r="A76" s="26" t="n">
+        <v>48</v>
+      </c>
+      <c r="B76" s="25" t="n"/>
+      <c r="C76" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D75" s="72" t="n">
-        <v>4</v>
-      </c>
-      <c r="E75" s="20" t="n"/>
-      <c r="F75" s="21" t="n">
+      <c r="D76" s="110" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="E76" s="26" t="n">
+        <v>52</v>
+      </c>
+      <c r="F76" s="27" t="n"/>
+      <c r="G76" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="H76" s="111" t="n">
+        <v>0.009</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="77">
+      <c r="A77" s="26" t="n"/>
+      <c r="B77" s="67" t="n">
         <v>11</v>
       </c>
-      <c r="G75" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="H75" s="17" t="n"/>
-    </row>
-    <row outlineLevel="0" r="76">
-      <c r="A76" s="27" t="n">
-        <v>48</v>
-      </c>
-      <c r="B76" s="26" t="n"/>
-      <c r="C76" s="13" t="s">
+      <c r="C77" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="D76" s="73" t="n">
-        <v>6.6</v>
-      </c>
-      <c r="E76" s="27" t="n">
-        <v>52</v>
-      </c>
-      <c r="F76" s="28" t="n"/>
-      <c r="G76" s="32" t="s">
+      <c r="D77" s="112" t="s">
         <v>128</v>
       </c>
-      <c r="H76" s="33" t="s"/>
-    </row>
-    <row outlineLevel="0" r="77">
-      <c r="A77" s="27" t="n"/>
-      <c r="B77" s="48" t="n">
-        <v>11</v>
-      </c>
-      <c r="C77" s="19" t="s">
+      <c r="E77" s="26" t="n">
+        <v>53</v>
+      </c>
+      <c r="F77" s="21" t="n">
+        <v>10</v>
+      </c>
+      <c r="G77" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="D77" s="74" t="s">
+      <c r="H77" s="17" t="n"/>
+    </row>
+    <row outlineLevel="0" r="78">
+      <c r="A78" s="26" t="n">
+        <v>49</v>
+      </c>
+      <c r="B78" s="25" t="n"/>
+      <c r="C78" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E77" s="27" t="n">
-        <v>53</v>
-      </c>
-      <c r="F77" s="28" t="n"/>
-      <c r="G77" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="H77" s="45" t="n">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="78">
-      <c r="A78" s="27" t="n">
-        <v>49</v>
-      </c>
-      <c r="B78" s="26" t="n"/>
-      <c r="C78" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D78" s="29" t="n"/>
+      <c r="D78" s="28" t="n"/>
       <c r="E78" s="22" t="n">
         <v>54</v>
       </c>
-      <c r="F78" s="28" t="n"/>
-      <c r="G78" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="H78" s="42" t="s"/>
+      <c r="F78" s="25" t="n"/>
+      <c r="G78" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="H78" s="113" t="s"/>
     </row>
     <row outlineLevel="0" r="79">
       <c r="A79" s="20" t="n">
         <v>50</v>
       </c>
       <c r="B79" s="21" t="n"/>
-      <c r="C79" s="75" t="s">
-        <v>134</v>
-      </c>
-      <c r="D79" s="76" t="s"/>
+      <c r="C79" s="114" t="s">
+        <v>132</v>
+      </c>
+      <c r="D79" s="115" t="s"/>
       <c r="E79" s="20" t="n"/>
       <c r="F79" s="21" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G79" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="H79" s="36" t="s"/>
+        <v>133</v>
+      </c>
+      <c r="H79" s="17" t="n"/>
     </row>
     <row outlineLevel="0" r="80">
       <c r="A80" s="17" t="n"/>
@@ -3988,105 +4768,103 @@
         <v>12</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D80" s="17" t="n"/>
       <c r="E80" s="22" t="n">
         <v>55</v>
       </c>
-      <c r="F80" s="17" t="n"/>
-      <c r="G80" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="H80" s="23" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="I80" s="35" t="n"/>
+      <c r="F80" s="27" t="n"/>
+      <c r="G80" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="H80" s="1" t="n"/>
+      <c r="I80" s="34" t="n"/>
     </row>
     <row outlineLevel="0" r="81">
-      <c r="A81" s="27" t="n">
+      <c r="A81" s="26" t="n">
         <v>51</v>
       </c>
-      <c r="B81" s="28" t="n"/>
+      <c r="B81" s="27" t="n"/>
       <c r="C81" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="D81" s="45" t="n">
+        <v>135</v>
+      </c>
+      <c r="D81" s="58" t="n">
         <v>0.03</v>
       </c>
       <c r="E81" s="22" t="n">
         <v>56</v>
       </c>
-      <c r="F81" s="17" t="n"/>
-      <c r="G81" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="H81" s="23" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="I81" s="35" t="n"/>
+      <c r="F81" s="27" t="n"/>
+      <c r="G81" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="H81" s="58" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I81" s="34" t="n"/>
     </row>
     <row outlineLevel="0" r="82">
-      <c r="A82" s="27" t="n">
+      <c r="A82" s="26" t="n">
         <v>52</v>
       </c>
-      <c r="B82" s="26" t="n"/>
-      <c r="C82" s="77" t="s">
-        <v>139</v>
-      </c>
-      <c r="D82" s="78" t="s"/>
+      <c r="B82" s="25" t="n"/>
+      <c r="C82" s="116" t="s">
+        <v>137</v>
+      </c>
+      <c r="D82" s="117" t="s"/>
       <c r="E82" s="22" t="n">
         <v>57</v>
       </c>
-      <c r="F82" s="17" t="n"/>
-      <c r="G82" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="H82" s="23" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="I82" s="35" t="n"/>
+      <c r="F82" s="27" t="n"/>
+      <c r="G82" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="H82" s="1" t="n"/>
+      <c r="I82" s="34" t="n"/>
     </row>
     <row outlineLevel="0" r="83">
-      <c r="A83" s="27" t="n">
+      <c r="A83" s="26" t="n">
         <v>53</v>
       </c>
-      <c r="B83" s="26" t="n"/>
+      <c r="B83" s="25" t="n"/>
       <c r="C83" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="D83" s="45" t="n">
+        <v>139</v>
+      </c>
+      <c r="D83" s="58" t="n">
         <v>0.015</v>
       </c>
       <c r="E83" s="20" t="n"/>
       <c r="F83" s="21" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G83" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="H83" s="36" t="s"/>
+        <v>140</v>
+      </c>
+      <c r="H83" s="118" t="s"/>
       <c r="I83" s="1" t="n"/>
     </row>
     <row outlineLevel="0" r="84">
-      <c r="A84" s="27" t="n">
+      <c r="A84" s="26" t="n">
         <v>54</v>
       </c>
-      <c r="B84" s="26" t="n"/>
+      <c r="B84" s="25" t="n"/>
       <c r="C84" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="D84" s="29" t="n">
+        <v>141</v>
+      </c>
+      <c r="D84" s="28" t="n">
         <v>0.01</v>
       </c>
       <c r="E84" s="22" t="n">
         <v>58</v>
       </c>
-      <c r="F84" s="28" t="n"/>
-      <c r="G84" s="79" t="s">
-        <v>144</v>
-      </c>
-      <c r="H84" s="80" t="s"/>
+      <c r="F84" s="17" t="n"/>
+      <c r="G84" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H84" s="23" t="n">
+        <v>0.7</v>
+      </c>
       <c r="I84" s="24" t="n"/>
     </row>
     <row outlineLevel="0" r="85">
@@ -4095,36 +4873,40 @@
         <v>13</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D85" s="36" t="s"/>
+        <v>133</v>
+      </c>
+      <c r="D85" s="119" t="s"/>
       <c r="E85" s="22" t="n">
         <v>59</v>
       </c>
       <c r="F85" s="17" t="n"/>
-      <c r="G85" s="81" t="s">
-        <v>145</v>
-      </c>
-      <c r="H85" s="82" t="s"/>
+      <c r="G85" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="H85" s="23" t="n">
+        <v>2.2</v>
+      </c>
       <c r="I85" s="24" t="n"/>
     </row>
     <row outlineLevel="0" r="86">
-      <c r="A86" s="27" t="n">
+      <c r="A86" s="26" t="n">
         <v>55</v>
       </c>
-      <c r="B86" s="26" t="n"/>
+      <c r="B86" s="25" t="n"/>
       <c r="C86" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="D86" s="34" t="s"/>
+        <v>144</v>
+      </c>
+      <c r="D86" s="120" t="s"/>
       <c r="E86" s="22" t="n">
         <v>60</v>
       </c>
-      <c r="F86" s="28" t="n"/>
-      <c r="G86" s="81" t="s">
-        <v>147</v>
-      </c>
-      <c r="H86" s="82" t="s"/>
+      <c r="F86" s="17" t="n"/>
+      <c r="G86" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="H86" s="23" t="n">
+        <v>0.45</v>
+      </c>
       <c r="I86" s="24" t="n"/>
     </row>
     <row outlineLevel="0" r="87">
@@ -4133,17 +4915,17 @@
         <v>14</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D87" s="36" t="s"/>
+        <v>140</v>
+      </c>
+      <c r="D87" s="121" t="s"/>
       <c r="E87" s="20" t="n"/>
       <c r="F87" s="21" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G87" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H87" s="36" t="s"/>
+        <v>146</v>
+      </c>
+      <c r="H87" s="122" t="s"/>
     </row>
     <row outlineLevel="0" r="88">
       <c r="A88" s="22" t="n">
@@ -4151,19 +4933,19 @@
       </c>
       <c r="B88" s="17" t="n"/>
       <c r="C88" s="13" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D88" s="23" t="n">
         <v>0.84</v>
       </c>
-      <c r="E88" s="27" t="n">
+      <c r="E88" s="26" t="n">
         <v>61</v>
       </c>
-      <c r="F88" s="28" t="n"/>
-      <c r="G88" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="H88" s="33" t="s"/>
+      <c r="F88" s="27" t="n"/>
+      <c r="G88" s="123" t="s">
+        <v>147</v>
+      </c>
+      <c r="H88" s="124" t="s"/>
     </row>
     <row outlineLevel="0" r="89">
       <c r="A89" s="22" t="n">
@@ -4171,15 +4953,17 @@
       </c>
       <c r="B89" s="17" t="n"/>
       <c r="C89" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="D89" s="83" t="n">
+        <v>143</v>
+      </c>
+      <c r="D89" s="125" t="n">
         <v>2.64</v>
       </c>
-      <c r="E89" s="84" t="n"/>
-      <c r="F89" s="85" t="n"/>
-      <c r="G89" s="86" t="n"/>
-      <c r="H89" s="87" t="s"/>
+      <c r="E89" s="126" t="n"/>
+      <c r="F89" s="17" t="n"/>
+      <c r="G89" s="127" t="s">
+        <v>148</v>
+      </c>
+      <c r="H89" s="128" t="s"/>
     </row>
     <row outlineLevel="0" r="90">
       <c r="A90" s="22" t="n">
@@ -4187,15 +4971,17 @@
       </c>
       <c r="B90" s="17" t="n"/>
       <c r="C90" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D90" s="83" t="n">
+        <v>145</v>
+      </c>
+      <c r="D90" s="125" t="n">
         <v>0.54</v>
       </c>
-      <c r="E90" s="88" t="n"/>
-      <c r="F90" s="7" t="n"/>
-      <c r="G90" s="89" t="n"/>
-      <c r="H90" s="89" t="s"/>
+      <c r="E90" s="129" t="n"/>
+      <c r="F90" s="27" t="n"/>
+      <c r="G90" s="127" t="s">
+        <v>149</v>
+      </c>
+      <c r="H90" s="130" t="s"/>
     </row>
     <row outlineLevel="0" r="91">
       <c r="A91" s="17" t="n"/>
@@ -4203,69 +4989,77 @@
         <v>13</v>
       </c>
       <c r="C91" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="D91" s="90" t="n"/>
+        <v>129</v>
+      </c>
+      <c r="D91" s="131" t="n"/>
       <c r="E91" s="5" t="n"/>
-      <c r="F91" s="91" t="n"/>
-      <c r="G91" s="92" t="n"/>
-      <c r="H91" s="92" t="s"/>
+      <c r="F91" s="21" t="n">
+        <v>12</v>
+      </c>
+      <c r="G91" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="H91" s="132" t="s"/>
     </row>
     <row outlineLevel="0" r="92">
       <c r="A92" s="22" t="n">
         <v>59</v>
       </c>
-      <c r="B92" s="26" t="n"/>
+      <c r="B92" s="25" t="n"/>
       <c r="C92" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="D92" s="34" t="s"/>
-      <c r="E92" s="93" t="n"/>
-      <c r="F92" s="7" t="n"/>
-      <c r="G92" s="94" t="n"/>
-      <c r="H92" s="94" t="s"/>
+        <v>150</v>
+      </c>
+      <c r="D92" s="133" t="s"/>
+      <c r="E92" s="134" t="n"/>
+      <c r="F92" s="27" t="n"/>
+      <c r="G92" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="H92" s="135" t="s"/>
     </row>
     <row outlineLevel="0" r="93">
       <c r="C93" s="1" t="n"/>
       <c r="D93" s="1" t="n"/>
+      <c r="F93" s="1" t="n"/>
+      <c r="G93" s="1" t="n"/>
     </row>
     <row outlineLevel="0" r="94">
       <c r="C94" s="1" t="n"/>
       <c r="D94" s="1" t="n"/>
       <c r="E94" s="0" t="n"/>
-      <c r="F94" s="95" t="n"/>
-      <c r="G94" s="95" t="n"/>
+      <c r="F94" s="136" t="n"/>
+      <c r="G94" s="136" t="n"/>
       <c r="I94" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="95">
       <c r="C95" s="1" t="n"/>
       <c r="D95" s="1" t="n"/>
       <c r="E95" s="0" t="n"/>
-      <c r="F95" s="95" t="n"/>
-      <c r="G95" s="95" t="n"/>
-      <c r="H95" s="95" t="n"/>
+      <c r="F95" s="136" t="n"/>
+      <c r="G95" s="136" t="n"/>
+      <c r="H95" s="136" t="n"/>
       <c r="I95" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="96">
       <c r="C96" s="1" t="n"/>
       <c r="D96" s="1" t="n"/>
       <c r="E96" s="0" t="n"/>
-      <c r="F96" s="95" t="n"/>
-      <c r="G96" s="95" t="n"/>
-      <c r="H96" s="95" t="n"/>
+      <c r="F96" s="136" t="n"/>
+      <c r="G96" s="136" t="n"/>
+      <c r="H96" s="136" t="n"/>
       <c r="I96" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="97">
       <c r="C97" s="1" t="n"/>
       <c r="D97" s="1" t="n"/>
       <c r="E97" s="0" t="n"/>
-      <c r="F97" s="95" t="n"/>
-      <c r="G97" s="95" t="n"/>
-      <c r="H97" s="95" t="n"/>
+      <c r="F97" s="136" t="n"/>
+      <c r="G97" s="136" t="n"/>
+      <c r="H97" s="136" t="n"/>
       <c r="I97" s="0" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="75">
+  <mergeCells count="72">
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:D18"/>
@@ -4294,22 +5088,14 @@
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="G35:H35"/>
     <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G92:H92"/>
-    <mergeCell ref="G91:H91"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="G83:H83"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C85:D85"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C47:D47"/>
@@ -4323,24 +5109,29 @@
     <mergeCell ref="C65:D65"/>
     <mergeCell ref="C66:D66"/>
     <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G92:H92"/>
+    <mergeCell ref="G91:H91"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="G83:H83"/>
+    <mergeCell ref="G82:H82"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="G72:H72"/>
     <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="G53:H53"/>
     <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G49:H49"/>
     <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G42:H42"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.300000011920929" header="0.300000011920929" left="0.700000047683716" right="0.700000047683716" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
rates 01.03.2025 parcel, transfer
</commit_message>
<xml_diff>
--- a/calc/files/letter2.xlsx
+++ b/calc/files/letter2.xlsx
@@ -37,7 +37,7 @@
         <rFont val="Arial"/>
         <sz val="11"/>
       </rPr>
-      <t>от 19 декабря 2024 № 1162</t>
+      <t>от 27.02.2025 № 193</t>
     </r>
   </si>
   <si>
@@ -68,7 +68,7 @@
         <color rgb="FF0000" tint="0"/>
         <sz val="11"/>
       </rPr>
-      <t>в действии c 01.01.2025</t>
+      <t>в действии c 01.03.2025</t>
     </r>
   </si>
   <si>
@@ -919,7 +919,6 @@
       <t>За хрупкие посылки с отметкой "Хрупкое и громоздкие взимается надбавка к плате за пересылку посылки   в   размере   50%.   Если   посылка   является   одновременно   хрупкой   и   громоздкой,   то дополнительная плата взимается только один раз</t>
     </r>
   </si>
-  <si/>
   <si>
     <r>
       <rPr>
@@ -1531,7 +1530,7 @@
         <rFont val="Arial"/>
         <sz val="11"/>
       </rPr>
-      <t>*При  пересылке  почтового  денежного  перевода  суммой  свыше  150,00  рублей  предоставляются скидки согласно действующему Положению о порядке применения скидок</t>
+      <t>*При  пересылке  почтового  денежного  перевода  суммой  свыше  200,00  рублей  предоставляются скидки согласно действующему Положению о порядке применения скидок</t>
     </r>
   </si>
   <si>
@@ -1695,17 +1694,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a15="http://schemas.microsoft.com/office/drawing/2012/main" xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:co="http://ncloudtech.com" xmlns:co-ooxml="http://ncloudtech.com/ooxml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:x="urn:schemas-microsoft-com:office:excel" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" mc:Ignorable="co co-ooxml w14 x14 w15">
   <numFmts>
-    <numFmt co:extendedFormatCode="0.0%" formatCode="0.0%" numFmtId="1004"/>
-    <numFmt co:extendedFormatCode="0.000" formatCode="0.000" numFmtId="1005"/>
-    <numFmt co:extendedFormatCode="0.00" formatCode="0.00" numFmtId="1003"/>
-    <numFmt co:extendedFormatCode="0.0000" formatCode="0.0000" numFmtId="1007"/>
-    <numFmt co:extendedFormatCode="0.00;-0.00" formatCode="0.00;-0.00" numFmtId="1001"/>
-    <numFmt co:extendedFormatCode="@" formatCode="@" numFmtId="1006"/>
-    <numFmt co:extendedFormatCode="0" formatCode="0" numFmtId="1002"/>
+    <numFmt co:extendedFormatCode="0" formatCode="0" numFmtId="1004"/>
+    <numFmt co:extendedFormatCode="0.0%" formatCode="0.0%" numFmtId="1006"/>
+    <numFmt co:extendedFormatCode="0.00" formatCode="0.00" numFmtId="1005"/>
+    <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1012"/>
+    <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1002"/>
+    <numFmt co:extendedFormatCode="0.00;-0.00" formatCode="0.00;-0.00" numFmtId="1003"/>
+    <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1001"/>
     <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1000"/>
-    <numFmt co:extendedFormatCode="0.00%" formatCode="0.00%" numFmtId="1009"/>
-    <numFmt co:extendedFormatCode="0.00000;-0.00000" formatCode="0.00000;-0.00000" numFmtId="1008"/>
-    <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1010"/>
+    <numFmt co:extendedFormatCode="@" formatCode="@" numFmtId="1008"/>
+    <numFmt co:extendedFormatCode="0.0000" formatCode="0.0000" numFmtId="1009"/>
+    <numFmt co:extendedFormatCode="0.00000;-0.00000" formatCode="0.00000;-0.00000" numFmtId="1010"/>
+    <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1013"/>
+    <numFmt co:extendedFormatCode="0.000" formatCode="0.000" numFmtId="1007"/>
+    <numFmt co:extendedFormatCode="0.00%" formatCode="0.00%" numFmtId="1011"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -1749,7 +1751,9 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="true"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -1779,7 +1783,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="68">
+  <borders count="78">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -2110,17 +2114,6 @@
       </bottom>
     </border>
     <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="000000" tint="0"/>
       </left>
@@ -2145,97 +2138,143 @@
       </bottom>
     </border>
     <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
     </border>
     <border>
       <right style="thin">
@@ -2325,37 +2364,52 @@
       </bottom>
     </border>
     <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000000" tint="0"/>
+      </top>
     </border>
     <border>
       <top style="thin">
@@ -2502,7 +2556,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="150">
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2525,6 +2579,9 @@
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="2" numFmtId="1001" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
@@ -2534,12 +2591,15 @@
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="bottom" wrapText="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="2" fontId="5" numFmtId="1002" quotePrefix="false">
+      <alignment horizontal="left" indent="2" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
+      <alignment horizontal="center" vertical="bottom" wrapText="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="2" fontId="5" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" indent="2" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="3" numFmtId="1001" quotePrefix="false">
-      <alignment horizontal="center" vertical="bottom" wrapText="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
@@ -2555,7 +2615,7 @@
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1004" quotePrefix="false">
       <alignment horizontal="right" shrinkToFit="true" vertical="top"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
@@ -2564,349 +2624,382 @@
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="center" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1004" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1005" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1005" quotePrefix="false">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1005" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1006" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1007" quotePrefix="false">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="7" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="11" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="12" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="13" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1008" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="14" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="15" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1008" quotePrefix="false">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1005" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1009" quotePrefix="false">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="16" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1010" quotePrefix="false">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="17" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="18" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1008" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="19" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="7" numFmtId="1005" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="20" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1006" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="21" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="22" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" indent="1" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="23" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="24" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="25" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="26" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="27" fillId="0" fontId="6" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="28" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" borderId="29" fillId="0" fontId="8" quotePrefix="false">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1003" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" borderId="29" fillId="0" fontId="9" quotePrefix="false">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1011" quotePrefix="false">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="32" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="33" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="34" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="35" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="36" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="37" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="38" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1005" quotePrefix="false">
+      <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="39" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="40" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="41" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="42" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="43" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="44" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="45" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="46" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="48" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1006" quotePrefix="false">
+      <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="49" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="50" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="51" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="52" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="53" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="54" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="54" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="54" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="55" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="56" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="57" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1011" quotePrefix="false">
+      <alignment horizontal="right" indent="5" shrinkToFit="true" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1006" quotePrefix="false">
+      <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="58" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="59" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1011" quotePrefix="false">
+      <alignment horizontal="right" indent="5" shrinkToFit="true" vertical="center"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1003" quotePrefix="false">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1007" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1005" quotePrefix="false">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="7" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="11" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="12" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="13" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1006" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="14" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="15" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1006" quotePrefix="false">
-      <alignment horizontal="center" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1003" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1007" quotePrefix="false">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="16" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1008" quotePrefix="false">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="17" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="18" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1006" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="19" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="7" numFmtId="1003" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="20" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="21" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="22" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" indent="1" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="23" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="24" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="25" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="26" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="27" fillId="0" fontId="6" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="28" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" borderId="29" fillId="0" fontId="8" quotePrefix="false">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1001" quotePrefix="false">
-      <alignment horizontal="center" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1001" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" borderId="29" fillId="0" fontId="9" quotePrefix="false">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1009" quotePrefix="false">
-      <alignment horizontal="center" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1010" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="32" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="33" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="34" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="35" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="36" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
-      <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="37" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="38" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="39" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="40" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="41" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="42" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
-      <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="43" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="44" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="45" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="46" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="48" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="49" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="center" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="50" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1009" quotePrefix="false">
-      <alignment horizontal="right" indent="5" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
-      <alignment horizontal="right" indent="6" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="51" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1009" quotePrefix="false">
-      <alignment horizontal="right" indent="5" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1001" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1001" quotePrefix="false">
-      <alignment horizontal="center" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1005" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="52" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="10" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="53" fillId="0" fontId="10" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="54" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="55" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="56" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="57" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="58" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="59" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="justify" vertical="top" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="60" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="justify" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="61" fillId="0" fontId="3" numFmtId="1003" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="10" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="61" fillId="0" fontId="10" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="62" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="2" numFmtId="1012" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="63" fillId="0" fontId="2" numFmtId="1012" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="64" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="65" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="66" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="67" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="68" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="69" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="70" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="justify" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="71" fillId="0" fontId="3" numFmtId="1005" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="62" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="72" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="justify" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="63" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="73" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="justify" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="64" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="74" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="justify" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="61" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="71" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="65" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="66" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="75" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="2" numFmtId="1013" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="76" fillId="0" fontId="2" numFmtId="1013" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1004" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="67" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="77" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="justify" vertical="top" wrapText="true"/>
     </xf>
     <xf applyBorder="false" applyFill="false" applyFont="true" borderId="0" fillId="0" fontId="11" quotePrefix="false"/>
@@ -3183,1839 +3276,1837 @@
       <c r="E3" s="5" t="n"/>
       <c r="F3" s="3" t="n"/>
       <c r="G3" s="3" t="n"/>
-      <c r="H3" s="8" t="str">
+      <c r="H3" s="9" t="str">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D3</f>
-        <v>от 19 декабря 2024 № 1162</v>
+        <v>от 27.02.2025 № 193</v>
       </c>
     </row>
     <row customHeight="true" ht="41.25" outlineLevel="0" r="4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s"/>
-      <c r="C4" s="9" t="s"/>
-      <c r="D4" s="9" t="s"/>
-      <c r="E4" s="9" t="s">
+      <c r="B4" s="10" t="s"/>
+      <c r="C4" s="10" t="s"/>
+      <c r="D4" s="10" t="s"/>
+      <c r="E4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="9" t="s"/>
-      <c r="G4" s="9" t="s"/>
-      <c r="H4" s="9" t="s"/>
+      <c r="F4" s="10" t="s"/>
+      <c r="G4" s="10" t="s"/>
+      <c r="H4" s="10" t="s"/>
     </row>
     <row customHeight="true" ht="17" outlineLevel="0" r="5">
-      <c r="A5" s="10" t="n"/>
-      <c r="B5" s="10" t="n"/>
-      <c r="C5" s="10" t="n"/>
-      <c r="D5" s="11" t="s">
+      <c r="A5" s="11" t="n"/>
+      <c r="B5" s="11" t="n"/>
+      <c r="C5" s="11" t="n"/>
+      <c r="D5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="12" t="n"/>
-      <c r="F5" s="10" t="n"/>
-      <c r="G5" s="10" t="n"/>
-      <c r="H5" s="11" t="str">
+      <c r="E5" s="13" t="n"/>
+      <c r="F5" s="11" t="n"/>
+      <c r="G5" s="11" t="n"/>
+      <c r="H5" s="14" t="str">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D5</f>
-        <v>в действии c 01.01.2025</v>
+        <v>в действии c 01.03.2025</v>
       </c>
     </row>
     <row customHeight="true" ht="27.25" outlineLevel="0" r="6">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="7">
-      <c r="A7" s="17" t="n"/>
-      <c r="B7" s="18" t="n">
+      <c r="A7" s="19" t="n"/>
+      <c r="B7" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="17" t="n"/>
-      <c r="E7" s="20" t="n"/>
-      <c r="F7" s="21" t="n">
+      <c r="D7" s="19" t="n"/>
+      <c r="E7" s="22" t="n"/>
+      <c r="F7" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="17" t="n"/>
+      <c r="H7" s="19" t="n"/>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="8">
-      <c r="A8" s="22" t="n">
+      <c r="A8" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="17" t="n"/>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="19" t="n"/>
+      <c r="C8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="23" t="n">
+      <c r="D8" s="25" t="n">
         <v>2.94</v>
       </c>
-      <c r="E8" s="22" t="n">
+      <c r="E8" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="17" t="n"/>
-      <c r="G8" s="13" t="s">
+      <c r="F8" s="19" t="n"/>
+      <c r="G8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="23" t="n">
+      <c r="H8" s="25" t="n">
         <v>2.45</v>
       </c>
-      <c r="I8" s="24" t="n"/>
+      <c r="I8" s="26" t="n"/>
       <c r="J8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="9">
-      <c r="A9" s="17" t="n"/>
-      <c r="B9" s="18" t="n">
+      <c r="A9" s="19" t="n"/>
+      <c r="B9" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="17" t="n"/>
-      <c r="E9" s="20" t="n"/>
-      <c r="F9" s="21" t="n">
+      <c r="D9" s="19" t="n"/>
+      <c r="E9" s="22" t="n"/>
+      <c r="F9" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="17" t="n"/>
-      <c r="I9" s="24" t="n"/>
+      <c r="H9" s="19" t="n"/>
+      <c r="I9" s="26" t="n"/>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="10">
-      <c r="A10" s="22" t="n">
+      <c r="A10" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="B10" s="17" t="n"/>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="19" t="n"/>
+      <c r="C10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="23" t="n">
+      <c r="D10" s="25" t="n">
         <v>3.24</v>
       </c>
-      <c r="E10" s="22" t="n">
+      <c r="E10" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="17" t="n"/>
-      <c r="G10" s="13" t="s">
+      <c r="F10" s="19" t="n"/>
+      <c r="G10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="23" t="n">
+      <c r="H10" s="25" t="n">
         <v>2.7</v>
       </c>
-      <c r="I10" s="24" t="n">
+      <c r="I10" s="26" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">H10*1.2</f>
         <v>3.24</v>
       </c>
-      <c r="J10" s="24" t="n"/>
-      <c r="K10" s="24" t="n"/>
+      <c r="J10" s="26" t="n"/>
+      <c r="K10" s="26" t="n"/>
     </row>
     <row customHeight="true" ht="25.9999694824219" outlineLevel="0" r="11">
-      <c r="A11" s="22" t="n">
+      <c r="A11" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="B11" s="17" t="n"/>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="19" t="n"/>
+      <c r="C11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="23" t="n">
+      <c r="D11" s="25" t="n">
         <v>0.07</v>
       </c>
-      <c r="E11" s="22" t="n">
+      <c r="E11" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="F11" s="17" t="n"/>
-      <c r="G11" s="25" t="s">
+      <c r="F11" s="19" t="n"/>
+      <c r="G11" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="23" t="n">
+      <c r="H11" s="25" t="n">
         <v>0.06</v>
       </c>
-      <c r="I11" s="24" t="n"/>
-      <c r="J11" s="24" t="n"/>
-      <c r="K11" s="24" t="n"/>
+      <c r="I11" s="26" t="n"/>
+      <c r="J11" s="26" t="n"/>
+      <c r="K11" s="26" t="n"/>
     </row>
     <row customHeight="true" ht="12.75" outlineLevel="0" r="12">
-      <c r="A12" s="17" t="n"/>
-      <c r="B12" s="18" t="n">
+      <c r="A12" s="19" t="n"/>
+      <c r="B12" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="17" t="n"/>
-      <c r="E12" s="20" t="n"/>
-      <c r="F12" s="21" t="n">
+      <c r="D12" s="19" t="n"/>
+      <c r="E12" s="22" t="n"/>
+      <c r="F12" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="17" t="n"/>
-      <c r="I12" s="24" t="n"/>
+      <c r="H12" s="19" t="n"/>
+      <c r="I12" s="26" t="n"/>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="13">
-      <c r="A13" s="22" t="n">
+      <c r="A13" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="B13" s="17" t="n"/>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="19" t="n"/>
+      <c r="C13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="23" t="n">
+      <c r="D13" s="25" t="n">
         <v>0.9</v>
       </c>
-      <c r="E13" s="22" t="n">
+      <c r="E13" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="F13" s="17" t="n"/>
-      <c r="G13" s="13" t="s">
+      <c r="F13" s="19" t="n"/>
+      <c r="G13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="23" t="n">
+      <c r="H13" s="25" t="n">
         <v>0.75</v>
       </c>
-      <c r="I13" s="24" t="n"/>
+      <c r="I13" s="26" t="n"/>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="14">
-      <c r="A14" s="22" t="n">
+      <c r="A14" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="B14" s="17" t="n"/>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="19" t="n"/>
+      <c r="C14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="23" t="n">
+      <c r="D14" s="25" t="n">
         <v>3.24</v>
       </c>
-      <c r="E14" s="22" t="n">
+      <c r="E14" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="F14" s="17" t="n"/>
-      <c r="G14" s="13" t="s">
+      <c r="F14" s="19" t="n"/>
+      <c r="G14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="23" t="n">
+      <c r="H14" s="25" t="n">
         <v>2.7</v>
       </c>
-      <c r="I14" s="24" t="n"/>
+      <c r="I14" s="26" t="n"/>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="15">
-      <c r="A15" s="22" t="n">
+      <c r="A15" s="24" t="n">
         <v>6</v>
       </c>
-      <c r="B15" s="17" t="n"/>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="19" t="n"/>
+      <c r="C15" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="23" t="n">
+      <c r="D15" s="25" t="n">
         <v>3.72</v>
       </c>
-      <c r="E15" s="22" t="n">
+      <c r="E15" s="24" t="n">
         <v>6</v>
       </c>
-      <c r="F15" s="17" t="n"/>
-      <c r="G15" s="13" t="s">
+      <c r="F15" s="19" t="n"/>
+      <c r="G15" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="23" t="n">
+      <c r="H15" s="25" t="n">
         <v>3.2</v>
       </c>
-      <c r="I15" s="24" t="n">
+      <c r="I15" s="26" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">H15*1.2</f>
         <v>3.84</v>
       </c>
     </row>
     <row customHeight="true" ht="43.25" outlineLevel="0" r="16">
-      <c r="A16" s="26" t="n">
+      <c r="A16" s="28" t="n">
         <v>7</v>
       </c>
-      <c r="B16" s="27" t="n"/>
-      <c r="C16" s="25" t="s">
+      <c r="B16" s="29" t="n"/>
+      <c r="C16" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="28" t="n">
+      <c r="D16" s="30" t="n">
         <v>0.07</v>
       </c>
-      <c r="E16" s="26" t="n">
+      <c r="E16" s="28" t="n">
         <v>7</v>
       </c>
-      <c r="F16" s="25" t="n"/>
-      <c r="G16" s="13" t="s">
+      <c r="F16" s="27" t="n"/>
+      <c r="G16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="28" t="n">
+      <c r="H16" s="30" t="n">
         <v>0.06</v>
       </c>
-      <c r="I16" s="24" t="n"/>
+      <c r="I16" s="26" t="n"/>
     </row>
     <row customHeight="true" ht="22.75" outlineLevel="0" r="17">
-      <c r="A17" s="22" t="n">
+      <c r="A17" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="B17" s="27" t="n"/>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="29" t="n"/>
+      <c r="C17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="29" t="n">
+      <c r="D17" s="31" t="n">
         <v>0.036</v>
       </c>
-      <c r="E17" s="22" t="n">
+      <c r="E17" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="F17" s="17" t="n"/>
-      <c r="G17" s="13" t="s">
+      <c r="F17" s="19" t="n"/>
+      <c r="G17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="29" t="n">
+      <c r="H17" s="31" t="n">
         <v>0.03</v>
       </c>
-      <c r="I17" s="30" t="n"/>
+      <c r="I17" s="32" t="n"/>
     </row>
     <row customHeight="true" ht="36.3837280273438" outlineLevel="0" r="18">
-      <c r="A18" s="26" t="n">
+      <c r="A18" s="28" t="n">
         <v>9</v>
       </c>
-      <c r="B18" s="27" t="n"/>
-      <c r="C18" s="31" t="s">
+      <c r="B18" s="29" t="n"/>
+      <c r="C18" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="32" t="s"/>
-      <c r="E18" s="26" t="n">
+      <c r="D18" s="34" t="s"/>
+      <c r="E18" s="28" t="n">
         <v>9</v>
       </c>
-      <c r="F18" s="25" t="n"/>
-      <c r="G18" s="13" t="s">
+      <c r="F18" s="27" t="n"/>
+      <c r="G18" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="33" t="s"/>
-      <c r="I18" s="24" t="n"/>
-      <c r="J18" s="34" t="n"/>
+      <c r="H18" s="35" t="s"/>
+      <c r="I18" s="26" t="n"/>
+      <c r="J18" s="36" t="n"/>
     </row>
     <row customHeight="true" ht="49.1162414550781" outlineLevel="0" r="19">
-      <c r="A19" s="26" t="n">
+      <c r="A19" s="28" t="n">
         <v>10</v>
       </c>
-      <c r="B19" s="27" t="n"/>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="29" t="n"/>
+      <c r="C19" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="35" t="s"/>
-      <c r="E19" s="26" t="n">
+      <c r="D19" s="37" t="s"/>
+      <c r="E19" s="28" t="n">
         <v>10</v>
       </c>
-      <c r="F19" s="27" t="n"/>
-      <c r="G19" s="13" t="s">
+      <c r="F19" s="29" t="n"/>
+      <c r="G19" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="36" t="s"/>
-      <c r="I19" s="24" t="n"/>
+      <c r="H19" s="38" t="s"/>
+      <c r="I19" s="26" t="n"/>
     </row>
     <row customHeight="true" ht="13.25" outlineLevel="0" r="20">
-      <c r="A20" s="17" t="n"/>
-      <c r="B20" s="18" t="n">
+      <c r="A20" s="19" t="n"/>
+      <c r="B20" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="37" t="s"/>
-      <c r="E20" s="20" t="n"/>
-      <c r="F20" s="21" t="n">
+      <c r="D20" s="39" t="s"/>
+      <c r="E20" s="22" t="n"/>
+      <c r="F20" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="38" t="s"/>
-      <c r="I20" s="24" t="n"/>
+      <c r="H20" s="40" t="s"/>
+      <c r="I20" s="26" t="n"/>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="21">
-      <c r="A21" s="22" t="n">
+      <c r="A21" s="24" t="n">
         <v>11</v>
       </c>
-      <c r="B21" s="17" t="n"/>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="19" t="n"/>
+      <c r="C21" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="23" t="n">
+      <c r="D21" s="25" t="n">
         <v>2.04</v>
       </c>
-      <c r="E21" s="22" t="n">
+      <c r="E21" s="24" t="n">
         <v>11</v>
       </c>
-      <c r="F21" s="17" t="n"/>
-      <c r="G21" s="13" t="s">
+      <c r="F21" s="19" t="n"/>
+      <c r="G21" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="23" t="n">
+      <c r="H21" s="25" t="n">
         <v>1.7</v>
       </c>
-      <c r="I21" s="24" t="n"/>
+      <c r="I21" s="26" t="n"/>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="22">
-      <c r="A22" s="22" t="n">
+      <c r="A22" s="24" t="n">
         <v>12</v>
       </c>
-      <c r="B22" s="17" t="n"/>
-      <c r="C22" s="13" t="s">
+      <c r="B22" s="19" t="n"/>
+      <c r="C22" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="23" t="n">
+      <c r="D22" s="25" t="n">
         <v>0.42</v>
       </c>
-      <c r="E22" s="22" t="n">
+      <c r="E22" s="24" t="n">
         <v>12</v>
       </c>
-      <c r="F22" s="17" t="n"/>
-      <c r="G22" s="13" t="s">
+      <c r="F22" s="19" t="n"/>
+      <c r="G22" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="23" t="n">
+      <c r="H22" s="25" t="n">
         <v>0.35</v>
       </c>
-      <c r="I22" s="24" t="n"/>
+      <c r="I22" s="26" t="n"/>
     </row>
     <row customHeight="true" ht="36.75" outlineLevel="0" r="23">
-      <c r="A23" s="26" t="n">
+      <c r="A23" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="B23" s="27" t="n"/>
-      <c r="C23" s="13" t="s">
+      <c r="B23" s="29" t="n"/>
+      <c r="C23" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="39" t="s"/>
-      <c r="E23" s="26" t="n">
+      <c r="D23" s="41" t="s"/>
+      <c r="E23" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="F23" s="27" t="n"/>
-      <c r="G23" s="13" t="s">
+      <c r="F23" s="29" t="n"/>
+      <c r="G23" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="40" t="s"/>
+      <c r="H23" s="42" t="s"/>
     </row>
     <row customHeight="true" ht="38" outlineLevel="0" r="24">
-      <c r="A24" s="26" t="n">
+      <c r="A24" s="28" t="n">
         <v>14</v>
       </c>
-      <c r="B24" s="27" t="n"/>
-      <c r="C24" s="13" t="s">
+      <c r="B24" s="29" t="n"/>
+      <c r="C24" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="41" t="s"/>
-      <c r="E24" s="26" t="n">
+      <c r="D24" s="43" t="s"/>
+      <c r="E24" s="28" t="n">
         <v>14</v>
       </c>
-      <c r="F24" s="25" t="n"/>
-      <c r="G24" s="13" t="s">
+      <c r="F24" s="27" t="n"/>
+      <c r="G24" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H24" s="42" t="s"/>
+      <c r="H24" s="44" t="s"/>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="25">
-      <c r="A25" s="17" t="n"/>
-      <c r="B25" s="18" t="n">
+      <c r="A25" s="19" t="n"/>
+      <c r="B25" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="43" t="s"/>
-      <c r="E25" s="20" t="n"/>
-      <c r="F25" s="21" t="n">
+      <c r="D25" s="45" t="s"/>
+      <c r="E25" s="22" t="n"/>
+      <c r="F25" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="H25" s="17" t="n"/>
-      <c r="K25" s="24" t="n"/>
+      <c r="H25" s="19" t="n"/>
+      <c r="K25" s="26" t="n"/>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="26">
-      <c r="A26" s="44" t="n">
+      <c r="A26" s="46" t="n">
         <v>15</v>
       </c>
-      <c r="B26" s="17" t="n"/>
-      <c r="C26" s="13" t="s">
+      <c r="B26" s="19" t="n"/>
+      <c r="C26" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="45" t="s"/>
-      <c r="E26" s="20" t="n"/>
-      <c r="F26" s="17" t="n"/>
-      <c r="G26" s="13" t="s">
+      <c r="D26" s="47" t="s"/>
+      <c r="E26" s="22" t="n"/>
+      <c r="F26" s="19" t="n"/>
+      <c r="G26" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H26" s="46" t="s"/>
+      <c r="H26" s="48" t="s"/>
     </row>
     <row customHeight="true" ht="14" outlineLevel="0" r="27">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="17" t="n"/>
-      <c r="C27" s="13" t="s">
+      <c r="B27" s="19" t="n"/>
+      <c r="C27" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="23" t="n">
+      <c r="D27" s="50" t="n">
+        <v>4</v>
+      </c>
+      <c r="E27" s="24" t="n">
+        <v>15</v>
+      </c>
+      <c r="F27" s="19" t="n"/>
+      <c r="G27" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" s="50" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I27" s="51" t="n"/>
+      <c r="J27" s="51" t="n"/>
+      <c r="K27" s="51" t="n"/>
+    </row>
+    <row customHeight="true" ht="28.75" outlineLevel="0" r="28">
+      <c r="A28" s="46" t="n">
+        <v>16</v>
+      </c>
+      <c r="B28" s="29" t="n"/>
+      <c r="C28" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="52" t="s"/>
+      <c r="E28" s="24" t="n">
+        <v>16</v>
+      </c>
+      <c r="F28" s="19" t="n"/>
+      <c r="G28" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="50" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="I28" s="26" t="n"/>
+      <c r="J28" s="36" t="n"/>
+      <c r="K28" s="53" t="n"/>
+      <c r="L28" s="36" t="n"/>
+      <c r="M28" s="36" t="n"/>
+      <c r="N28" s="36" t="n"/>
+      <c r="O28" s="36" t="n"/>
+    </row>
+    <row customHeight="true" ht="45.4999389648438" outlineLevel="0" r="29">
+      <c r="A29" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="19" t="n"/>
+      <c r="C29" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="50" t="n">
+        <v>4</v>
+      </c>
+      <c r="E29" s="24" t="n">
+        <v>17</v>
+      </c>
+      <c r="F29" s="29" t="n"/>
+      <c r="G29" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" s="54" t="s"/>
+      <c r="I29" s="26" t="n"/>
+      <c r="J29" s="36" t="n"/>
+      <c r="K29" s="51" t="n"/>
+      <c r="L29" s="36" t="n"/>
+      <c r="M29" s="36" t="n"/>
+      <c r="N29" s="36" t="n"/>
+    </row>
+    <row customHeight="true" hidden="false" ht="45" outlineLevel="0" r="30">
+      <c r="A30" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="19" t="n"/>
+      <c r="C30" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="50" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E30" s="28" t="n">
+        <v>18</v>
+      </c>
+      <c r="F30" s="29" t="n"/>
+      <c r="G30" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H30" s="55" t="s"/>
+      <c r="I30" s="26" t="n"/>
+    </row>
+    <row customHeight="true" ht="38.75" outlineLevel="0" r="31">
+      <c r="A31" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="27" t="n"/>
+      <c r="C31" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="57" t="s"/>
+      <c r="E31" s="24" t="n">
+        <v>19</v>
+      </c>
+      <c r="F31" s="29" t="n"/>
+      <c r="G31" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="58" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row customHeight="true" ht="36.4999389648438" outlineLevel="0" r="32">
+      <c r="A32" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="29" t="n"/>
+      <c r="C32" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="59" t="s"/>
+      <c r="E32" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="F32" s="29" t="n"/>
+      <c r="G32" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H32" s="60" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row customHeight="true" ht="36.4999389648438" outlineLevel="0" r="33">
+      <c r="A33" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="24" t="n">
+        <v>21</v>
+      </c>
+      <c r="F33" s="29" t="n"/>
+      <c r="G33" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" s="61" t="s"/>
+    </row>
+    <row outlineLevel="0" r="34">
+      <c r="A34" s="28" t="n">
+        <v>19</v>
+      </c>
+      <c r="B34" s="29" t="n"/>
+      <c r="C34" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="62" t="s"/>
+      <c r="E34" s="28" t="n">
+        <v>22</v>
+      </c>
+      <c r="F34" s="29" t="n"/>
+      <c r="G34" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="H34" s="64" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="35">
+      <c r="A35" s="24" t="n">
+        <v>20</v>
+      </c>
+      <c r="B35" s="29" t="n"/>
+      <c r="C35" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="31" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E35" s="28" t="n">
+        <v>23</v>
+      </c>
+      <c r="F35" s="29" t="n"/>
+      <c r="G35" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="H35" s="65" t="s"/>
+    </row>
+    <row outlineLevel="0" r="36">
+      <c r="A36" s="24" t="n">
+        <v>21</v>
+      </c>
+      <c r="B36" s="29" t="n"/>
+      <c r="C36" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="66" t="s"/>
+      <c r="E36" s="24" t="n">
+        <v>24</v>
+      </c>
+      <c r="F36" s="19" t="n"/>
+      <c r="G36" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="31" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="37">
+      <c r="A37" s="24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B37" s="29" t="n"/>
+      <c r="C37" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="67" t="s"/>
+      <c r="E37" s="24" t="n">
+        <v>25</v>
+      </c>
+      <c r="F37" s="29" t="n"/>
+      <c r="G37" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H37" s="68" t="s"/>
+    </row>
+    <row outlineLevel="0" r="38">
+      <c r="A38" s="29" t="n"/>
+      <c r="B38" s="20" t="n">
+        <v>6</v>
+      </c>
+      <c r="C38" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="70" t="s"/>
+      <c r="E38" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="39">
+      <c r="A39" s="24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B39" s="29" t="n"/>
+      <c r="C39" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="71" t="s"/>
+      <c r="E39" s="24" t="n"/>
+      <c r="F39" s="72" t="n">
+        <v>6</v>
+      </c>
+      <c r="G39" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" s="73" t="n"/>
+    </row>
+    <row outlineLevel="0" r="40">
+      <c r="A40" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="29" t="n"/>
+      <c r="C40" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" s="74" t="n">
         <v>3.5</v>
       </c>
-      <c r="E27" s="22" t="n">
+      <c r="E40" s="22" t="n"/>
+      <c r="F40" s="75" t="n">
+        <v>26</v>
+      </c>
+      <c r="G40" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40" s="73" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="41">
+      <c r="A41" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="29" t="n"/>
+      <c r="C41" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="50" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E41" s="24" t="n">
+        <v>26</v>
+      </c>
+      <c r="F41" s="75" t="n">
+        <v>27</v>
+      </c>
+      <c r="G41" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="H41" s="76" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="42">
+      <c r="A42" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="29" t="n"/>
+      <c r="C42" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="50" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E42" s="24" t="n">
+        <v>27</v>
+      </c>
+      <c r="F42" s="75" t="n">
+        <v>28</v>
+      </c>
+      <c r="G42" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="H42" s="78" t="s"/>
+    </row>
+    <row outlineLevel="0" r="43">
+      <c r="A43" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="29" t="n"/>
+      <c r="C43" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="79" t="s"/>
+      <c r="E43" s="24" t="n">
+        <v>28</v>
+      </c>
+      <c r="F43" s="23" t="n">
+        <v>7</v>
+      </c>
+      <c r="G43" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="H43" s="81" t="s"/>
+    </row>
+    <row outlineLevel="0" r="44">
+      <c r="A44" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="29" t="n"/>
+      <c r="C44" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="E44" s="82" t="n"/>
+      <c r="F44" s="19" t="n"/>
+      <c r="G44" s="80" t="s">
+        <v>77</v>
+      </c>
+      <c r="H44" s="83" t="s"/>
+    </row>
+    <row outlineLevel="0" r="45">
+      <c r="A45" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="29" t="n"/>
+      <c r="C45" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="25" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E45" s="24" t="n">
+        <v>29</v>
+      </c>
+      <c r="F45" s="22" t="n">
+        <v>29</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H45" s="25" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="46">
+      <c r="A46" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="27" t="n"/>
+      <c r="C46" s="84" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="85" t="s"/>
+      <c r="E46" s="24" t="n">
+        <v>30</v>
+      </c>
+      <c r="F46" s="22" t="n">
+        <v>30</v>
+      </c>
+      <c r="G46" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H46" s="25" t="n">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="47">
+      <c r="A47" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="27" t="n"/>
+      <c r="C47" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="86" t="s"/>
+      <c r="E47" s="24" t="n">
+        <v>31</v>
+      </c>
+      <c r="F47" s="22" t="n">
+        <v>31</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="H47" s="25" t="n">
+        <v>4.1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="48">
+      <c r="A48" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="27" t="n"/>
+      <c r="C48" s="84" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="87" t="s"/>
+      <c r="E48" s="24" t="n"/>
+      <c r="F48" s="22" t="n"/>
+      <c r="G48" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H48" s="88" t="s"/>
+    </row>
+    <row outlineLevel="0" r="49">
+      <c r="A49" s="24" t="n">
+        <v>28</v>
+      </c>
+      <c r="B49" s="29" t="n"/>
+      <c r="C49" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" s="31" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E49" s="24" t="n">
+        <v>32</v>
+      </c>
+      <c r="F49" s="22" t="n">
+        <v>32</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="H49" s="89" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="50">
+      <c r="A50" s="24" t="n">
+        <v>29</v>
+      </c>
+      <c r="B50" s="29" t="n"/>
+      <c r="C50" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="90" t="s"/>
+      <c r="E50" s="24" t="n">
+        <v>33</v>
+      </c>
+      <c r="F50" s="22" t="n">
+        <v>33</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="H50" s="89" t="n">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="51">
+      <c r="A51" s="24" t="n"/>
+      <c r="B51" s="29" t="n">
+        <v>7</v>
+      </c>
+      <c r="C51" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="73" t="n"/>
+      <c r="E51" s="24" t="n">
+        <v>34</v>
+      </c>
+      <c r="F51" s="22" t="n">
+        <v>34</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H51" s="89" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="52">
+      <c r="A52" s="24" t="n">
+        <v>30</v>
+      </c>
+      <c r="B52" s="29" t="n"/>
+      <c r="C52" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="73" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E52" s="82" t="n"/>
+      <c r="F52" s="29" t="n"/>
+      <c r="G52" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="H52" s="91" t="s"/>
+    </row>
+    <row outlineLevel="0" r="53">
+      <c r="A53" s="24" t="n">
+        <v>31</v>
+      </c>
+      <c r="B53" s="29" t="n"/>
+      <c r="C53" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" s="76" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E53" s="24" t="n">
+        <v>35</v>
+      </c>
+      <c r="F53" s="29" t="n"/>
+      <c r="G53" s="92" t="s">
+        <v>95</v>
+      </c>
+      <c r="H53" s="93" t="s"/>
+    </row>
+    <row outlineLevel="0" r="54">
+      <c r="A54" s="24" t="n">
+        <v>32</v>
+      </c>
+      <c r="B54" s="29" t="n"/>
+      <c r="C54" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" s="94" t="s"/>
+      <c r="E54" s="24" t="n">
+        <v>36</v>
+      </c>
+      <c r="F54" s="29" t="n"/>
+      <c r="G54" s="77" t="s">
+        <v>97</v>
+      </c>
+      <c r="H54" s="95" t="s"/>
+    </row>
+    <row outlineLevel="0" r="55">
+      <c r="A55" s="29" t="n"/>
+      <c r="B55" s="20" t="n">
+        <v>8</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D55" s="96" t="s"/>
+      <c r="E55" s="24" t="n">
+        <v>37</v>
+      </c>
+      <c r="F55" s="29" t="n"/>
+      <c r="G55" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="H55" s="97" t="s"/>
+    </row>
+    <row outlineLevel="0" r="56">
+      <c r="A56" s="19" t="n"/>
+      <c r="B56" s="19" t="n"/>
+      <c r="C56" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="98" t="s"/>
+      <c r="E56" s="24" t="n">
+        <v>38</v>
+      </c>
+      <c r="F56" s="23" t="n">
+        <v>7</v>
+      </c>
+      <c r="G56" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="H56" s="99" t="s"/>
+    </row>
+    <row outlineLevel="0" r="57">
+      <c r="A57" s="24" t="n">
+        <v>33</v>
+      </c>
+      <c r="B57" s="19" t="n"/>
+      <c r="C57" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D57" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="E57" s="24" t="n">
+        <v>39</v>
+      </c>
+      <c r="F57" s="19" t="n"/>
+      <c r="G57" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="H57" s="89" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="58">
+      <c r="A58" s="24" t="n">
+        <v>34</v>
+      </c>
+      <c r="B58" s="19" t="n"/>
+      <c r="C58" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D58" s="25" t="n">
+        <v>3.96</v>
+      </c>
+      <c r="E58" s="82" t="n"/>
+      <c r="F58" s="19" t="n"/>
+      <c r="G58" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="H58" s="89" t="n">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="59">
+      <c r="A59" s="24" t="n">
+        <v>35</v>
+      </c>
+      <c r="B59" s="19" t="n"/>
+      <c r="C59" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D59" s="25" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="E59" s="24" t="n">
+        <v>40</v>
+      </c>
+      <c r="F59" s="19" t="n"/>
+      <c r="G59" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="H59" s="89" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="60">
+      <c r="A60" s="19" t="n"/>
+      <c r="B60" s="19" t="n"/>
+      <c r="C60" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="100" t="s"/>
+      <c r="E60" s="24" t="n">
+        <v>41</v>
+      </c>
+      <c r="F60" s="29" t="n"/>
+      <c r="G60" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H60" s="101" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="61">
+      <c r="A61" s="24" t="n">
+        <v>36</v>
+      </c>
+      <c r="B61" s="19" t="n"/>
+      <c r="C61" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D61" s="25" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="E61" s="24" t="n">
+        <v>42</v>
+      </c>
+      <c r="F61" s="29" t="n"/>
+      <c r="G61" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="H61" s="102" t="s"/>
+    </row>
+    <row outlineLevel="0" r="62">
+      <c r="A62" s="24" t="n">
+        <v>37</v>
+      </c>
+      <c r="B62" s="19" t="n"/>
+      <c r="C62" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="25" t="n">
+        <v>6.78</v>
+      </c>
+      <c r="E62" s="22" t="n"/>
+      <c r="F62" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="G62" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="H62" s="103" t="s"/>
+    </row>
+    <row outlineLevel="0" r="63">
+      <c r="A63" s="24" t="n">
+        <v>38</v>
+      </c>
+      <c r="B63" s="19" t="n"/>
+      <c r="C63" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D63" s="25" t="n">
+        <v>9.72</v>
+      </c>
+      <c r="E63" s="24" t="n">
+        <v>43</v>
+      </c>
+      <c r="F63" s="19" t="n"/>
+      <c r="G63" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="H63" s="89" t="n">
         <v>15</v>
       </c>
-      <c r="F27" s="17" t="n"/>
-      <c r="G27" s="13" t="s">
+    </row>
+    <row outlineLevel="0" r="64">
+      <c r="A64" s="29" t="n"/>
+      <c r="B64" s="29" t="n"/>
+      <c r="C64" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D64" s="104" t="s"/>
+      <c r="E64" s="82" t="n"/>
+      <c r="F64" s="19" t="n"/>
+      <c r="G64" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="H64" s="89" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="65">
+      <c r="A65" s="28" t="n">
+        <v>39</v>
+      </c>
+      <c r="B65" s="29" t="n"/>
+      <c r="C65" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="D65" s="105" t="s"/>
+      <c r="E65" s="24" t="n">
+        <v>44</v>
+      </c>
+      <c r="F65" s="19" t="n"/>
+      <c r="G65" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="H65" s="89" t="n">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="66">
+      <c r="A66" s="24" t="n">
+        <v>40</v>
+      </c>
+      <c r="B66" s="29" t="n"/>
+      <c r="C66" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D66" s="106" t="s"/>
+      <c r="E66" s="24" t="n">
+        <v>45</v>
+      </c>
+      <c r="F66" s="23" t="n">
+        <v>9</v>
+      </c>
+      <c r="G66" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="H66" s="19" t="n"/>
+    </row>
+    <row outlineLevel="0" r="67">
+      <c r="A67" s="107" t="n">
         <v>41</v>
       </c>
-      <c r="H27" s="48" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="I27" s="49" t="n"/>
-      <c r="J27" s="49" t="n"/>
-      <c r="K27" s="49" t="n"/>
-    </row>
-    <row customHeight="true" ht="28.75" outlineLevel="0" r="28">
-      <c r="A28" s="44" t="n">
-        <v>16</v>
-      </c>
-      <c r="B28" s="27" t="n"/>
-      <c r="C28" s="13" t="s">
+      <c r="B67" s="108" t="n"/>
+      <c r="C67" s="109" t="s">
+        <v>108</v>
+      </c>
+      <c r="D67" s="110" t="s"/>
+      <c r="E67" s="28" t="n">
+        <v>46</v>
+      </c>
+      <c r="F67" s="29" t="n"/>
+      <c r="G67" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H67" s="101" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="68">
+      <c r="A68" s="19" t="n"/>
+      <c r="B68" s="23" t="n">
+        <v>9</v>
+      </c>
+      <c r="C68" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D68" s="111" t="s"/>
+      <c r="E68" s="112" t="n"/>
+      <c r="F68" s="29" t="n"/>
+      <c r="G68" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="H68" s="113" t="s"/>
+    </row>
+    <row outlineLevel="0" r="69">
+      <c r="A69" s="24" t="n">
         <v>42</v>
       </c>
-      <c r="D28" s="50" t="s"/>
-      <c r="E28" s="22" t="n">
-        <v>16</v>
-      </c>
-      <c r="F28" s="17" t="n"/>
-      <c r="G28" s="13" t="s">
+      <c r="B69" s="19" t="n"/>
+      <c r="C69" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D69" s="25" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="E69" s="28" t="n">
+        <v>47</v>
+      </c>
+      <c r="F69" s="27" t="n"/>
+      <c r="G69" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="H69" s="114" t="n">
+        <v>0.0233</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="70">
+      <c r="A70" s="24" t="n">
         <v>43</v>
       </c>
-      <c r="H28" s="48" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="I28" s="24" t="n"/>
-      <c r="J28" s="34" t="n"/>
-      <c r="K28" s="51" t="n"/>
-      <c r="L28" s="34" t="n"/>
-      <c r="M28" s="34" t="n"/>
-      <c r="N28" s="34" t="n"/>
-      <c r="O28" s="34" t="n"/>
-    </row>
-    <row customHeight="true" ht="45.4999389648438" outlineLevel="0" r="29">
-      <c r="A29" s="47" t="s">
+      <c r="B70" s="19" t="n"/>
+      <c r="C70" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D70" s="25" t="n">
+        <v>6.78</v>
+      </c>
+      <c r="E70" s="28" t="n">
+        <v>48</v>
+      </c>
+      <c r="F70" s="27" t="n"/>
+      <c r="G70" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="H70" s="114" t="n">
+        <v>0.0233</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="71">
+      <c r="A71" s="24" t="n">
         <v>44</v>
       </c>
-      <c r="B29" s="17" t="n"/>
-      <c r="C29" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="48" t="n">
+      <c r="B71" s="19" t="n"/>
+      <c r="C71" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D71" s="25" t="n">
+        <v>9.72</v>
+      </c>
+      <c r="E71" s="28" t="n">
+        <v>49</v>
+      </c>
+      <c r="F71" s="27" t="n"/>
+      <c r="G71" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H71" s="115" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="72">
+      <c r="A72" s="24" t="n">
+        <v>45</v>
+      </c>
+      <c r="B72" s="19" t="n"/>
+      <c r="C72" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D72" s="31" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E72" s="24" t="n">
+        <v>50</v>
+      </c>
+      <c r="F72" s="27" t="n"/>
+      <c r="G72" s="92" t="s">
+        <v>117</v>
+      </c>
+      <c r="H72" s="116" t="s"/>
+    </row>
+    <row outlineLevel="0" r="73">
+      <c r="A73" s="28" t="n">
+        <v>46</v>
+      </c>
+      <c r="B73" s="29" t="n"/>
+      <c r="C73" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D73" s="117" t="s"/>
+      <c r="E73" s="22" t="n"/>
+      <c r="F73" s="27" t="n"/>
+      <c r="G73" s="84" t="s">
+        <v>119</v>
+      </c>
+      <c r="H73" s="118" t="n">
+        <v>0.0233</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="74">
+      <c r="A74" s="19" t="n"/>
+      <c r="B74" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D74" s="19" t="n"/>
+      <c r="E74" s="24" t="n">
+        <v>51</v>
+      </c>
+      <c r="F74" s="29" t="n"/>
+      <c r="G74" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H74" s="60" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="75">
+      <c r="A75" s="28" t="n">
+        <v>47</v>
+      </c>
+      <c r="B75" s="29" t="n"/>
+      <c r="C75" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D75" s="119" t="n">
         <v>4</v>
       </c>
-      <c r="E29" s="22" t="n">
-        <v>17</v>
-      </c>
-      <c r="F29" s="27" t="n"/>
-      <c r="G29" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="H29" s="52" t="s"/>
-      <c r="I29" s="24" t="n"/>
-      <c r="J29" s="34" t="n"/>
-      <c r="K29" s="49" t="n"/>
-      <c r="L29" s="34" t="n"/>
-      <c r="M29" s="34" t="n"/>
-      <c r="N29" s="34" t="n"/>
-    </row>
-    <row customHeight="true" hidden="false" ht="45" outlineLevel="0" r="30">
-      <c r="A30" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="17" t="n"/>
-      <c r="C30" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="48" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="E30" s="26" t="n">
-        <v>18</v>
-      </c>
-      <c r="F30" s="27" t="n"/>
-      <c r="G30" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H30" s="53" t="s"/>
-      <c r="I30" s="24" t="n"/>
-    </row>
-    <row customHeight="true" ht="38.75" outlineLevel="0" r="31">
-      <c r="A31" s="54" t="s">
+      <c r="E75" s="22" t="n"/>
+      <c r="F75" s="27" t="n"/>
+      <c r="G75" s="84" t="s">
+        <v>123</v>
+      </c>
+      <c r="H75" s="60" t="n">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="76">
+      <c r="A76" s="28" t="n">
         <v>48</v>
       </c>
-      <c r="B31" s="25" t="n"/>
-      <c r="C31" s="13" t="s">
+      <c r="B76" s="27" t="n"/>
+      <c r="C76" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D76" s="120" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="E76" s="28" t="n">
+        <v>52</v>
+      </c>
+      <c r="F76" s="29" t="n"/>
+      <c r="G76" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="H76" s="121" t="n">
+        <v>0.009</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="77">
+      <c r="A77" s="28" t="n"/>
+      <c r="B77" s="69" t="n">
+        <v>11</v>
+      </c>
+      <c r="C77" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D77" s="122" t="s">
+        <v>127</v>
+      </c>
+      <c r="E77" s="28" t="n">
+        <v>53</v>
+      </c>
+      <c r="F77" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="G77" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="H77" s="19" t="n"/>
+    </row>
+    <row outlineLevel="0" r="78">
+      <c r="A78" s="28" t="n">
         <v>49</v>
       </c>
-      <c r="D31" s="55" t="s"/>
-      <c r="E31" s="22" t="n">
-        <v>19</v>
-      </c>
-      <c r="F31" s="27" t="n"/>
-      <c r="G31" s="25" t="s">
+      <c r="B78" s="27" t="n"/>
+      <c r="C78" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D78" s="30" t="n"/>
+      <c r="E78" s="24" t="n">
+        <v>54</v>
+      </c>
+      <c r="F78" s="27" t="n"/>
+      <c r="G78" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="H78" s="123" t="s"/>
+    </row>
+    <row outlineLevel="0" r="79">
+      <c r="A79" s="22" t="n">
         <v>50</v>
       </c>
-      <c r="H31" s="56" t="n">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row customHeight="true" ht="36.4999389648438" outlineLevel="0" r="32">
-      <c r="A32" s="54" t="s">
+      <c r="B79" s="23" t="n"/>
+      <c r="C79" s="124" t="s">
+        <v>131</v>
+      </c>
+      <c r="D79" s="125" t="s"/>
+      <c r="E79" s="22" t="n"/>
+      <c r="F79" s="23" t="n">
+        <v>11</v>
+      </c>
+      <c r="G79" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="H79" s="19" t="n"/>
+    </row>
+    <row outlineLevel="0" r="80">
+      <c r="A80" s="19" t="n"/>
+      <c r="B80" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="C80" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" s="19" t="n"/>
+      <c r="E80" s="24" t="n">
+        <v>55</v>
+      </c>
+      <c r="F80" s="29" t="n"/>
+      <c r="G80" s="126" t="s">
+        <v>133</v>
+      </c>
+      <c r="H80" s="127" t="s"/>
+      <c r="I80" s="36" t="n"/>
+    </row>
+    <row outlineLevel="0" r="81">
+      <c r="A81" s="28" t="n">
         <v>51</v>
       </c>
-      <c r="B32" s="27" t="n"/>
-      <c r="C32" s="25" t="s">
+      <c r="B81" s="29" t="n"/>
+      <c r="C81" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D81" s="60" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E81" s="24" t="n">
+        <v>56</v>
+      </c>
+      <c r="F81" s="29" t="n"/>
+      <c r="G81" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="H81" s="60" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I81" s="36" t="n"/>
+    </row>
+    <row outlineLevel="0" r="82">
+      <c r="A82" s="28" t="n">
         <v>52</v>
       </c>
-      <c r="D32" s="57" t="s"/>
-      <c r="E32" s="26" t="n">
-        <v>20</v>
-      </c>
-      <c r="F32" s="27" t="n"/>
-      <c r="G32" s="13" t="s">
+      <c r="B82" s="27" t="n"/>
+      <c r="C82" s="128" t="s">
+        <v>136</v>
+      </c>
+      <c r="D82" s="129" t="s"/>
+      <c r="E82" s="24" t="n">
+        <v>57</v>
+      </c>
+      <c r="F82" s="29" t="n"/>
+      <c r="G82" s="77" t="s">
+        <v>137</v>
+      </c>
+      <c r="H82" s="130" t="s"/>
+      <c r="I82" s="36" t="n"/>
+    </row>
+    <row outlineLevel="0" r="83">
+      <c r="A83" s="28" t="n">
         <v>53</v>
       </c>
-      <c r="H32" s="58" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row customHeight="true" ht="36.4999389648438" outlineLevel="0" r="33">
-      <c r="A33" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="22" t="n">
-        <v>21</v>
-      </c>
-      <c r="F33" s="27" t="n"/>
-      <c r="G33" s="25" t="s">
+      <c r="B83" s="27" t="n"/>
+      <c r="C83" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D83" s="60" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="E83" s="22" t="n"/>
+      <c r="F83" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="G83" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H83" s="131" t="s"/>
+      <c r="I83" s="1" t="n"/>
+    </row>
+    <row outlineLevel="0" r="84">
+      <c r="A84" s="28" t="n">
         <v>54</v>
       </c>
-      <c r="H33" s="59" t="s"/>
-    </row>
-    <row outlineLevel="0" r="34">
-      <c r="A34" s="26" t="n">
-        <v>19</v>
-      </c>
-      <c r="B34" s="27" t="n"/>
-      <c r="C34" s="25" t="s">
+      <c r="B84" s="27" t="n"/>
+      <c r="C84" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="D84" s="30" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E84" s="24" t="n">
+        <v>58</v>
+      </c>
+      <c r="F84" s="19" t="n"/>
+      <c r="G84" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="H84" s="25" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="I84" s="26" t="n"/>
+    </row>
+    <row outlineLevel="0" r="85">
+      <c r="A85" s="19" t="n"/>
+      <c r="B85" s="23" t="n">
+        <v>13</v>
+      </c>
+      <c r="C85" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D85" s="132" t="s"/>
+      <c r="E85" s="24" t="n">
+        <v>59</v>
+      </c>
+      <c r="F85" s="19" t="n"/>
+      <c r="G85" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H85" s="25" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="I85" s="26" t="n"/>
+    </row>
+    <row outlineLevel="0" r="86">
+      <c r="A86" s="28" t="n">
         <v>55</v>
       </c>
-      <c r="D34" s="60" t="s"/>
-      <c r="E34" s="26" t="n">
-        <v>22</v>
-      </c>
-      <c r="F34" s="27" t="n"/>
-      <c r="G34" s="61" t="s">
+      <c r="B86" s="27" t="n"/>
+      <c r="C86" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D86" s="133" t="s"/>
+      <c r="E86" s="24" t="n">
+        <v>60</v>
+      </c>
+      <c r="F86" s="19" t="n"/>
+      <c r="G86" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="H86" s="25" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I86" s="26" t="n"/>
+    </row>
+    <row outlineLevel="0" r="87">
+      <c r="A87" s="19" t="n"/>
+      <c r="B87" s="23" t="n">
+        <v>14</v>
+      </c>
+      <c r="C87" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="D87" s="134" t="s"/>
+      <c r="E87" s="22" t="n"/>
+      <c r="F87" s="23" t="n">
+        <v>13</v>
+      </c>
+      <c r="G87" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="H87" s="135" t="s"/>
+    </row>
+    <row outlineLevel="0" r="88">
+      <c r="A88" s="24" t="n">
         <v>56</v>
       </c>
-      <c r="H34" s="62" t="s">
+      <c r="B88" s="19" t="n"/>
+      <c r="C88" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D88" s="25" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="E88" s="28" t="n">
+        <v>61</v>
+      </c>
+      <c r="F88" s="29" t="n"/>
+      <c r="G88" s="126" t="s">
+        <v>146</v>
+      </c>
+      <c r="H88" s="136" t="s"/>
+    </row>
+    <row outlineLevel="0" r="89">
+      <c r="A89" s="24" t="n">
         <v>57</v>
       </c>
-    </row>
-    <row outlineLevel="0" r="35">
-      <c r="A35" s="22" t="n">
-        <v>20</v>
-      </c>
-      <c r="B35" s="27" t="n"/>
-      <c r="C35" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="29" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="E35" s="26" t="n">
-        <v>23</v>
-      </c>
-      <c r="F35" s="27" t="n"/>
-      <c r="G35" s="25" t="s">
+      <c r="B89" s="19" t="n"/>
+      <c r="C89" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D89" s="137" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="E89" s="138" t="n"/>
+      <c r="F89" s="19" t="n"/>
+      <c r="G89" s="139" t="s">
+        <v>147</v>
+      </c>
+      <c r="H89" s="140" t="s"/>
+    </row>
+    <row outlineLevel="0" r="90">
+      <c r="A90" s="24" t="n">
         <v>58</v>
       </c>
-      <c r="H35" s="63" t="s"/>
-    </row>
-    <row outlineLevel="0" r="36">
-      <c r="A36" s="22" t="n">
-        <v>21</v>
-      </c>
-      <c r="B36" s="27" t="n"/>
-      <c r="C36" s="25" t="s">
+      <c r="B90" s="19" t="n"/>
+      <c r="C90" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D90" s="137" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="E90" s="141" t="n"/>
+      <c r="F90" s="29" t="n"/>
+      <c r="G90" s="139" t="s">
+        <v>148</v>
+      </c>
+      <c r="H90" s="142" t="s"/>
+    </row>
+    <row outlineLevel="0" r="91">
+      <c r="A91" s="19" t="n"/>
+      <c r="B91" s="23" t="n">
+        <v>13</v>
+      </c>
+      <c r="C91" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="D91" s="143" t="n"/>
+      <c r="E91" s="5" t="n"/>
+      <c r="F91" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="G91" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="H91" s="144" t="s"/>
+    </row>
+    <row outlineLevel="0" r="92">
+      <c r="A92" s="24" t="n">
         <v>59</v>
       </c>
-      <c r="D36" s="64" t="s"/>
-      <c r="E36" s="22" t="n">
-        <v>24</v>
-      </c>
-      <c r="F36" s="17" t="n"/>
-      <c r="G36" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H36" s="29" t="n">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="37">
-      <c r="A37" s="22" t="n">
-        <v>22</v>
-      </c>
-      <c r="B37" s="27" t="n"/>
-      <c r="C37" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="65" t="s"/>
-      <c r="E37" s="22" t="n">
-        <v>25</v>
-      </c>
-      <c r="F37" s="27" t="n"/>
-      <c r="G37" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="H37" s="66" t="s"/>
-    </row>
-    <row outlineLevel="0" r="38">
-      <c r="A38" s="27" t="n"/>
-      <c r="B38" s="18" t="n">
-        <v>6</v>
-      </c>
-      <c r="C38" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="68" t="s"/>
-      <c r="E38" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="39">
-      <c r="A39" s="22" t="n">
-        <v>23</v>
-      </c>
-      <c r="B39" s="27" t="n"/>
-      <c r="C39" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="69" t="s"/>
-      <c r="E39" s="22" t="n"/>
-      <c r="F39" s="70" t="n">
-        <v>6</v>
-      </c>
-      <c r="G39" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="H39" s="71" t="n"/>
-    </row>
-    <row outlineLevel="0" r="40">
-      <c r="A40" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" s="27" t="n"/>
-      <c r="C40" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="72" t="n">
-        <v>3</v>
-      </c>
-      <c r="E40" s="20" t="n"/>
-      <c r="F40" s="73" t="n">
-        <v>26</v>
-      </c>
-      <c r="G40" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="H40" s="71" t="n">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="41">
-      <c r="A41" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="27" t="n"/>
-      <c r="C41" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="23" t="n">
-        <v>4</v>
-      </c>
-      <c r="E41" s="22" t="n">
-        <v>26</v>
-      </c>
-      <c r="F41" s="73" t="n">
-        <v>27</v>
-      </c>
-      <c r="G41" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="H41" s="74" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="42">
-      <c r="A42" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" s="27" t="n"/>
-      <c r="C42" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D42" s="23" t="n">
-        <v>5</v>
-      </c>
-      <c r="E42" s="22" t="n">
-        <v>27</v>
-      </c>
-      <c r="F42" s="73" t="n">
-        <v>28</v>
-      </c>
-      <c r="G42" s="75" t="s">
-        <v>72</v>
-      </c>
-      <c r="H42" s="1" t="n"/>
-    </row>
-    <row outlineLevel="0" r="43">
-      <c r="A43" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="27" t="n"/>
-      <c r="C43" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D43" s="76" t="s"/>
-      <c r="E43" s="22" t="n">
-        <v>28</v>
-      </c>
-      <c r="F43" s="21" t="n">
-        <v>7</v>
-      </c>
-      <c r="G43" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="H43" s="1" t="n"/>
-    </row>
-    <row outlineLevel="0" r="44">
-      <c r="A44" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="27" t="n"/>
-      <c r="C44" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D44" s="23" t="n">
-        <v>4</v>
-      </c>
-      <c r="E44" s="77" t="n"/>
-      <c r="F44" s="17" t="n"/>
-      <c r="G44" s="78" t="s">
-        <v>77</v>
-      </c>
-      <c r="H44" s="79" t="s"/>
-    </row>
-    <row outlineLevel="0" r="45">
-      <c r="A45" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="B45" s="27" t="n"/>
-      <c r="C45" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D45" s="23" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="E45" s="22" t="n">
-        <v>29</v>
-      </c>
-      <c r="F45" s="20" t="n">
-        <v>29</v>
-      </c>
-      <c r="G45" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H45" s="23" t="n">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="46">
-      <c r="A46" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" s="25" t="n"/>
-      <c r="C46" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="81" t="s"/>
-      <c r="E46" s="22" t="n">
-        <v>30</v>
-      </c>
-      <c r="F46" s="20" t="n">
-        <v>30</v>
-      </c>
-      <c r="G46" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="H46" s="23" t="n">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="47">
-      <c r="A47" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="B47" s="25" t="n"/>
-      <c r="C47" s="80" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47" s="82" t="s"/>
-      <c r="E47" s="22" t="n">
-        <v>31</v>
-      </c>
-      <c r="F47" s="20" t="n">
-        <v>31</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="H47" s="23" t="n">
-        <v>4.1</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="48">
-      <c r="A48" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" s="25" t="n"/>
-      <c r="C48" s="80" t="s">
-        <v>87</v>
-      </c>
-      <c r="D48" s="83" t="s"/>
-      <c r="E48" s="22" t="n"/>
-      <c r="F48" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="G48" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="H48" s="84" t="s"/>
-    </row>
-    <row outlineLevel="0" r="49">
-      <c r="A49" s="22" t="n">
-        <v>28</v>
-      </c>
-      <c r="B49" s="27" t="n"/>
-      <c r="C49" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D49" s="29" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E49" s="22" t="n">
-        <v>32</v>
-      </c>
-      <c r="F49" s="20" t="n">
-        <v>32</v>
-      </c>
-      <c r="G49" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="H49" s="85" t="n">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="50">
-      <c r="A50" s="22" t="n">
-        <v>29</v>
-      </c>
-      <c r="B50" s="27" t="n"/>
-      <c r="C50" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D50" s="86" t="s"/>
-      <c r="E50" s="22" t="n">
-        <v>33</v>
-      </c>
-      <c r="F50" s="20" t="n">
-        <v>33</v>
-      </c>
-      <c r="G50" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="H50" s="85" t="n">
-        <v>5.65</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="51">
-      <c r="A51" s="22" t="n"/>
-      <c r="B51" s="27" t="n">
-        <v>7</v>
-      </c>
-      <c r="C51" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="D51" s="71" t="n"/>
-      <c r="E51" s="22" t="n">
-        <v>34</v>
-      </c>
-      <c r="F51" s="20" t="n">
-        <v>34</v>
-      </c>
-      <c r="G51" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="H51" s="85" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="52">
-      <c r="A52" s="22" t="n">
-        <v>30</v>
-      </c>
-      <c r="B52" s="27" t="n"/>
-      <c r="C52" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D52" s="71" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E52" s="77" t="n"/>
-      <c r="F52" s="27" t="n"/>
-      <c r="G52" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="H52" s="87" t="s"/>
-    </row>
-    <row outlineLevel="0" r="53">
-      <c r="A53" s="22" t="n">
-        <v>31</v>
-      </c>
-      <c r="B53" s="27" t="n"/>
-      <c r="C53" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D53" s="74" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E53" s="22" t="n">
-        <v>35</v>
-      </c>
-      <c r="F53" s="27" t="n"/>
-      <c r="G53" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="H53" s="1" t="n"/>
-    </row>
-    <row outlineLevel="0" r="54">
-      <c r="A54" s="22" t="n">
-        <v>32</v>
-      </c>
-      <c r="B54" s="27" t="n"/>
-      <c r="C54" s="88" t="s">
-        <v>97</v>
-      </c>
-      <c r="D54" s="89" t="s"/>
-      <c r="E54" s="22" t="n">
-        <v>36</v>
-      </c>
-      <c r="F54" s="27" t="n"/>
-      <c r="G54" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H54" s="1" t="n"/>
-    </row>
-    <row outlineLevel="0" r="55">
-      <c r="A55" s="27" t="n"/>
-      <c r="B55" s="18" t="n">
-        <v>8</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D55" s="90" t="s"/>
-      <c r="E55" s="22" t="n">
-        <v>37</v>
-      </c>
-      <c r="F55" s="27" t="n"/>
-      <c r="G55" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="H55" s="1" t="n"/>
-    </row>
-    <row outlineLevel="0" r="56">
-      <c r="A56" s="17" t="n"/>
-      <c r="B56" s="17" t="n"/>
-      <c r="C56" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D56" s="91" t="s"/>
-      <c r="E56" s="22" t="n">
-        <v>38</v>
-      </c>
-      <c r="F56" s="21" t="n">
-        <v>7</v>
-      </c>
-      <c r="G56" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="H56" s="1" t="n"/>
-    </row>
-    <row outlineLevel="0" r="57">
-      <c r="A57" s="22" t="n">
-        <v>33</v>
-      </c>
-      <c r="B57" s="17" t="n"/>
-      <c r="C57" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D57" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="E57" s="22" t="n">
-        <v>39</v>
-      </c>
-      <c r="F57" s="17" t="n"/>
-      <c r="G57" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="H57" s="85" t="n">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="58">
-      <c r="A58" s="22" t="n">
-        <v>34</v>
-      </c>
-      <c r="B58" s="17" t="n"/>
-      <c r="C58" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D58" s="23" t="n">
-        <v>3.96</v>
-      </c>
-      <c r="E58" s="77" t="n"/>
-      <c r="F58" s="17" t="n"/>
-      <c r="G58" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="H58" s="85" t="n">
-        <v>5.65</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="59">
-      <c r="A59" s="22" t="n">
-        <v>35</v>
-      </c>
-      <c r="B59" s="17" t="n"/>
-      <c r="C59" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D59" s="23" t="n">
-        <v>4.92</v>
-      </c>
-      <c r="E59" s="22" t="n">
-        <v>40</v>
-      </c>
-      <c r="F59" s="17" t="n"/>
-      <c r="G59" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="H59" s="85" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="60">
-      <c r="A60" s="17" t="n"/>
-      <c r="B60" s="17" t="n"/>
-      <c r="C60" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D60" s="92" t="s"/>
-      <c r="E60" s="22" t="n">
-        <v>41</v>
-      </c>
-      <c r="F60" s="27" t="n"/>
-      <c r="G60" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H60" s="93" t="n">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="61">
-      <c r="A61" s="22" t="n">
-        <v>36</v>
-      </c>
-      <c r="B61" s="17" t="n"/>
-      <c r="C61" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D61" s="23" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="E61" s="22" t="n">
-        <v>42</v>
-      </c>
-      <c r="F61" s="27" t="n"/>
-      <c r="G61" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="H61" s="1" t="n"/>
-    </row>
-    <row outlineLevel="0" r="62">
-      <c r="A62" s="22" t="n">
-        <v>37</v>
-      </c>
-      <c r="B62" s="17" t="n"/>
-      <c r="C62" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D62" s="23" t="n">
-        <v>6.78</v>
-      </c>
-      <c r="E62" s="20" t="n"/>
-      <c r="F62" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="G62" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="H62" s="94" t="s"/>
-    </row>
-    <row outlineLevel="0" r="63">
-      <c r="A63" s="22" t="n">
-        <v>38</v>
-      </c>
-      <c r="B63" s="17" t="n"/>
-      <c r="C63" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="D63" s="23" t="n">
-        <v>9.72</v>
-      </c>
-      <c r="E63" s="22" t="n">
-        <v>43</v>
-      </c>
-      <c r="F63" s="17" t="n"/>
-      <c r="G63" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="H63" s="85" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="64">
-      <c r="A64" s="27" t="n"/>
-      <c r="B64" s="27" t="n"/>
-      <c r="C64" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="D64" s="95" t="s"/>
-      <c r="E64" s="77" t="n"/>
-      <c r="F64" s="17" t="n"/>
-      <c r="G64" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="H64" s="85" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="65">
-      <c r="A65" s="26" t="n">
-        <v>39</v>
-      </c>
-      <c r="B65" s="27" t="n"/>
-      <c r="C65" s="61" t="s">
-        <v>96</v>
-      </c>
-      <c r="D65" s="96" t="s"/>
-      <c r="E65" s="22" t="n">
-        <v>44</v>
-      </c>
-      <c r="F65" s="17" t="n"/>
-      <c r="G65" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="H65" s="85" t="n">
-        <v>42.5</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="66">
-      <c r="A66" s="22" t="n">
-        <v>40</v>
-      </c>
-      <c r="B66" s="27" t="n"/>
-      <c r="C66" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D66" s="97" t="s"/>
-      <c r="E66" s="22" t="n">
-        <v>45</v>
-      </c>
-      <c r="F66" s="21" t="n">
-        <v>9</v>
-      </c>
-      <c r="G66" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="H66" s="17" t="n"/>
-    </row>
-    <row outlineLevel="0" r="67">
-      <c r="A67" s="98" t="n">
-        <v>41</v>
-      </c>
-      <c r="B67" s="99" t="n"/>
-      <c r="C67" s="100" t="s">
-        <v>109</v>
-      </c>
-      <c r="D67" s="101" t="s"/>
-      <c r="E67" s="26" t="n">
-        <v>46</v>
-      </c>
-      <c r="F67" s="27" t="n"/>
-      <c r="G67" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="H67" s="93" t="n">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="68">
-      <c r="A68" s="17" t="n"/>
-      <c r="B68" s="21" t="n">
-        <v>9</v>
-      </c>
-      <c r="C68" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D68" s="102" t="s"/>
-      <c r="E68" s="103" t="n"/>
-      <c r="F68" s="27" t="n"/>
-      <c r="G68" s="80" t="s">
-        <v>111</v>
-      </c>
-      <c r="H68" s="104" t="s"/>
-    </row>
-    <row outlineLevel="0" r="69">
-      <c r="A69" s="22" t="n">
-        <v>42</v>
-      </c>
-      <c r="B69" s="17" t="n"/>
-      <c r="C69" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="D69" s="23" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="E69" s="26" t="n">
-        <v>47</v>
-      </c>
-      <c r="F69" s="25" t="n"/>
-      <c r="G69" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="H69" s="105" t="n">
-        <v>0.0233</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="70">
-      <c r="A70" s="22" t="n">
-        <v>43</v>
-      </c>
-      <c r="B70" s="17" t="n"/>
-      <c r="C70" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D70" s="23" t="n">
-        <v>6.78</v>
-      </c>
-      <c r="E70" s="26" t="n">
-        <v>48</v>
-      </c>
-      <c r="F70" s="25" t="n"/>
-      <c r="G70" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="H70" s="105" t="n">
-        <v>0.0233</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="71">
-      <c r="A71" s="22" t="n">
-        <v>44</v>
-      </c>
-      <c r="B71" s="17" t="n"/>
-      <c r="C71" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="D71" s="23" t="n">
-        <v>9.72</v>
-      </c>
-      <c r="E71" s="26" t="n">
-        <v>49</v>
-      </c>
-      <c r="F71" s="25" t="n"/>
-      <c r="G71" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H71" s="106" t="n">
-        <v>0.015</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="72">
-      <c r="A72" s="22" t="n">
-        <v>45</v>
-      </c>
-      <c r="B72" s="17" t="n"/>
-      <c r="C72" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D72" s="29" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="E72" s="22" t="n">
-        <v>50</v>
-      </c>
-      <c r="F72" s="25" t="n"/>
-      <c r="G72" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H72" s="1" t="n"/>
-    </row>
-    <row outlineLevel="0" r="73">
-      <c r="A73" s="26" t="n">
-        <v>46</v>
-      </c>
-      <c r="B73" s="27" t="n"/>
-      <c r="C73" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D73" s="107" t="s"/>
-      <c r="E73" s="20" t="n"/>
-      <c r="F73" s="25" t="n"/>
-      <c r="G73" s="80" t="s">
-        <v>120</v>
-      </c>
-      <c r="H73" s="108" t="n">
-        <v>0.0233</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="74">
-      <c r="A74" s="17" t="n"/>
-      <c r="B74" s="21" t="n">
-        <v>10</v>
-      </c>
-      <c r="C74" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="D74" s="17" t="n"/>
-      <c r="E74" s="22" t="n">
-        <v>51</v>
-      </c>
-      <c r="F74" s="27" t="n"/>
-      <c r="G74" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="H74" s="58" t="n">
-        <v>0.015</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="75">
-      <c r="A75" s="26" t="n">
-        <v>47</v>
-      </c>
-      <c r="B75" s="27" t="n"/>
-      <c r="C75" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D75" s="109" t="n">
-        <v>4</v>
-      </c>
-      <c r="E75" s="20" t="n"/>
-      <c r="F75" s="25" t="n"/>
-      <c r="G75" s="80" t="s">
-        <v>124</v>
-      </c>
-      <c r="H75" s="58" t="n">
-        <v>0.005</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="76">
-      <c r="A76" s="26" t="n">
-        <v>48</v>
-      </c>
-      <c r="B76" s="25" t="n"/>
-      <c r="C76" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D76" s="110" t="n">
-        <v>6.6</v>
-      </c>
-      <c r="E76" s="26" t="n">
-        <v>52</v>
-      </c>
-      <c r="F76" s="27" t="n"/>
-      <c r="G76" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="H76" s="111" t="n">
-        <v>0.009</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="77">
-      <c r="A77" s="26" t="n"/>
-      <c r="B77" s="67" t="n">
-        <v>11</v>
-      </c>
-      <c r="C77" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="D77" s="112" t="s">
-        <v>128</v>
-      </c>
-      <c r="E77" s="26" t="n">
-        <v>53</v>
-      </c>
-      <c r="F77" s="21" t="n">
-        <v>10</v>
-      </c>
-      <c r="G77" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="H77" s="17" t="n"/>
-    </row>
-    <row outlineLevel="0" r="78">
-      <c r="A78" s="26" t="n">
-        <v>49</v>
-      </c>
-      <c r="B78" s="25" t="n"/>
-      <c r="C78" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="D78" s="28" t="n"/>
-      <c r="E78" s="22" t="n">
-        <v>54</v>
-      </c>
-      <c r="F78" s="25" t="n"/>
-      <c r="G78" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="H78" s="113" t="s"/>
-    </row>
-    <row outlineLevel="0" r="79">
-      <c r="A79" s="20" t="n">
-        <v>50</v>
-      </c>
-      <c r="B79" s="21" t="n"/>
-      <c r="C79" s="114" t="s">
-        <v>132</v>
-      </c>
-      <c r="D79" s="115" t="s"/>
-      <c r="E79" s="20" t="n"/>
-      <c r="F79" s="21" t="n">
-        <v>11</v>
-      </c>
-      <c r="G79" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="H79" s="17" t="n"/>
-    </row>
-    <row outlineLevel="0" r="80">
-      <c r="A80" s="17" t="n"/>
-      <c r="B80" s="21" t="n">
-        <v>12</v>
-      </c>
-      <c r="C80" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="D80" s="17" t="n"/>
-      <c r="E80" s="22" t="n">
-        <v>55</v>
-      </c>
-      <c r="F80" s="27" t="n"/>
-      <c r="G80" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="H80" s="1" t="n"/>
-      <c r="I80" s="34" t="n"/>
-    </row>
-    <row outlineLevel="0" r="81">
-      <c r="A81" s="26" t="n">
-        <v>51</v>
-      </c>
-      <c r="B81" s="27" t="n"/>
-      <c r="C81" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D81" s="58" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="E81" s="22" t="n">
-        <v>56</v>
-      </c>
-      <c r="F81" s="27" t="n"/>
-      <c r="G81" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="H81" s="58" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="I81" s="34" t="n"/>
-    </row>
-    <row outlineLevel="0" r="82">
-      <c r="A82" s="26" t="n">
-        <v>52</v>
-      </c>
-      <c r="B82" s="25" t="n"/>
-      <c r="C82" s="116" t="s">
-        <v>137</v>
-      </c>
-      <c r="D82" s="117" t="s"/>
-      <c r="E82" s="22" t="n">
-        <v>57</v>
-      </c>
-      <c r="F82" s="27" t="n"/>
-      <c r="G82" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="H82" s="1" t="n"/>
-      <c r="I82" s="34" t="n"/>
-    </row>
-    <row outlineLevel="0" r="83">
-      <c r="A83" s="26" t="n">
-        <v>53</v>
-      </c>
-      <c r="B83" s="25" t="n"/>
-      <c r="C83" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D83" s="58" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="E83" s="20" t="n"/>
-      <c r="F83" s="21" t="n">
-        <v>12</v>
-      </c>
-      <c r="G83" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="H83" s="118" t="s"/>
-      <c r="I83" s="1" t="n"/>
-    </row>
-    <row outlineLevel="0" r="84">
-      <c r="A84" s="26" t="n">
-        <v>54</v>
-      </c>
-      <c r="B84" s="25" t="n"/>
-      <c r="C84" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="D84" s="28" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E84" s="22" t="n">
-        <v>58</v>
-      </c>
-      <c r="F84" s="17" t="n"/>
-      <c r="G84" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="H84" s="23" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="I84" s="24" t="n"/>
-    </row>
-    <row outlineLevel="0" r="85">
-      <c r="A85" s="17" t="n"/>
-      <c r="B85" s="21" t="n">
-        <v>13</v>
-      </c>
-      <c r="C85" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D85" s="119" t="s"/>
-      <c r="E85" s="22" t="n">
-        <v>59</v>
-      </c>
-      <c r="F85" s="17" t="n"/>
-      <c r="G85" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="H85" s="23" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="I85" s="24" t="n"/>
-    </row>
-    <row outlineLevel="0" r="86">
-      <c r="A86" s="26" t="n">
-        <v>55</v>
-      </c>
-      <c r="B86" s="25" t="n"/>
-      <c r="C86" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="D86" s="120" t="s"/>
-      <c r="E86" s="22" t="n">
-        <v>60</v>
-      </c>
-      <c r="F86" s="17" t="n"/>
-      <c r="G86" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="H86" s="23" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="I86" s="24" t="n"/>
-    </row>
-    <row outlineLevel="0" r="87">
-      <c r="A87" s="17" t="n"/>
-      <c r="B87" s="21" t="n">
-        <v>14</v>
-      </c>
-      <c r="C87" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D87" s="121" t="s"/>
-      <c r="E87" s="20" t="n"/>
-      <c r="F87" s="21" t="n">
-        <v>13</v>
-      </c>
-      <c r="G87" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="H87" s="122" t="s"/>
-    </row>
-    <row outlineLevel="0" r="88">
-      <c r="A88" s="22" t="n">
-        <v>56</v>
-      </c>
-      <c r="B88" s="17" t="n"/>
-      <c r="C88" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="D88" s="23" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="E88" s="26" t="n">
-        <v>61</v>
-      </c>
-      <c r="F88" s="27" t="n"/>
-      <c r="G88" s="123" t="s">
-        <v>147</v>
-      </c>
-      <c r="H88" s="124" t="s"/>
-    </row>
-    <row outlineLevel="0" r="89">
-      <c r="A89" s="22" t="n">
-        <v>57</v>
-      </c>
-      <c r="B89" s="17" t="n"/>
-      <c r="C89" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="D89" s="125" t="n">
-        <v>2.64</v>
-      </c>
-      <c r="E89" s="126" t="n"/>
-      <c r="F89" s="17" t="n"/>
-      <c r="G89" s="127" t="s">
-        <v>148</v>
-      </c>
-      <c r="H89" s="128" t="s"/>
-    </row>
-    <row outlineLevel="0" r="90">
-      <c r="A90" s="22" t="n">
-        <v>58</v>
-      </c>
-      <c r="B90" s="17" t="n"/>
-      <c r="C90" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="D90" s="125" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="E90" s="129" t="n"/>
-      <c r="F90" s="27" t="n"/>
-      <c r="G90" s="127" t="s">
+      <c r="B92" s="27" t="n"/>
+      <c r="C92" s="145" t="s">
         <v>149</v>
       </c>
-      <c r="H90" s="130" t="s"/>
-    </row>
-    <row outlineLevel="0" r="91">
-      <c r="A91" s="17" t="n"/>
-      <c r="B91" s="21" t="n">
-        <v>13</v>
-      </c>
-      <c r="C91" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="D91" s="131" t="n"/>
-      <c r="E91" s="5" t="n"/>
-      <c r="F91" s="21" t="n">
-        <v>12</v>
-      </c>
-      <c r="G91" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="H91" s="132" t="s"/>
-    </row>
-    <row outlineLevel="0" r="92">
-      <c r="A92" s="22" t="n">
-        <v>59</v>
-      </c>
-      <c r="B92" s="25" t="n"/>
-      <c r="C92" s="13" t="s">
+      <c r="D92" s="146" t="s"/>
+      <c r="E92" s="147" t="n"/>
+      <c r="F92" s="29" t="n"/>
+      <c r="G92" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="D92" s="133" t="s"/>
-      <c r="E92" s="134" t="n"/>
-      <c r="F92" s="27" t="n"/>
-      <c r="G92" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="H92" s="135" t="s"/>
+      <c r="H92" s="148" t="s"/>
     </row>
     <row outlineLevel="0" r="93">
       <c r="C93" s="1" t="n"/>
@@ -5027,43 +5118,54 @@
       <c r="C94" s="1" t="n"/>
       <c r="D94" s="1" t="n"/>
       <c r="E94" s="0" t="n"/>
-      <c r="F94" s="136" t="n"/>
-      <c r="G94" s="136" t="n"/>
+      <c r="F94" s="149" t="n"/>
+      <c r="G94" s="149" t="n"/>
       <c r="I94" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="95">
       <c r="C95" s="1" t="n"/>
       <c r="D95" s="1" t="n"/>
       <c r="E95" s="0" t="n"/>
-      <c r="F95" s="136" t="n"/>
-      <c r="G95" s="136" t="n"/>
-      <c r="H95" s="136" t="n"/>
+      <c r="F95" s="149" t="n"/>
+      <c r="G95" s="149" t="n"/>
+      <c r="H95" s="149" t="n"/>
       <c r="I95" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="96">
       <c r="C96" s="1" t="n"/>
       <c r="D96" s="1" t="n"/>
       <c r="E96" s="0" t="n"/>
-      <c r="F96" s="136" t="n"/>
-      <c r="G96" s="136" t="n"/>
-      <c r="H96" s="136" t="n"/>
+      <c r="F96" s="149" t="n"/>
+      <c r="G96" s="149" t="n"/>
+      <c r="H96" s="149" t="n"/>
       <c r="I96" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="97">
       <c r="C97" s="1" t="n"/>
       <c r="D97" s="1" t="n"/>
       <c r="E97" s="0" t="n"/>
-      <c r="F97" s="136" t="n"/>
-      <c r="G97" s="136" t="n"/>
-      <c r="H97" s="136" t="n"/>
+      <c r="F97" s="149" t="n"/>
+      <c r="G97" s="149" t="n"/>
+      <c r="H97" s="149" t="n"/>
       <c r="I97" s="0" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="72">
     <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:H4"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G37:H37"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
@@ -5077,29 +5179,18 @@
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G37:H37"/>
     <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C79:D79"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
     <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="C55:D55"/>
@@ -5119,13 +5210,13 @@
     <mergeCell ref="G82:H82"/>
     <mergeCell ref="G80:H80"/>
     <mergeCell ref="G78:H78"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G54:H54"/>
     <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="G62:H62"/>
     <mergeCell ref="G53:H53"/>
     <mergeCell ref="G52:H52"/>
     <mergeCell ref="G48:H48"/>

</xml_diff>